<commit_message>
report.xlsx + ssim calculator were updated
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06C4E32E-E729-4298-A67B-86C475E02F9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5633918A-4FF3-405A-A7DC-F4193373E955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -87,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -95,16 +95,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +533,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,145 +543,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>4.7584999999999999E-5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>5.2172000000000001E-5</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.98638159751891996</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>0.98625609278678805</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>44.551791885375899</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <v>44.431202526092498</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>2.97197137606417E-5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>4.9983045878434399E-5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>0.99022671604156498</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.98905416399240498</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>46.815808181762698</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>45.094495229720998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>3.1105244397622299E-5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>3.9920973520565801E-5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>0.99036687827110204</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>0.989428309440612</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>46.621712463378898</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <v>46.194469482421802</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>2.4782623311693801E-5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>3.0639810910315597E-5</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>0.98962343120574903</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>0.98931997328996601</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>47.534561019897403</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <v>47.041751003265297</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
updated report.xlsx for D-AO
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5633918A-4FF3-405A-A7DC-F4193373E955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D1695C-C4D2-49C2-A5CD-23CB45716C8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,12 +605,24 @@
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="3">
+        <v>4.7231523702066599E-5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6.52277783556201E-5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.98537614727020195</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.98554356670379595</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44.644213973999001</v>
+      </c>
+      <c r="G4" s="4">
+        <v>43.405451065063403</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">

</xml_diff>

<commit_message>
added conditional color formatting
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D1695C-C4D2-49C2-A5CD-23CB45716C8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23415B0-D2F7-413B-9D7A-C9FC13BF244F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,6 +721,36 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B3:B9">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
report.xlsx on view 3 trasfer learning was updated
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23415B0-D2F7-413B-9D7A-C9FC13BF244F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119A2B76-FCFE-412F-B9D8-38A711BF24BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>Base Model</t>
   </si>
@@ -36,18 +36,12 @@
     <t>NM</t>
   </si>
   <si>
-    <t>NM-AO</t>
-  </si>
-  <si>
     <t>NM-AO-2</t>
   </si>
   <si>
     <t>NM-D</t>
   </si>
   <si>
-    <t>NM-D-AO</t>
-  </si>
-  <si>
     <t>MSE</t>
   </si>
   <si>
@@ -64,6 +58,24 @@
   </si>
   <si>
     <t xml:space="preserve">train </t>
+  </si>
+  <si>
+    <t>NM-D-AO-2</t>
+  </si>
+  <si>
+    <t>View 2</t>
+  </si>
+  <si>
+    <t>Transfer Learning</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>sample size</t>
+  </si>
+  <si>
+    <t>epochs</t>
   </si>
 </sst>
 </file>
@@ -87,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -96,26 +108,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -192,29 +184,161 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,198 +654,467 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772B2B59-BFB6-478B-B725-E3B9ED7A196F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10" t="s">
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="6" t="s">
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="G2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4.7584999999999999E-5</v>
+      </c>
+      <c r="C3" s="11">
+        <v>5.2172000000000001E-5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.98638159751891996</v>
+      </c>
+      <c r="E3" s="11">
+        <v>0.98625609278678805</v>
+      </c>
+      <c r="F3" s="1">
+        <v>44.551791885375899</v>
+      </c>
+      <c r="G3" s="2">
+        <v>44.431202526092498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.7231523702066599E-5</v>
+      </c>
+      <c r="C4" s="12">
+        <v>6.52277783556201E-5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.98537614727020195</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.98554356670379595</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44.644213973999001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>43.405451065063403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.97197137606417E-5</v>
+      </c>
+      <c r="C5" s="12">
+        <v>4.9983045878434399E-5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.99022671604156498</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.98905416399240498</v>
+      </c>
+      <c r="F5" s="1">
+        <v>46.815808181762698</v>
+      </c>
+      <c r="G5" s="2">
+        <v>45.094495229720998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3.1105244397622299E-5</v>
+      </c>
+      <c r="C6" s="12">
+        <v>3.9920973520565801E-5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.99036687827110204</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.989428309440612</v>
+      </c>
+      <c r="F6" s="1">
+        <v>46.621712463378898</v>
+      </c>
+      <c r="G6" s="2">
+        <v>46.194469482421802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.4782623311693801E-5</v>
+      </c>
+      <c r="C7" s="12">
+        <v>3.0639810910315597E-5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.98962343120574903</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.98931997328996601</v>
+      </c>
+      <c r="F7" s="1">
+        <v>47.534561019897403</v>
+      </c>
+      <c r="G7" s="2">
+        <v>47.041751003265297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="B8" s="4">
+        <v>3.2275466786813899E-5</v>
+      </c>
+      <c r="C8" s="13">
+        <v>4.3752327041147497E-5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.98957584166526702</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.98907267785072295</v>
+      </c>
+      <c r="F8" s="4">
+        <v>46.418638732910097</v>
+      </c>
+      <c r="G8" s="5">
+        <v>45.699698272705</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="17"/>
+      <c r="I14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>6.0605635298997999E-5</v>
+      </c>
+      <c r="C15">
+        <v>3.8013758665329002E-5</v>
+      </c>
+      <c r="D15">
+        <v>0.98883432388305603</v>
+      </c>
+      <c r="E15">
+        <v>0.98978726458549504</v>
+      </c>
+      <c r="F15">
+        <v>44.758236083984301</v>
+      </c>
+      <c r="G15">
+        <v>45.553018432617101</v>
+      </c>
+      <c r="H15" s="17">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>2.6277137367287602E-5</v>
+      </c>
+      <c r="J15">
+        <v>4.7515599329926699E-5</v>
+      </c>
+      <c r="K15">
+        <v>0.98946990489959696</v>
+      </c>
+      <c r="L15">
+        <v>0.98824352288246098</v>
+      </c>
+      <c r="M15">
+        <v>46.518804321288997</v>
+      </c>
+      <c r="N15">
+        <v>45.308811874389598</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>4.2669727326938302E-5</v>
+      </c>
+      <c r="C16">
+        <v>3.8013758665329002E-5</v>
+      </c>
+      <c r="D16">
+        <v>0.98951791763305597</v>
+      </c>
+      <c r="E16">
+        <v>0.98978726458549504</v>
+      </c>
+      <c r="F16">
+        <v>45.472197189330998</v>
+      </c>
+      <c r="G16">
+        <v>45.553018432617101</v>
+      </c>
+      <c r="H16" s="17">
         <v>11</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="I16">
+        <v>2.3706448064331199E-5</v>
+      </c>
+      <c r="J16">
+        <v>4.1465255450020698E-5</v>
+      </c>
+      <c r="K16">
+        <v>0.99027964830398496</v>
+      </c>
+      <c r="L16">
+        <v>0.98803000092506399</v>
+      </c>
+      <c r="M16">
+        <v>47.521706008911103</v>
+      </c>
+      <c r="N16">
+        <v>45.765523239135703</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>75</v>
+      </c>
+      <c r="B17">
+        <v>5.0710975428955802E-5</v>
+      </c>
+      <c r="C17">
+        <v>3.8013758665329002E-5</v>
+      </c>
+      <c r="D17">
+        <v>0.98911257743835401</v>
+      </c>
+      <c r="E17">
+        <v>0.98978726458549504</v>
+      </c>
+      <c r="F17">
+        <v>45.241755879720003</v>
+      </c>
+      <c r="G17">
+        <v>45.553018432617101</v>
+      </c>
+      <c r="H17" s="17">
         <v>12</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3">
-        <v>4.7584999999999999E-5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>5.2172000000000001E-5</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.98638159751891996</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.98625609278678805</v>
-      </c>
-      <c r="F3" s="3">
-        <v>44.551791885375899</v>
-      </c>
-      <c r="G3" s="4">
-        <v>44.431202526092498</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
-        <v>4.7231523702066599E-5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>6.52277783556201E-5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.98537614727020195</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.98554356670379595</v>
-      </c>
-      <c r="F4" s="3">
-        <v>44.644213973999001</v>
-      </c>
-      <c r="G4" s="4">
-        <v>43.405451065063403</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2.97197137606417E-5</v>
-      </c>
-      <c r="C5" s="3">
-        <v>4.9983045878434399E-5</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.99022671604156498</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.98905416399240498</v>
-      </c>
-      <c r="F5" s="3">
-        <v>46.815808181762698</v>
-      </c>
-      <c r="G5" s="4">
-        <v>45.094495229720998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3.1105244397622299E-5</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3.9920973520565801E-5</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.99036687827110204</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.989428309440612</v>
-      </c>
-      <c r="F7" s="3">
-        <v>46.621712463378898</v>
-      </c>
-      <c r="G7" s="4">
-        <v>46.194469482421802</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2.4782623311693801E-5</v>
-      </c>
-      <c r="C8" s="3">
-        <v>3.0639810910315597E-5</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.98962343120574903</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.98931997328996601</v>
-      </c>
-      <c r="F8" s="3">
-        <v>47.534561019897403</v>
-      </c>
-      <c r="G8" s="4">
-        <v>47.041751003265297</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
+      <c r="I17">
+        <v>3.0852467843942503E-5</v>
+      </c>
+      <c r="J17">
+        <v>4.0872855341149197E-5</v>
+      </c>
+      <c r="K17">
+        <v>0.98987901608149198</v>
+      </c>
+      <c r="L17">
+        <v>0.98891655802726697</v>
+      </c>
+      <c r="M17">
+        <v>46.963905639648402</v>
+      </c>
+      <c r="N17">
+        <v>45.852032043457001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
+        <v>100</v>
+      </c>
+      <c r="H18" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="11">
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B9">
+  <conditionalFormatting sqref="B3:B8">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F8">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -731,8 +1124,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D9">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="B3:B7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D7">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -741,8 +1144,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F9">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="F3:F7">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
finished view 3 TL report
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119A2B76-FCFE-412F-B9D8-38A711BF24BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E613D6-A696-40CA-B03E-E55B7A800053}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -657,7 +657,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,7 +1068,45 @@
       <c r="A18" s="18">
         <v>100</v>
       </c>
-      <c r="H18" s="18"/>
+      <c r="B18">
+        <v>4.5256131484165903E-5</v>
+      </c>
+      <c r="C18">
+        <v>3.8013758665329002E-5</v>
+      </c>
+      <c r="D18">
+        <v>0.98969455003738405</v>
+      </c>
+      <c r="E18">
+        <v>0.98978726458549504</v>
+      </c>
+      <c r="F18">
+        <v>45.500738525390602</v>
+      </c>
+      <c r="G18">
+        <v>45.553018432617101</v>
+      </c>
+      <c r="H18" s="18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>3.01593978929304E-5</v>
+      </c>
+      <c r="J18">
+        <v>3.8595762001932601E-5</v>
+      </c>
+      <c r="K18">
+        <v>0.98965702772140496</v>
+      </c>
+      <c r="L18">
+        <v>0.98832294464111303</v>
+      </c>
+      <c r="M18">
+        <v>46.934795570373502</v>
+      </c>
+      <c r="N18">
+        <v>45.775898559570301</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
Updated report.xlsx for base model View 5
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82F156C-CFD8-4851-9D6A-0D99C0A5DF3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8278214-9DFF-4323-BCAB-87B7D05F22EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="19">
   <si>
     <t>Base Model</t>
   </si>
@@ -108,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -364,11 +364,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -388,15 +412,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,6 +442,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +538,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$X$11:$X$14</c:f>
+              <c:f>Sheet1!$AW$11:$AW$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -532,7 +559,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Y$11:$Y$14</c:f>
+              <c:f>Sheet1!$AX$11:$AX$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -575,7 +602,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$X$11:$X$14</c:f>
+              <c:f>Sheet1!$AW$11:$AW$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -596,7 +623,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Z$11:$Z$14</c:f>
+              <c:f>Sheet1!$AY$11:$AY$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -872,7 +899,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$10</c:f>
+              <c:f>Sheet1!$AQ$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -895,7 +922,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$Q$11:$Q$14</c:f>
+              <c:f>Sheet1!$AP$11:$AP$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -916,7 +943,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$11:$R$14</c:f>
+              <c:f>Sheet1!$AQ$11:$AQ$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -947,7 +974,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$10</c:f>
+              <c:f>Sheet1!$AR$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -970,7 +997,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$Q$11:$Q$14</c:f>
+              <c:f>Sheet1!$AP$11:$AP$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -991,7 +1018,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$11:$S$14</c:f>
+              <c:f>Sheet1!$AR$11:$AR$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1022,7 +1049,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$10</c:f>
+              <c:f>Sheet1!$AS$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1045,7 +1072,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$Q$11:$Q$14</c:f>
+              <c:f>Sheet1!$AP$11:$AP$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1066,7 +1093,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$11:$T$14</c:f>
+              <c:f>Sheet1!$AS$11:$AS$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1097,7 +1124,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$10</c:f>
+              <c:f>Sheet1!$AT$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1120,7 +1147,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$Q$11:$Q$14</c:f>
+              <c:f>Sheet1!$AP$11:$AP$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1141,7 +1168,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$11:$U$14</c:f>
+              <c:f>Sheet1!$AT$11:$AT$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1398,7 +1425,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$Q$2:$Q$7</c:f>
+              <c:f>Sheet1!$AP$2:$AP$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1424,7 +1451,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$2:$S$7</c:f>
+              <c:f>Sheet1!$AR$2:$AR$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1656,7 +1683,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$Q$2:$Q$7</c:f>
+              <c:f>Sheet1!$AP$2:$AP$7</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1682,7 +1709,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$2:$T$7</c:f>
+              <c:f>Sheet1!$AS$2:$AS$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4080,13 +4107,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>51</xdr:col>
       <xdr:colOff>370453</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>36239</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>59</xdr:col>
       <xdr:colOff>40075</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>27940</xdr:rowOff>
@@ -4116,13 +4143,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>43</xdr:col>
       <xdr:colOff>397653</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>41830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>50</xdr:col>
       <xdr:colOff>161003</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>67122</xdr:rowOff>
@@ -4152,13 +4179,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>45</xdr:col>
       <xdr:colOff>628979</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>50</xdr:col>
       <xdr:colOff>106746</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>32844</xdr:rowOff>
@@ -4188,13 +4215,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>50</xdr:col>
       <xdr:colOff>156013</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>54</xdr:col>
       <xdr:colOff>372788</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>57478</xdr:rowOff>
@@ -4523,46 +4550,53 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772B2B59-BFB6-478B-B725-E3B9ED7A196F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:AY38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="M6" zoomScale="116" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="21"/>
+      <c r="G1" s="31"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
+    <row r="2" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
@@ -4581,20 +4615,20 @@
       <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="AP2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="18">
+      <c r="AQ2" s="18">
         <v>4.7584999999999999E-5</v>
       </c>
-      <c r="S2" s="1">
+      <c r="AR2" s="1">
         <v>0.98638159751891996</v>
       </c>
-      <c r="T2" s="1">
+      <c r="AS2" s="1">
         <v>44.551791885375899</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -4624,20 +4658,20 @@
         <f>D3/E3</f>
         <v>1.00012725369511</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="AP3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="1">
+      <c r="AQ3" s="1">
         <v>4.7231523702066599E-5</v>
       </c>
-      <c r="S3" s="1">
+      <c r="AR3" s="1">
         <v>0.98537614727020195</v>
       </c>
-      <c r="T3" s="1">
+      <c r="AS3" s="1">
         <v>44.644213973999001</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
@@ -4667,20 +4701,20 @@
         <f>1/(D4/E4)</f>
         <v>1.0001699040859247</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="AP4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="1">
+      <c r="AQ4" s="1">
         <v>2.97197137606417E-5</v>
       </c>
-      <c r="S4" s="1">
+      <c r="AR4" s="1">
         <v>0.99022671604156498</v>
       </c>
-      <c r="T4" s="1">
+      <c r="AS4" s="1">
         <v>46.815808181762698</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -4710,20 +4744,20 @@
         <f t="shared" ref="J5:J8" si="1">D5/E5</f>
         <v>1.00118552865136</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="AP5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="R5" s="1">
+      <c r="AQ5" s="1">
         <v>3.1105244397622299E-5</v>
       </c>
-      <c r="S5" s="1">
+      <c r="AR5" s="1">
         <v>0.99036687827110204</v>
       </c>
-      <c r="T5" s="1">
+      <c r="AS5" s="1">
         <v>46.621712463378898</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -4753,20 +4787,20 @@
         <f t="shared" si="1"/>
         <v>1.0009485971055554</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="AP6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="R6" s="1">
+      <c r="AQ6" s="1">
         <v>2.4782623311693801E-5</v>
       </c>
-      <c r="S6" s="1">
+      <c r="AR6" s="1">
         <v>0.98962343120574903</v>
       </c>
-      <c r="T6" s="1">
+      <c r="AS6" s="1">
         <v>47.534561019897403</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
@@ -4796,20 +4830,20 @@
         <f t="shared" si="1"/>
         <v>1.000306733841402</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="AP7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="4">
+      <c r="AQ7" s="4">
         <v>3.2275466786813899E-5</v>
       </c>
-      <c r="S7" s="4">
+      <c r="AR7" s="4">
         <v>0.98957584166526702</v>
       </c>
-      <c r="T7" s="4">
+      <c r="AS7" s="4">
         <v>46.418638732910097</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
@@ -4840,163 +4874,227 @@
         <v>1.000508722792381</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R10" t="s">
+    <row r="10" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AQ10" t="s">
         <v>8</v>
       </c>
-      <c r="S10" t="s">
+      <c r="AR10" t="s">
         <v>9</v>
       </c>
-      <c r="T10" t="s">
+      <c r="AS10" t="s">
         <v>17</v>
       </c>
-      <c r="U10" t="s">
+      <c r="AT10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="21"/>
+      <c r="P11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="28" t="s">
+      <c r="R11" s="19"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="24"/>
-      <c r="Q11" s="12">
+      <c r="X11" s="19"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="21"/>
+      <c r="AP11" s="12">
         <v>25</v>
       </c>
-      <c r="R11" s="1">
+      <c r="AQ11" s="1">
         <v>6.0605635298997999E-5</v>
       </c>
-      <c r="S11" s="1">
+      <c r="AR11" s="1">
         <v>3.8013758665329002E-5</v>
       </c>
-      <c r="T11" s="1">
+      <c r="AS11" s="1">
         <v>2.6277137367287602E-5</v>
       </c>
-      <c r="U11" s="1">
+      <c r="AT11" s="1">
         <v>4.7515599329926699E-5</v>
       </c>
-      <c r="X11" s="12">
+      <c r="AW11" s="12">
         <v>25</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="AX11" s="1">
         <v>2.6277137367287602E-5</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="AY11" s="1">
         <v>4.7515599329926699E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="27"/>
-      <c r="Q12" s="12">
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="24"/>
+      <c r="P12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>3</v>
+      </c>
+      <c r="R12" s="22"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
+      <c r="AA12" s="23"/>
+      <c r="AB12" s="23"/>
+      <c r="AC12" s="24"/>
+      <c r="AP12" s="12">
         <v>50</v>
       </c>
-      <c r="R12" s="1">
+      <c r="AQ12" s="1">
         <v>4.2669727326938302E-5</v>
       </c>
-      <c r="S12" s="1">
+      <c r="AR12" s="1">
         <v>3.8013758665329002E-5</v>
       </c>
-      <c r="T12" s="1">
+      <c r="AS12" s="1">
         <v>2.3706448064331199E-5</v>
       </c>
-      <c r="U12" s="1">
+      <c r="AT12" s="1">
         <v>4.1465255450020698E-5</v>
       </c>
-      <c r="X12" s="12">
+      <c r="AW12" s="12">
         <v>50</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="AX12" s="1">
         <v>2.3706448064331199E-5</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="AY12" s="1">
         <v>4.1465255450020698E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20" t="s">
+      <c r="C13" s="29"/>
+      <c r="D13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20" t="s">
+      <c r="E13" s="29"/>
+      <c r="F13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="19" t="s">
+      <c r="G13" s="29"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20" t="s">
+      <c r="J13" s="29"/>
+      <c r="K13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20" t="s">
+      <c r="L13" s="29"/>
+      <c r="M13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="21"/>
-      <c r="Q13" s="12">
+      <c r="N13" s="31"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="V13" s="29"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC13" s="31"/>
+      <c r="AP13" s="12">
         <v>75</v>
       </c>
-      <c r="R13" s="1">
+      <c r="AQ13" s="1">
         <v>5.0710975428955802E-5</v>
       </c>
-      <c r="S13" s="1">
+      <c r="AR13" s="1">
         <v>3.8013758665329002E-5</v>
       </c>
-      <c r="T13" s="1">
+      <c r="AS13" s="1">
         <v>3.0852467843942503E-5</v>
       </c>
-      <c r="U13" s="1">
+      <c r="AT13" s="1">
         <v>4.0872855341149197E-5</v>
       </c>
-      <c r="X13" s="12">
+      <c r="AW13" s="12">
         <v>75</v>
       </c>
-      <c r="Y13" s="1">
+      <c r="AX13" s="1">
         <v>3.0852467843942503E-5</v>
       </c>
-      <c r="Z13" s="1">
+      <c r="AY13" s="1">
         <v>4.0872855341149197E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>15</v>
       </c>
@@ -5018,7 +5116,7 @@
       <c r="G14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="30"/>
+      <c r="H14" s="27"/>
       <c r="I14" s="4" t="s">
         <v>8</v>
       </c>
@@ -5037,279 +5135,447 @@
       <c r="N14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="P14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W14" s="27"/>
+      <c r="X14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP14" s="13">
         <v>100</v>
       </c>
-      <c r="R14" s="4">
+      <c r="AQ14" s="4">
         <v>4.5256131484165903E-5</v>
       </c>
-      <c r="S14" s="4">
+      <c r="AR14" s="4">
         <v>3.8013758665329002E-5</v>
       </c>
-      <c r="T14" s="4">
+      <c r="AS14" s="4">
         <v>3.01593978929304E-5</v>
       </c>
-      <c r="U14" s="4">
+      <c r="AT14" s="4">
         <v>3.8595762001932601E-5</v>
       </c>
-      <c r="X14" s="13">
+      <c r="AW14" s="13">
         <v>100</v>
       </c>
-      <c r="Y14" s="4">
+      <c r="AX14" s="4">
         <v>3.01593978929304E-5</v>
       </c>
-      <c r="Z14" s="4">
+      <c r="AY14" s="4">
         <v>3.8595762001932601E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>25</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="2"/>
+      <c r="P15" s="12">
+        <v>25</v>
+      </c>
+      <c r="Q15" s="1">
         <v>6.0605635298997999E-5</v>
       </c>
-      <c r="C15" s="1">
+      <c r="R15" s="1">
         <v>3.8013758665329002E-5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="S15" s="1">
         <v>0.98883432388305603</v>
       </c>
-      <c r="E15" s="1">
+      <c r="T15" s="1">
         <v>0.98978726458549504</v>
       </c>
-      <c r="F15" s="1">
+      <c r="U15" s="1">
         <v>44.758236083984301</v>
       </c>
-      <c r="G15" s="1">
+      <c r="V15" s="1">
         <v>45.553018432617101</v>
       </c>
-      <c r="H15" s="12">
+      <c r="W15" s="12">
         <v>13</v>
       </c>
-      <c r="I15" s="1">
+      <c r="X15" s="1">
         <v>2.6277137367287602E-5</v>
       </c>
-      <c r="J15" s="1">
+      <c r="Y15" s="1">
         <v>4.7515599329926699E-5</v>
       </c>
-      <c r="K15" s="1">
+      <c r="Z15" s="1">
         <v>0.98946990489959696</v>
       </c>
-      <c r="L15" s="1">
+      <c r="AA15" s="1">
         <v>0.98824352288246098</v>
       </c>
-      <c r="M15" s="1">
+      <c r="AB15" s="1">
         <v>46.518804321288997</v>
       </c>
-      <c r="N15" s="2">
+      <c r="AC15" s="2">
         <v>45.308811874389598</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>50</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="2"/>
+      <c r="P16" s="12">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="1">
         <v>4.2669727326938302E-5</v>
       </c>
-      <c r="C16" s="1">
+      <c r="R16" s="1">
         <v>3.8013758665329002E-5</v>
       </c>
-      <c r="D16" s="1">
+      <c r="S16" s="1">
         <v>0.98951791763305597</v>
       </c>
-      <c r="E16" s="1">
+      <c r="T16" s="1">
         <v>0.98978726458549504</v>
       </c>
-      <c r="F16" s="1">
+      <c r="U16" s="1">
         <v>45.472197189330998</v>
       </c>
-      <c r="G16" s="1">
+      <c r="V16" s="1">
         <v>45.553018432617101</v>
       </c>
-      <c r="H16" s="12">
+      <c r="W16" s="12">
         <v>11</v>
       </c>
-      <c r="I16" s="1">
+      <c r="X16" s="1">
         <v>2.3706448064331199E-5</v>
       </c>
-      <c r="J16" s="1">
+      <c r="Y16" s="1">
         <v>4.1465255450020698E-5</v>
       </c>
-      <c r="K16" s="1">
+      <c r="Z16" s="1">
         <v>0.99027964830398496</v>
       </c>
-      <c r="L16" s="1">
+      <c r="AA16" s="1">
         <v>0.98803000092506399</v>
       </c>
-      <c r="M16" s="1">
+      <c r="AB16" s="1">
         <v>47.521706008911103</v>
       </c>
-      <c r="N16" s="2">
+      <c r="AC16" s="2">
         <v>45.765523239135703</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>75</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="2"/>
+      <c r="P17" s="12">
+        <v>75</v>
+      </c>
+      <c r="Q17" s="1">
         <v>5.0710975428955802E-5</v>
       </c>
-      <c r="C17" s="1">
+      <c r="R17" s="1">
         <v>3.8013758665329002E-5</v>
       </c>
-      <c r="D17" s="1">
+      <c r="S17" s="1">
         <v>0.98911257743835401</v>
       </c>
-      <c r="E17" s="1">
+      <c r="T17" s="1">
         <v>0.98978726458549504</v>
       </c>
-      <c r="F17" s="1">
+      <c r="U17" s="1">
         <v>45.241755879720003</v>
       </c>
-      <c r="G17" s="1">
+      <c r="V17" s="1">
         <v>45.553018432617101</v>
       </c>
-      <c r="H17" s="12">
+      <c r="W17" s="12">
         <v>12</v>
       </c>
-      <c r="I17" s="1">
+      <c r="X17" s="1">
         <v>3.0852467843942503E-5</v>
       </c>
-      <c r="J17" s="1">
+      <c r="Y17" s="1">
         <v>4.0872855341149197E-5</v>
       </c>
-      <c r="K17" s="1">
+      <c r="Z17" s="1">
         <v>0.98987901608149198</v>
       </c>
-      <c r="L17" s="1">
+      <c r="AA17" s="1">
         <v>0.98891655802726697</v>
       </c>
-      <c r="M17" s="1">
+      <c r="AB17" s="1">
         <v>46.963905639648402</v>
       </c>
-      <c r="N17" s="2">
+      <c r="AC17" s="2">
         <v>45.852032043457001</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>100</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="5"/>
+      <c r="P18" s="13">
+        <v>100</v>
+      </c>
+      <c r="Q18" s="4">
         <v>4.5256131484165903E-5</v>
       </c>
-      <c r="C18" s="4">
+      <c r="R18" s="4">
         <v>3.8013758665329002E-5</v>
       </c>
-      <c r="D18" s="4">
+      <c r="S18" s="4">
         <v>0.98969455003738405</v>
       </c>
-      <c r="E18" s="4">
+      <c r="T18" s="4">
         <v>0.98978726458549504</v>
       </c>
-      <c r="F18" s="4">
+      <c r="U18" s="4">
         <v>45.500738525390602</v>
       </c>
-      <c r="G18" s="4">
+      <c r="V18" s="4">
         <v>45.553018432617101</v>
       </c>
-      <c r="H18" s="13">
+      <c r="W18" s="13">
         <v>10</v>
       </c>
-      <c r="I18" s="4">
+      <c r="X18" s="4">
         <v>3.01593978929304E-5</v>
       </c>
-      <c r="J18" s="4">
+      <c r="Y18" s="4">
         <v>3.8595762001932601E-5</v>
       </c>
-      <c r="K18" s="4">
+      <c r="Z18" s="4">
         <v>0.98965702772140496</v>
       </c>
-      <c r="L18" s="4">
+      <c r="AA18" s="4">
         <v>0.98832294464111303</v>
       </c>
-      <c r="M18" s="4">
+      <c r="AB18" s="4">
         <v>46.934795570373502</v>
       </c>
-      <c r="N18" s="5">
+      <c r="AC18" s="5">
         <v>45.775898559570301</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="21"/>
+      <c r="P20" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q20" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="28" t="s">
+      <c r="R20" s="19"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="24"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="21"/>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="5">
         <v>5</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="27"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="24"/>
+      <c r="P21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>5</v>
+      </c>
+      <c r="R21" s="22"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="22"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="23"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="24"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20" t="s">
+      <c r="C22" s="29"/>
+      <c r="D22" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20" t="s">
+      <c r="E22" s="29"/>
+      <c r="F22" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="19" t="s">
+      <c r="G22" s="29"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20" t="s">
+      <c r="J22" s="29"/>
+      <c r="K22" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20" t="s">
+      <c r="L22" s="29"/>
+      <c r="M22" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="N22" s="21"/>
+      <c r="N22" s="31"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="V22" s="29"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA22" s="29"/>
+      <c r="AB22" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC22" s="31"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>15</v>
       </c>
@@ -5331,7 +5597,7 @@
       <c r="G23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="30"/>
+      <c r="H23" s="27"/>
       <c r="I23" s="3" t="s">
         <v>8</v>
       </c>
@@ -5350,185 +5616,445 @@
       <c r="N23" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="P23" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W23" s="27"/>
+      <c r="X23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC23" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>25</v>
       </c>
       <c r="B24" s="1">
+        <v>2.4653750238940098E-4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.6380583521095101E-4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.97098705768585203</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.97596170330047605</v>
+      </c>
+      <c r="F24" s="1">
+        <v>37.838398132324201</v>
+      </c>
+      <c r="G24" s="1">
+        <v>38.738027618408204</v>
+      </c>
+      <c r="H24" s="12">
+        <v>20</v>
+      </c>
+      <c r="I24" s="17">
+        <v>3.9403537084581299E-5</v>
+      </c>
+      <c r="J24" s="1">
+        <v>7.2134182042645902E-5</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.98528852224349905</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.984893836021423</v>
+      </c>
+      <c r="M24" s="1">
+        <v>45.241317138671803</v>
+      </c>
+      <c r="N24" s="2">
+        <v>43.585022903442301</v>
+      </c>
+      <c r="P24" s="12">
+        <v>25</v>
+      </c>
+      <c r="Q24" s="1">
         <v>1.87023348844377E-4</v>
       </c>
-      <c r="C24" s="1">
+      <c r="R24" s="1">
         <v>1.22301794988743E-4</v>
       </c>
-      <c r="D24" s="1">
+      <c r="S24" s="1">
         <v>0.97240586042404098</v>
       </c>
-      <c r="E24" s="1">
+      <c r="T24" s="1">
         <v>0.97232422828674303</v>
       </c>
-      <c r="F24" s="1">
+      <c r="U24" s="1">
         <v>39.379602890014603</v>
       </c>
-      <c r="G24" s="1">
+      <c r="V24" s="1">
         <v>40.267239433288502</v>
       </c>
-      <c r="H24" s="12">
+      <c r="W24" s="12">
         <v>23</v>
       </c>
-      <c r="I24" s="1">
+      <c r="X24" s="1">
         <v>2.61555348333786E-5</v>
       </c>
-      <c r="J24" s="1">
+      <c r="Y24" s="1">
         <v>5.0274230328795899E-5</v>
       </c>
-      <c r="K24" s="1">
+      <c r="Z24" s="1">
         <v>0.98747579097747795</v>
       </c>
-      <c r="L24" s="1">
+      <c r="AA24" s="1">
         <v>0.986951784372329</v>
       </c>
-      <c r="M24" s="1">
+      <c r="AB24" s="1">
         <v>46.992552947998</v>
       </c>
-      <c r="N24" s="2">
+      <c r="AC24" s="2">
         <v>45.924456985473597</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>50</v>
       </c>
       <c r="B25" s="1">
+        <v>2.3111993759812301E-4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1.6380583521095101E-4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.97455258607864303</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.97596170330047605</v>
+      </c>
+      <c r="F25" s="1">
+        <v>37.491713485717703</v>
+      </c>
+      <c r="G25" s="1">
+        <v>38.738027618408204</v>
+      </c>
+      <c r="H25" s="12">
+        <v>15</v>
+      </c>
+      <c r="I25" s="17">
+        <v>3.9216583481902401E-5</v>
+      </c>
+      <c r="J25" s="1">
+        <v>5.7327120801346602E-5</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.98647799134254399</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.98440427637100203</v>
+      </c>
+      <c r="M25" s="1">
+        <v>45.802333297729398</v>
+      </c>
+      <c r="N25" s="2">
+        <v>44.442697509765601</v>
+      </c>
+      <c r="P25" s="12">
+        <v>50</v>
+      </c>
+      <c r="Q25" s="1">
         <v>1.7721809726936E-4</v>
       </c>
-      <c r="C25" s="1">
+      <c r="R25" s="1">
         <v>1.22301794988743E-4</v>
       </c>
-      <c r="D25" s="1">
+      <c r="S25" s="1">
         <v>0.97305006861686705</v>
       </c>
-      <c r="E25" s="1">
+      <c r="T25" s="1">
         <v>0.97232422828674303</v>
       </c>
-      <c r="F25" s="1">
+      <c r="U25" s="1">
         <v>39.059421005249</v>
       </c>
-      <c r="G25" s="1">
+      <c r="V25" s="1">
         <v>40.267239433288502</v>
       </c>
-      <c r="H25" s="12">
+      <c r="W25" s="12">
         <v>25</v>
       </c>
-      <c r="I25" s="1">
+      <c r="X25" s="1">
         <v>2.8246186520846E-5</v>
       </c>
-      <c r="J25" s="1">
+      <c r="Y25" s="1">
         <v>3.7750013843833499E-5</v>
       </c>
-      <c r="K25" s="1">
+      <c r="Z25" s="1">
         <v>0.98940120100975004</v>
       </c>
-      <c r="L25" s="1">
+      <c r="AA25" s="1">
         <v>0.98895520210266097</v>
       </c>
-      <c r="M25" s="1">
+      <c r="AB25" s="1">
         <v>47.8213184356689</v>
       </c>
-      <c r="N25" s="2">
+      <c r="AC25" s="2">
         <v>46.968940277099598</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>75</v>
       </c>
       <c r="B26" s="1">
+        <v>5.2472879542619897E-5</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1.6380583521095101E-4</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.98518298149108796</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.97596170330047605</v>
+      </c>
+      <c r="F26" s="1">
+        <v>44.5394985961914</v>
+      </c>
+      <c r="G26" s="1">
+        <v>38.738027618408204</v>
+      </c>
+      <c r="H26" s="12">
+        <v>13</v>
+      </c>
+      <c r="I26" s="17">
+        <v>3.9045478309465802E-5</v>
+      </c>
+      <c r="J26" s="1">
+        <v>4.8959196778014297E-5</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.98727482398350996</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.98669388318061801</v>
+      </c>
+      <c r="M26" s="1">
+        <v>45.909998931884701</v>
+      </c>
+      <c r="N26" s="2">
+        <v>45.086626022338798</v>
+      </c>
+      <c r="P26" s="12">
+        <v>75</v>
+      </c>
+      <c r="Q26" s="1">
         <v>1.61925740151976E-4</v>
       </c>
-      <c r="C26" s="1">
+      <c r="R26" s="1">
         <v>1.22301794988743E-4</v>
       </c>
-      <c r="D26" s="1">
+      <c r="S26" s="1">
         <v>0.97214901447296098</v>
       </c>
-      <c r="E26" s="1">
+      <c r="T26" s="1">
         <v>0.97232422828674303</v>
       </c>
-      <c r="F26" s="1">
+      <c r="U26" s="1">
         <v>39.407296702067001</v>
       </c>
-      <c r="G26" s="1">
+      <c r="V26" s="1">
         <v>40.267239433288502</v>
       </c>
-      <c r="H26" s="12">
+      <c r="W26" s="12">
         <v>22</v>
       </c>
-      <c r="I26" s="17">
+      <c r="X26" s="17">
         <v>2.94253816173295E-5</v>
       </c>
-      <c r="J26" s="1">
+      <c r="Y26" s="1">
         <v>3.2551214095292297E-5</v>
       </c>
-      <c r="K26" s="1">
+      <c r="Z26" s="1">
         <v>0.98908270676930699</v>
       </c>
-      <c r="L26" s="1">
+      <c r="AA26" s="1">
         <v>0.988458636760711</v>
       </c>
-      <c r="M26" s="1">
+      <c r="AB26" s="1">
         <v>47.706615549723303</v>
       </c>
-      <c r="N26" s="2">
+      <c r="AC26" s="2">
         <v>47.325179077148398</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>100</v>
       </c>
       <c r="B27" s="4">
+        <v>2.12330623944581E-4</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1.6380583521095101E-4</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.97309926092624599</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.97596170330047605</v>
+      </c>
+      <c r="F27" s="4">
+        <v>37.719122200012201</v>
+      </c>
+      <c r="G27" s="4">
+        <v>38.738027618408204</v>
+      </c>
+      <c r="H27" s="13">
+        <v>10</v>
+      </c>
+      <c r="I27" s="3">
+        <v>3.7516255051741599E-5</v>
+      </c>
+      <c r="J27" s="4">
+        <v>4.8215005996098602E-5</v>
+      </c>
+      <c r="K27" s="4">
+        <v>0.98767679333686798</v>
+      </c>
+      <c r="L27" s="4">
+        <v>0.98690433216094897</v>
+      </c>
+      <c r="M27" s="4">
+        <v>45.932556419372503</v>
+      </c>
+      <c r="N27" s="5">
+        <v>45.130912704467697</v>
+      </c>
+      <c r="P27" s="13">
+        <v>100</v>
+      </c>
+      <c r="Q27" s="4">
         <v>1.5695816919105701E-4</v>
       </c>
-      <c r="C27" s="4">
+      <c r="R27" s="4">
         <v>1.22301794988743E-4</v>
       </c>
-      <c r="D27" s="4">
+      <c r="S27" s="4">
         <v>0.97247086942195804</v>
       </c>
-      <c r="E27" s="4">
+      <c r="T27" s="4">
         <v>0.97232422828674303</v>
       </c>
-      <c r="F27" s="4">
+      <c r="U27" s="4">
         <v>39.453057918548502</v>
       </c>
-      <c r="G27" s="4">
+      <c r="V27" s="4">
         <v>40.267239433288502</v>
       </c>
-      <c r="H27" s="13">
+      <c r="W27" s="13">
         <v>13</v>
       </c>
-      <c r="I27" s="3">
+      <c r="X27" s="3">
         <v>2.9531874833992299E-5</v>
       </c>
-      <c r="J27" s="4">
+      <c r="Y27" s="4">
         <v>3.2329415906133299E-5</v>
       </c>
-      <c r="K27" s="4">
+      <c r="Z27" s="4">
         <v>0.98975329101085596</v>
       </c>
-      <c r="L27" s="4">
+      <c r="AA27" s="4">
         <v>0.98950933218002302</v>
       </c>
-      <c r="M27" s="4">
+      <c r="AB27" s="4">
         <v>47.705362815856901</v>
       </c>
-      <c r="N27" s="5">
+      <c r="AC27" s="5">
         <v>47.355676757812503</v>
       </c>
+    </row>
+    <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P29" s="34">
+        <v>200</v>
+      </c>
+      <c r="Q29" s="32">
+        <v>1.0744010523922E-4</v>
+      </c>
+      <c r="R29" s="32">
+        <v>1.3207085607427801E-4</v>
+      </c>
+      <c r="S29" s="32">
+        <v>0.97247788453102102</v>
+      </c>
+      <c r="T29" s="32">
+        <v>0.97338824462890605</v>
+      </c>
+      <c r="U29" s="32">
+        <v>40.785670326232903</v>
+      </c>
+      <c r="V29" s="32">
+        <v>40.443220672607403</v>
+      </c>
+      <c r="W29" s="34">
+        <v>15</v>
+      </c>
+      <c r="X29" s="32">
+        <v>2.6981619124853701E-5</v>
+      </c>
+      <c r="Y29" s="32">
+        <v>2.8614148161068399E-5</v>
+      </c>
+      <c r="Z29" s="32">
+        <v>0.98452750730514504</v>
+      </c>
+      <c r="AA29" s="32">
+        <v>0.98452728366851805</v>
+      </c>
+      <c r="AB29" s="32">
+        <v>47.195258300781198</v>
+      </c>
+      <c r="AC29" s="33">
+        <v>47.304651504516599</v>
+      </c>
+    </row>
+    <row r="38" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="40">
     <mergeCell ref="C20:G21"/>
     <mergeCell ref="H20:H23"/>
     <mergeCell ref="I20:N21"/>
@@ -5538,22 +6064,40 @@
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="X11:AC12"/>
+    <mergeCell ref="W11:W14"/>
+    <mergeCell ref="C11:G12"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:N12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
-    <mergeCell ref="C11:G12"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="R11:V12"/>
     <mergeCell ref="M13:N13"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I11:N12"/>
-    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="R20:V21"/>
+    <mergeCell ref="W20:W23"/>
+    <mergeCell ref="X20:AC21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5563,6 +6107,186 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D8">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F8">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B7">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D7">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F7">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ2:AQ7">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ7">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ2:AQ6">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR2:AR7">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR2:AR6">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS2:AS7">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS2:AS6">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q24:Q27">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S24:S27">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U24:U27">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X24:X27">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z24:Z27">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB24:AB27">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -5572,18 +6296,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F8">
+  <conditionalFormatting sqref="Y24:Y27">
     <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5592,137 +6306,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B7">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D7">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F7">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R7">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R7">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R6">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S7">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S6">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T7">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T6">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:B27">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D27">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F24:F27">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24:I27">
+  <conditionalFormatting sqref="I38">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -5732,7 +6316,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K24:K27">
+  <conditionalFormatting sqref="K38">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -5742,7 +6326,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24:M27">
+  <conditionalFormatting sqref="M38">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -5752,7 +6336,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J24:J27">
+  <conditionalFormatting sqref="J38">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
report.xlsx was updated with new correct data-set
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8278214-9DFF-4323-BCAB-87B7D05F22EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3389D4CB-D652-4753-A2C5-568746F9FFDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="19">
   <si>
     <t>Base Model</t>
   </si>
@@ -108,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -250,30 +250,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -392,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -400,25 +378,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -439,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -451,9 +430,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4552,8 +4528,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AY38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M6" zoomScale="116" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4579,24 +4555,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="31"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
+      <c r="A2" s="28"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
@@ -4615,10 +4591,10 @@
       <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AP2" s="9" t="s">
+      <c r="AP2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="AQ2" s="18">
+      <c r="AQ2" s="16">
         <v>4.7584999999999999E-5</v>
       </c>
       <c r="AR2" s="1">
@@ -4629,36 +4605,36 @@
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18">
-        <v>4.7584999999999999E-5</v>
-      </c>
-      <c r="C3" s="6">
-        <v>5.2172000000000001E-5</v>
+      <c r="B3" s="1">
+        <v>4.4384981214534402E-5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4.3598451313755497E-5</v>
       </c>
       <c r="D3" s="1">
-        <v>0.98638159751891996</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0.98625609278678805</v>
+        <v>0.98570186853408803</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.98624380275607104</v>
       </c>
       <c r="F3" s="1">
-        <v>44.551791885375899</v>
+        <v>44.889844085693298</v>
       </c>
       <c r="G3" s="2">
-        <v>44.431202526092498</v>
+        <v>45.043708372116001</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I6" si="0">B3/C3</f>
-        <v>0.91207927624012874</v>
+        <f>(MIN(B3:C3)/MAX(B3:C3))</f>
+        <v>0.98227936839767438</v>
       </c>
       <c r="J3">
-        <f>D3/E3</f>
-        <v>1.00012725369511</v>
-      </c>
-      <c r="AP3" s="10" t="s">
+        <f>(MIN(D3:E3)/MAX(D3:E3))</f>
+        <v>0.99945050684174785</v>
+      </c>
+      <c r="AP3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="AQ3" s="1">
@@ -4672,36 +4648,14 @@
       </c>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4.7231523702066599E-5</v>
-      </c>
-      <c r="C4" s="7">
-        <v>6.52277783556201E-5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.98537614727020195</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0.98554356670379595</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44.644213973999001</v>
-      </c>
-      <c r="G4" s="2">
-        <v>43.405451065063403</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0.7241013705014081</v>
-      </c>
-      <c r="J4">
-        <f>1/(D4/E4)</f>
-        <v>1.0001699040859247</v>
-      </c>
-      <c r="AP4" s="10" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2"/>
+      <c r="AP4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="AQ4" s="1">
@@ -4715,36 +4669,36 @@
       </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>2.97197137606417E-5</v>
-      </c>
-      <c r="C5" s="7">
-        <v>4.9983045878434399E-5</v>
+        <v>2.8511245238405499E-5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.8728576925232099E-5</v>
       </c>
       <c r="D5" s="1">
-        <v>0.99022671604156498</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0.98905416399240498</v>
+        <v>0.99027996993064804</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.99051213473081501</v>
       </c>
       <c r="F5" s="1">
-        <v>46.815808181762698</v>
+        <v>47.013923629760697</v>
       </c>
       <c r="G5" s="2">
-        <v>45.094495229720998</v>
+        <v>47.092300043106</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
-        <v>0.59459589223362075</v>
+        <f t="shared" ref="I5:I8" si="0">(MIN(B5:C5)/MAX(B5:C5))</f>
+        <v>0.99243499991690443</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J8" si="1">D5/E5</f>
-        <v>1.00118552865136</v>
-      </c>
-      <c r="AP5" s="10" t="s">
+        <f>(MIN(D5:E5)/MAX(D5:E5))</f>
+        <v>0.99976561135191944</v>
+      </c>
+      <c r="AP5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="AQ5" s="1">
@@ -4758,36 +4712,36 @@
       </c>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>3.1105244397622299E-5</v>
-      </c>
-      <c r="C6" s="7">
-        <v>3.9920973520565801E-5</v>
+        <v>3.1105838688745197E-5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3.1866090255334703E-5</v>
       </c>
       <c r="D6" s="1">
-        <v>0.99036687827110204</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0.989428309440612</v>
+        <v>0.99037553977966297</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.99035752817988398</v>
       </c>
       <c r="F6" s="1">
-        <v>46.621712463378898</v>
+        <v>46.641133148193298</v>
       </c>
       <c r="G6" s="2">
-        <v>46.194469482421802</v>
+        <v>46.648111543655297</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0.77917048745311868</v>
+        <v>0.97614230172268368</v>
       </c>
       <c r="J6">
-        <f t="shared" si="1"/>
-        <v>1.0009485971055554</v>
-      </c>
-      <c r="AP6" s="10" t="s">
+        <f>(MIN(D6:E6)/MAX(D6:E6))</f>
+        <v>0.9999818133636631</v>
+      </c>
+      <c r="AP6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="AQ6" s="1">
@@ -4801,36 +4755,36 @@
       </c>
     </row>
     <row r="7" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>2.4782623311693801E-5</v>
-      </c>
-      <c r="C7" s="7">
-        <v>3.0639810910315597E-5</v>
+        <v>2.4951792413048599E-5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2.5730579322953402E-5</v>
       </c>
       <c r="D7" s="1">
-        <v>0.98962343120574903</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0.98931997328996601</v>
+        <v>0.98987759256362895</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.98991635859012606</v>
       </c>
       <c r="F7" s="1">
-        <v>47.534561019897403</v>
+        <v>47.530662322997998</v>
       </c>
       <c r="G7" s="2">
-        <v>47.041751003265297</v>
+        <v>47.379944515228203</v>
       </c>
       <c r="I7">
-        <f>B7/C7</f>
-        <v>0.8088373451205001</v>
+        <f t="shared" si="0"/>
+        <v>0.96973302077151158</v>
       </c>
       <c r="J7">
-        <f t="shared" si="1"/>
-        <v>1.000306733841402</v>
-      </c>
-      <c r="AP7" s="11" t="s">
+        <f>(MIN(D7:E7)/MAX(D7:E7))</f>
+        <v>0.99996083908891831</v>
+      </c>
+      <c r="AP7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="AQ7" s="4">
@@ -4844,34 +4798,34 @@
       </c>
     </row>
     <row r="8" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="4">
-        <v>3.2275466786813899E-5</v>
-      </c>
-      <c r="C8" s="8">
-        <v>4.3752327041147497E-5</v>
+        <v>3.0885576104992602E-5</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.1265434369060997E-5</v>
       </c>
       <c r="D8" s="4">
-        <v>0.98957584166526702</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0.98907267785072295</v>
+        <v>0.98880489277839601</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.98897296860814099</v>
       </c>
       <c r="F8" s="4">
-        <v>46.418638732910097</v>
+        <v>46.554526840209903</v>
       </c>
       <c r="G8" s="5">
-        <v>45.699698272705</v>
+        <v>46.727471981048502</v>
       </c>
       <c r="I8">
-        <f>B8/C8</f>
-        <v>0.73768571798386806</v>
+        <f t="shared" si="0"/>
+        <v>0.98785053616768914</v>
       </c>
       <c r="J8">
-        <f t="shared" si="1"/>
-        <v>1.000508722792381</v>
+        <f>(MIN(D8:E8)/MAX(D8:E8))</f>
+        <v>0.99983005012767789</v>
       </c>
     </row>
     <row r="10" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4889,47 +4843,47 @@
       </c>
     </row>
     <row r="11" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="25" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="21"/>
-      <c r="P11" s="15" t="s">
+      <c r="I11" s="20"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="22"/>
+      <c r="P11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Q11" s="16" t="s">
+      <c r="Q11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="R11" s="19"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="20"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="25" t="s">
+      <c r="R11" s="20"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="X11" s="19"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
-      <c r="AC11" s="21"/>
-      <c r="AP11" s="12">
+      <c r="X11" s="20"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="21"/>
+      <c r="AC11" s="22"/>
+      <c r="AP11" s="10">
         <v>25</v>
       </c>
       <c r="AQ11" s="1">
@@ -4944,7 +4898,7 @@
       <c r="AT11" s="1">
         <v>4.7515599329926699E-5</v>
       </c>
-      <c r="AW11" s="12">
+      <c r="AW11" s="10">
         <v>25</v>
       </c>
       <c r="AX11" s="1">
@@ -4961,37 +4915,37 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="24"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="25"/>
       <c r="P12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
       </c>
-      <c r="R12" s="22"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="24"/>
-      <c r="AP12" s="12">
+      <c r="R12" s="23"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="24"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="25"/>
+      <c r="AP12" s="10">
         <v>50</v>
       </c>
       <c r="AQ12" s="1">
@@ -5006,7 +4960,7 @@
       <c r="AT12" s="1">
         <v>4.1465255450020698E-5</v>
       </c>
-      <c r="AW12" s="12">
+      <c r="AW12" s="10">
         <v>50</v>
       </c>
       <c r="AX12" s="1">
@@ -5017,59 +4971,59 @@
       </c>
     </row>
     <row r="13" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
-      <c r="B13" s="28" t="s">
+      <c r="A13" s="15"/>
+      <c r="B13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29" t="s">
+      <c r="E13" s="30"/>
+      <c r="F13" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="29"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="30" t="s">
+      <c r="G13" s="30"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29" t="s">
+      <c r="J13" s="30"/>
+      <c r="K13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29" t="s">
+      <c r="L13" s="30"/>
+      <c r="M13" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="31"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="28" t="s">
+      <c r="N13" s="32"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29" t="s">
+      <c r="R13" s="30"/>
+      <c r="S13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29" t="s">
+      <c r="T13" s="30"/>
+      <c r="U13" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="V13" s="29"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="30" t="s">
+      <c r="V13" s="30"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="Y13" s="29"/>
-      <c r="Z13" s="29" t="s">
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AA13" s="29"/>
-      <c r="AB13" s="29" t="s">
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="AC13" s="31"/>
-      <c r="AP13" s="12">
+      <c r="AC13" s="32"/>
+      <c r="AP13" s="10">
         <v>75</v>
       </c>
       <c r="AQ13" s="1">
@@ -5084,7 +5038,7 @@
       <c r="AT13" s="1">
         <v>4.0872855341149197E-5</v>
       </c>
-      <c r="AW13" s="12">
+      <c r="AW13" s="10">
         <v>75</v>
       </c>
       <c r="AX13" s="1">
@@ -5095,7 +5049,7 @@
       </c>
     </row>
     <row r="14" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -5116,7 +5070,7 @@
       <c r="G14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="27"/>
+      <c r="H14" s="28"/>
       <c r="I14" s="4" t="s">
         <v>8</v>
       </c>
@@ -5135,7 +5089,7 @@
       <c r="N14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P14" s="14" t="s">
+      <c r="P14" s="12" t="s">
         <v>15</v>
       </c>
       <c r="Q14" s="4" t="s">
@@ -5156,7 +5110,7 @@
       <c r="V14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W14" s="27"/>
+      <c r="W14" s="28"/>
       <c r="X14" s="4" t="s">
         <v>8</v>
       </c>
@@ -5175,7 +5129,7 @@
       <c r="AC14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AP14" s="13">
+      <c r="AP14" s="11">
         <v>100</v>
       </c>
       <c r="AQ14" s="4">
@@ -5190,7 +5144,7 @@
       <c r="AT14" s="4">
         <v>3.8595762001932601E-5</v>
       </c>
-      <c r="AW14" s="13">
+      <c r="AW14" s="11">
         <v>100</v>
       </c>
       <c r="AX14" s="4">
@@ -5201,7 +5155,7 @@
       </c>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="10">
         <v>25</v>
       </c>
       <c r="B15" s="1"/>
@@ -5210,14 +5164,14 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="2"/>
-      <c r="P15" s="12">
+      <c r="P15" s="10">
         <v>25</v>
       </c>
       <c r="Q15" s="1">
@@ -5238,7 +5192,7 @@
       <c r="V15" s="1">
         <v>45.553018432617101</v>
       </c>
-      <c r="W15" s="12">
+      <c r="W15" s="10">
         <v>13</v>
       </c>
       <c r="X15" s="1">
@@ -5261,7 +5215,7 @@
       </c>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="10">
         <v>50</v>
       </c>
       <c r="B16" s="1"/>
@@ -5270,14 +5224,14 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="10"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="2"/>
-      <c r="P16" s="12">
+      <c r="P16" s="10">
         <v>50</v>
       </c>
       <c r="Q16" s="1">
@@ -5298,7 +5252,7 @@
       <c r="V16" s="1">
         <v>45.553018432617101</v>
       </c>
-      <c r="W16" s="12">
+      <c r="W16" s="10">
         <v>11</v>
       </c>
       <c r="X16" s="1">
@@ -5321,7 +5275,7 @@
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="A17" s="10">
         <v>75</v>
       </c>
       <c r="B17" s="1"/>
@@ -5330,14 +5284,14 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="12"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="2"/>
-      <c r="P17" s="12">
+      <c r="P17" s="10">
         <v>75</v>
       </c>
       <c r="Q17" s="1">
@@ -5358,7 +5312,7 @@
       <c r="V17" s="1">
         <v>45.553018432617101</v>
       </c>
-      <c r="W17" s="12">
+      <c r="W17" s="10">
         <v>12</v>
       </c>
       <c r="X17" s="1">
@@ -5381,7 +5335,7 @@
       </c>
     </row>
     <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
+      <c r="A18" s="11">
         <v>100</v>
       </c>
       <c r="B18" s="4"/>
@@ -5390,14 +5344,14 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="13"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="5"/>
-      <c r="P18" s="13">
+      <c r="P18" s="11">
         <v>100</v>
       </c>
       <c r="Q18" s="4">
@@ -5418,7 +5372,7 @@
       <c r="V18" s="4">
         <v>45.553018432617101</v>
       </c>
-      <c r="W18" s="13">
+      <c r="W18" s="11">
         <v>10</v>
       </c>
       <c r="X18" s="4">
@@ -5442,46 +5396,46 @@
     </row>
     <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="25" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="21"/>
-      <c r="P20" s="15" t="s">
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="22"/>
+      <c r="P20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="Q20" s="16" t="s">
+      <c r="Q20" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="19"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="25" t="s">
+      <c r="R20" s="20"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="22"/>
+      <c r="W20" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="X20" s="19"/>
-      <c r="Y20" s="20"/>
-      <c r="Z20" s="20"/>
-      <c r="AA20" s="20"/>
-      <c r="AB20" s="20"/>
-      <c r="AC20" s="21"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="21"/>
+      <c r="AA20" s="21"/>
+      <c r="AB20" s="21"/>
+      <c r="AC20" s="22"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -5490,93 +5444,93 @@
       <c r="B21" s="5">
         <v>5</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="24"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="25"/>
       <c r="P21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q21" s="5">
         <v>5</v>
       </c>
-      <c r="R21" s="22"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="22"/>
-      <c r="Y21" s="23"/>
-      <c r="Z21" s="23"/>
-      <c r="AA21" s="23"/>
-      <c r="AB21" s="23"/>
-      <c r="AC21" s="24"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="24"/>
+      <c r="AB21" s="24"/>
+      <c r="AC21" s="25"/>
     </row>
     <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="28" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29" t="s">
+      <c r="E22" s="30"/>
+      <c r="F22" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="29"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="30" t="s">
+      <c r="G22" s="30"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29" t="s">
+      <c r="J22" s="30"/>
+      <c r="K22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29" t="s">
+      <c r="L22" s="30"/>
+      <c r="M22" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="N22" s="31"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="28" t="s">
+      <c r="N22" s="32"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29" t="s">
+      <c r="R22" s="30"/>
+      <c r="S22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="T22" s="29"/>
-      <c r="U22" s="29" t="s">
+      <c r="T22" s="30"/>
+      <c r="U22" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="V22" s="29"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="30" t="s">
+      <c r="V22" s="30"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="Y22" s="29"/>
-      <c r="Z22" s="29" t="s">
+      <c r="Y22" s="30"/>
+      <c r="Z22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AA22" s="29"/>
-      <c r="AB22" s="29" t="s">
+      <c r="AA22" s="30"/>
+      <c r="AB22" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="AC22" s="31"/>
+      <c r="AC22" s="32"/>
     </row>
     <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -5597,7 +5551,7 @@
       <c r="G23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="27"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="3" t="s">
         <v>8</v>
       </c>
@@ -5616,7 +5570,7 @@
       <c r="N23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P23" s="14" t="s">
+      <c r="P23" s="12" t="s">
         <v>15</v>
       </c>
       <c r="Q23" s="4" t="s">
@@ -5637,7 +5591,7 @@
       <c r="V23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W23" s="27"/>
+      <c r="W23" s="28"/>
       <c r="X23" s="3" t="s">
         <v>8</v>
       </c>
@@ -5658,7 +5612,7 @@
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
+      <c r="A24" s="10">
         <v>25</v>
       </c>
       <c r="B24" s="1">
@@ -5679,10 +5633,10 @@
       <c r="G24" s="1">
         <v>38.738027618408204</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="10">
         <v>20</v>
       </c>
-      <c r="I24" s="17">
+      <c r="I24" s="15">
         <v>3.9403537084581299E-5</v>
       </c>
       <c r="J24" s="1">
@@ -5700,7 +5654,7 @@
       <c r="N24" s="2">
         <v>43.585022903442301</v>
       </c>
-      <c r="P24" s="12">
+      <c r="P24" s="10">
         <v>25</v>
       </c>
       <c r="Q24" s="1">
@@ -5721,7 +5675,7 @@
       <c r="V24" s="1">
         <v>40.267239433288502</v>
       </c>
-      <c r="W24" s="12">
+      <c r="W24" s="10">
         <v>23</v>
       </c>
       <c r="X24" s="1">
@@ -5744,7 +5698,7 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
+      <c r="A25" s="10">
         <v>50</v>
       </c>
       <c r="B25" s="1">
@@ -5765,10 +5719,10 @@
       <c r="G25" s="1">
         <v>38.738027618408204</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="10">
         <v>15</v>
       </c>
-      <c r="I25" s="17">
+      <c r="I25" s="15">
         <v>3.9216583481902401E-5</v>
       </c>
       <c r="J25" s="1">
@@ -5786,7 +5740,7 @@
       <c r="N25" s="2">
         <v>44.442697509765601</v>
       </c>
-      <c r="P25" s="12">
+      <c r="P25" s="10">
         <v>50</v>
       </c>
       <c r="Q25" s="1">
@@ -5807,7 +5761,7 @@
       <c r="V25" s="1">
         <v>40.267239433288502</v>
       </c>
-      <c r="W25" s="12">
+      <c r="W25" s="10">
         <v>25</v>
       </c>
       <c r="X25" s="1">
@@ -5830,7 +5784,7 @@
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
+      <c r="A26" s="10">
         <v>75</v>
       </c>
       <c r="B26" s="1">
@@ -5851,10 +5805,10 @@
       <c r="G26" s="1">
         <v>38.738027618408204</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="10">
         <v>13</v>
       </c>
-      <c r="I26" s="17">
+      <c r="I26" s="15">
         <v>3.9045478309465802E-5</v>
       </c>
       <c r="J26" s="1">
@@ -5872,7 +5826,7 @@
       <c r="N26" s="2">
         <v>45.086626022338798</v>
       </c>
-      <c r="P26" s="12">
+      <c r="P26" s="10">
         <v>75</v>
       </c>
       <c r="Q26" s="1">
@@ -5893,10 +5847,10 @@
       <c r="V26" s="1">
         <v>40.267239433288502</v>
       </c>
-      <c r="W26" s="12">
+      <c r="W26" s="10">
         <v>22</v>
       </c>
-      <c r="X26" s="17">
+      <c r="X26" s="15">
         <v>2.94253816173295E-5</v>
       </c>
       <c r="Y26" s="1">
@@ -5916,7 +5870,7 @@
       </c>
     </row>
     <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13">
+      <c r="A27" s="11">
         <v>100</v>
       </c>
       <c r="B27" s="4">
@@ -5937,7 +5891,7 @@
       <c r="G27" s="4">
         <v>38.738027618408204</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="11">
         <v>10</v>
       </c>
       <c r="I27" s="3">
@@ -5958,7 +5912,7 @@
       <c r="N27" s="5">
         <v>45.130912704467697</v>
       </c>
-      <c r="P27" s="13">
+      <c r="P27" s="11">
         <v>100</v>
       </c>
       <c r="Q27" s="4">
@@ -5979,7 +5933,7 @@
       <c r="V27" s="4">
         <v>40.267239433288502</v>
       </c>
-      <c r="W27" s="13">
+      <c r="W27" s="11">
         <v>13</v>
       </c>
       <c r="X27" s="3">
@@ -6003,46 +5957,46 @@
     </row>
     <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="P29" s="34">
+      <c r="P29" s="19">
         <v>200</v>
       </c>
-      <c r="Q29" s="32">
+      <c r="Q29" s="17">
         <v>1.0744010523922E-4</v>
       </c>
-      <c r="R29" s="32">
+      <c r="R29" s="17">
         <v>1.3207085607427801E-4</v>
       </c>
-      <c r="S29" s="32">
+      <c r="S29" s="17">
         <v>0.97247788453102102</v>
       </c>
-      <c r="T29" s="32">
+      <c r="T29" s="17">
         <v>0.97338824462890605</v>
       </c>
-      <c r="U29" s="32">
+      <c r="U29" s="17">
         <v>40.785670326232903</v>
       </c>
-      <c r="V29" s="32">
+      <c r="V29" s="17">
         <v>40.443220672607403</v>
       </c>
-      <c r="W29" s="34">
+      <c r="W29" s="19">
         <v>15</v>
       </c>
-      <c r="X29" s="32">
+      <c r="X29" s="17">
         <v>2.6981619124853701E-5</v>
       </c>
-      <c r="Y29" s="32">
+      <c r="Y29" s="17">
         <v>2.8614148161068399E-5</v>
       </c>
-      <c r="Z29" s="32">
+      <c r="Z29" s="17">
         <v>0.98452750730514504</v>
       </c>
-      <c r="AA29" s="32">
+      <c r="AA29" s="17">
         <v>0.98452728366851805</v>
       </c>
-      <c r="AB29" s="32">
+      <c r="AB29" s="17">
         <v>47.195258300781198</v>
       </c>
-      <c r="AC29" s="33">
+      <c r="AC29" s="18">
         <v>47.304651504516599</v>
       </c>
     </row>
@@ -6096,8 +6050,338 @@
     <mergeCell ref="Z22:AA22"/>
     <mergeCell ref="AB22:AC22"/>
   </mergeCells>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ2:AQ7">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ7">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ2:AQ6">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR2:AR7">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR2:AR6">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS2:AS7">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS2:AS6">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q24:Q27">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S24:S27">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U24:U27">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X24:X27">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z24:Z27">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB24:AB27">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y24:Y27">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K38">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M38">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J38">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4 B6">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4 F6">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:B7 B4">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:D7 D4">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:F7 F4">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6107,7 +6391,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D8">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6117,7 +6401,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F8">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6126,28 +6410,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B7">
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D7">
-    <cfRule type="colorScale" priority="44">
+  <conditionalFormatting sqref="I3:I8">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6156,167 +6420,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F7">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ2:AQ7">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ7">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ2:AQ6">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR2:AR7">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR2:AR6">
-    <cfRule type="colorScale" priority="48">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AS2:AS7">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AS2:AS6">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q24:Q27">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S24:S27">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U24:U27">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X24:X27">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z24:Z27">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB24:AB27">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y24:Y27">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K38">
+  <conditionalFormatting sqref="J3:J8">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -6326,23 +6430,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M38">
+  <conditionalFormatting sqref="C3:C8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J38">
+  <conditionalFormatting sqref="E3:E8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
report.xlsx for V5 TL was updated
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3389D4CB-D652-4753-A2C5-568746F9FFDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B4A037-5658-4B1A-97DC-47487D28DF01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -91,13 +91,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -366,11 +372,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -430,6 +449,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4528,8 +4552,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AY38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="A8" sqref="A1:G8"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5399,7 +5423,7 @@
       <c r="A20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="20"/>
@@ -5441,7 +5465,7 @@
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="11">
         <v>5</v>
       </c>
       <c r="C21" s="23"/>
@@ -5530,10 +5554,10 @@
       <c r="AC22" s="32"/>
     </row>
     <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -5612,47 +5636,47 @@
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="15">
         <v>25</v>
       </c>
-      <c r="B24" s="1">
-        <v>2.4653750238940098E-4</v>
+      <c r="B24" s="15">
+        <v>1.0335394195863E-4</v>
       </c>
       <c r="C24" s="1">
-        <v>1.6380583521095101E-4</v>
+        <v>1.32593137650474E-4</v>
       </c>
       <c r="D24" s="1">
-        <v>0.97098705768585203</v>
+        <v>0.972033457756042</v>
       </c>
       <c r="E24" s="1">
-        <v>0.97596170330047605</v>
+        <v>0.97174575626850102</v>
       </c>
       <c r="F24" s="1">
-        <v>37.838398132324201</v>
+        <v>40.792933502197201</v>
       </c>
       <c r="G24" s="1">
-        <v>38.738027618408204</v>
+        <v>39.996493787765502</v>
       </c>
       <c r="H24" s="10">
-        <v>20</v>
-      </c>
-      <c r="I24" s="15">
-        <v>3.9403537084581299E-5</v>
+        <v>15</v>
+      </c>
+      <c r="I24" s="1">
+        <v>3.5954642553406297E-5</v>
       </c>
       <c r="J24" s="1">
-        <v>7.2134182042645902E-5</v>
+        <v>4.7578173664533001E-5</v>
       </c>
       <c r="K24" s="1">
-        <v>0.98528852224349905</v>
+        <v>0.983779838085174</v>
       </c>
       <c r="L24" s="1">
-        <v>0.984893836021423</v>
+        <v>0.98361665859818403</v>
       </c>
       <c r="M24" s="1">
-        <v>45.241317138671803</v>
+        <v>45.756995849609297</v>
       </c>
       <c r="N24" s="2">
-        <v>43.585022903442301</v>
+        <v>45.165402994155798</v>
       </c>
       <c r="P24" s="10">
         <v>25</v>
@@ -5698,47 +5722,47 @@
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="15">
         <v>50</v>
       </c>
-      <c r="B25" s="1">
-        <v>2.3111993759812301E-4</v>
+      <c r="B25" s="15">
+        <v>1.2837137142923799E-4</v>
       </c>
       <c r="C25" s="1">
-        <v>1.6380583521095101E-4</v>
+        <v>1.1997246892406099E-4</v>
       </c>
       <c r="D25" s="1">
-        <v>0.97455258607864303</v>
+        <v>0.973419519662857</v>
       </c>
       <c r="E25" s="1">
-        <v>0.97596170330047605</v>
+        <v>0.97225018918514206</v>
       </c>
       <c r="F25" s="1">
-        <v>37.491713485717703</v>
+        <v>40.158833007812497</v>
       </c>
       <c r="G25" s="1">
-        <v>38.738027618408204</v>
+        <v>40.475180215835501</v>
       </c>
       <c r="H25" s="10">
-        <v>15</v>
-      </c>
-      <c r="I25" s="15">
-        <v>3.9216583481902401E-5</v>
+        <v>20</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2.61542236421519E-5</v>
       </c>
       <c r="J25" s="1">
-        <v>5.7327120801346602E-5</v>
+        <v>3.00627074466319E-5</v>
       </c>
       <c r="K25" s="1">
-        <v>0.98647799134254399</v>
+        <v>0.99003720998764</v>
       </c>
       <c r="L25" s="1">
-        <v>0.98440427637100203</v>
+        <v>0.98952884152531595</v>
       </c>
       <c r="M25" s="1">
-        <v>45.802333297729398</v>
+        <v>48.122237396240202</v>
       </c>
       <c r="N25" s="2">
-        <v>44.442697509765601</v>
+        <v>47.562640924453703</v>
       </c>
       <c r="P25" s="10">
         <v>50</v>
@@ -5784,47 +5808,47 @@
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="15">
         <v>75</v>
       </c>
-      <c r="B26" s="1">
-        <v>5.2472879542619897E-5</v>
+      <c r="B26" s="15">
+        <v>1.2182683548113901E-4</v>
       </c>
       <c r="C26" s="1">
-        <v>1.6380583521095101E-4</v>
+        <v>1.26625652783332E-4</v>
       </c>
       <c r="D26" s="1">
-        <v>0.98518298149108796</v>
+        <v>0.97219605843226098</v>
       </c>
       <c r="E26" s="1">
-        <v>0.97596170330047605</v>
+        <v>0.97192650988698004</v>
       </c>
       <c r="F26" s="1">
-        <v>44.5394985961914</v>
+        <v>40.411686019897402</v>
       </c>
       <c r="G26" s="1">
-        <v>38.738027618408204</v>
+        <v>40.215824222564699</v>
       </c>
       <c r="H26" s="10">
-        <v>13</v>
-      </c>
-      <c r="I26" s="15">
-        <v>3.9045478309465802E-5</v>
+        <v>25</v>
+      </c>
+      <c r="I26" s="1">
+        <v>2.58598325490311E-5</v>
       </c>
       <c r="J26" s="1">
-        <v>4.8959196778014297E-5</v>
+        <v>2.6632548518819001E-5</v>
       </c>
       <c r="K26" s="1">
-        <v>0.98727482398350996</v>
+        <v>0.99063826402028399</v>
       </c>
       <c r="L26" s="1">
-        <v>0.98669388318061801</v>
+        <v>0.99046635508537295</v>
       </c>
       <c r="M26" s="1">
-        <v>45.909998931884701</v>
+        <v>48.085835418701102</v>
       </c>
       <c r="N26" s="2">
-        <v>45.086626022338798</v>
+        <v>47.838170747756898</v>
       </c>
       <c r="P26" s="10">
         <v>75</v>
@@ -5870,47 +5894,47 @@
       </c>
     </row>
     <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+      <c r="A27" s="3">
         <v>100</v>
       </c>
-      <c r="B27" s="4">
-        <v>2.12330623944581E-4</v>
+      <c r="B27" s="3">
+        <v>1.2481739358918199E-4</v>
       </c>
       <c r="C27" s="4">
-        <v>1.6380583521095101E-4</v>
+        <v>1.27318583963642E-4</v>
       </c>
       <c r="D27" s="4">
-        <v>0.97309926092624599</v>
+        <v>0.97236944019794402</v>
       </c>
       <c r="E27" s="4">
-        <v>0.97596170330047605</v>
+        <v>0.97191345453262301</v>
       </c>
       <c r="F27" s="4">
-        <v>37.719122200012201</v>
+        <v>40.242696590423499</v>
       </c>
       <c r="G27" s="4">
-        <v>38.738027618408204</v>
+        <v>40.189842977523803</v>
       </c>
       <c r="H27" s="11">
-        <v>10</v>
-      </c>
-      <c r="I27" s="3">
-        <v>3.7516255051741599E-5</v>
+        <v>30</v>
+      </c>
+      <c r="I27" s="35">
+        <v>2.4371969143430699E-5</v>
       </c>
       <c r="J27" s="4">
-        <v>4.8215005996098602E-5</v>
+        <v>2.62564474564896E-5</v>
       </c>
       <c r="K27" s="4">
-        <v>0.98767679333686798</v>
+        <v>0.990291525125503</v>
       </c>
       <c r="L27" s="4">
-        <v>0.98690433216094897</v>
+        <v>0.98999376922845805</v>
       </c>
       <c r="M27" s="4">
-        <v>45.932556419372503</v>
+        <v>48.127189064025799</v>
       </c>
       <c r="N27" s="5">
-        <v>45.130912704467697</v>
+        <v>47.923927621841401</v>
       </c>
       <c r="P27" s="11">
         <v>100</v>
@@ -5955,8 +5979,13 @@
         <v>47.355676757812503</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="34"/>
+      <c r="K28" s="33"/>
+    </row>
     <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
       <c r="P29" s="19">
         <v>200</v>
       </c>
@@ -5999,6 +6028,13 @@
       <c r="AC29" s="18">
         <v>47.304651504516599</v>
       </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J31" s="33"/>
     </row>
     <row r="38" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I38" s="1"/>

</xml_diff>

<commit_message>
loss values were filled in wrong place, were fixed
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B4A037-5658-4B1A-97DC-47487D28DF01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033F749F-2013-4210-95CB-E8F73F59D400}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -410,6 +410,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,11 +454,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4553,7 +4553,7 @@
   <dimension ref="A1:AY38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4579,24 +4579,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="32"/>
+      <c r="G1" s="37"/>
     </row>
     <row r="2" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
@@ -4873,40 +4873,40 @@
       <c r="B11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="26" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="22"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="27"/>
       <c r="P11" s="13" t="s">
         <v>13</v>
       </c>
       <c r="Q11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="R11" s="20"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="22"/>
-      <c r="W11" s="26" t="s">
+      <c r="R11" s="25"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="22"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="26"/>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="26"/>
+      <c r="AC11" s="27"/>
       <c r="AP11" s="10">
         <v>25</v>
       </c>
@@ -4939,36 +4939,36 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="30"/>
       <c r="P12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
       </c>
-      <c r="R12" s="23"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="25"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="29"/>
+      <c r="AB12" s="29"/>
+      <c r="AC12" s="30"/>
       <c r="AP12" s="10">
         <v>50</v>
       </c>
@@ -4996,57 +4996,57 @@
     </row>
     <row r="13" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30" t="s">
+      <c r="E13" s="35"/>
+      <c r="F13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="31" t="s">
+      <c r="G13" s="35"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30" t="s">
+      <c r="J13" s="35"/>
+      <c r="K13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30" t="s">
+      <c r="L13" s="35"/>
+      <c r="M13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="32"/>
+      <c r="N13" s="37"/>
       <c r="P13" s="15"/>
-      <c r="Q13" s="29" t="s">
+      <c r="Q13" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30" t="s">
+      <c r="R13" s="35"/>
+      <c r="S13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30" t="s">
+      <c r="T13" s="35"/>
+      <c r="U13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="V13" s="30"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="31" t="s">
+      <c r="V13" s="35"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="30" t="s">
+      <c r="Y13" s="35"/>
+      <c r="Z13" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AA13" s="30"/>
-      <c r="AB13" s="30" t="s">
+      <c r="AA13" s="35"/>
+      <c r="AB13" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="AC13" s="32"/>
+      <c r="AC13" s="37"/>
       <c r="AP13" s="10">
         <v>75</v>
       </c>
@@ -5094,7 +5094,7 @@
       <c r="G14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="4" t="s">
         <v>8</v>
       </c>
@@ -5134,7 +5134,7 @@
       <c r="V14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W14" s="28"/>
+      <c r="W14" s="33"/>
       <c r="X14" s="4" t="s">
         <v>8</v>
       </c>
@@ -5198,45 +5198,19 @@
       <c r="P15" s="10">
         <v>25</v>
       </c>
-      <c r="Q15" s="1">
-        <v>6.0605635298997999E-5</v>
-      </c>
-      <c r="R15" s="1">
-        <v>3.8013758665329002E-5</v>
-      </c>
-      <c r="S15" s="1">
-        <v>0.98883432388305603</v>
-      </c>
-      <c r="T15" s="1">
-        <v>0.98978726458549504</v>
-      </c>
-      <c r="U15" s="1">
-        <v>44.758236083984301</v>
-      </c>
-      <c r="V15" s="1">
-        <v>45.553018432617101</v>
-      </c>
-      <c r="W15" s="10">
-        <v>13</v>
-      </c>
-      <c r="X15" s="1">
-        <v>2.6277137367287602E-5</v>
-      </c>
-      <c r="Y15" s="1">
-        <v>4.7515599329926699E-5</v>
-      </c>
-      <c r="Z15" s="1">
-        <v>0.98946990489959696</v>
-      </c>
-      <c r="AA15" s="1">
-        <v>0.98824352288246098</v>
-      </c>
-      <c r="AB15" s="1">
-        <v>46.518804321288997</v>
-      </c>
-      <c r="AC15" s="2">
-        <v>45.308811874389598</v>
-      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="2"/>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
@@ -5258,45 +5232,19 @@
       <c r="P16" s="10">
         <v>50</v>
       </c>
-      <c r="Q16" s="1">
-        <v>4.2669727326938302E-5</v>
-      </c>
-      <c r="R16" s="1">
-        <v>3.8013758665329002E-5</v>
-      </c>
-      <c r="S16" s="1">
-        <v>0.98951791763305597</v>
-      </c>
-      <c r="T16" s="1">
-        <v>0.98978726458549504</v>
-      </c>
-      <c r="U16" s="1">
-        <v>45.472197189330998</v>
-      </c>
-      <c r="V16" s="1">
-        <v>45.553018432617101</v>
-      </c>
-      <c r="W16" s="10">
-        <v>11</v>
-      </c>
-      <c r="X16" s="1">
-        <v>2.3706448064331199E-5</v>
-      </c>
-      <c r="Y16" s="1">
-        <v>4.1465255450020698E-5</v>
-      </c>
-      <c r="Z16" s="1">
-        <v>0.99027964830398496</v>
-      </c>
-      <c r="AA16" s="1">
-        <v>0.98803000092506399</v>
-      </c>
-      <c r="AB16" s="1">
-        <v>47.521706008911103</v>
-      </c>
-      <c r="AC16" s="2">
-        <v>45.765523239135703</v>
-      </c>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="2"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -5318,45 +5266,19 @@
       <c r="P17" s="10">
         <v>75</v>
       </c>
-      <c r="Q17" s="1">
-        <v>5.0710975428955802E-5</v>
-      </c>
-      <c r="R17" s="1">
-        <v>3.8013758665329002E-5</v>
-      </c>
-      <c r="S17" s="1">
-        <v>0.98911257743835401</v>
-      </c>
-      <c r="T17" s="1">
-        <v>0.98978726458549504</v>
-      </c>
-      <c r="U17" s="1">
-        <v>45.241755879720003</v>
-      </c>
-      <c r="V17" s="1">
-        <v>45.553018432617101</v>
-      </c>
-      <c r="W17" s="10">
-        <v>12</v>
-      </c>
-      <c r="X17" s="1">
-        <v>3.0852467843942503E-5</v>
-      </c>
-      <c r="Y17" s="1">
-        <v>4.0872855341149197E-5</v>
-      </c>
-      <c r="Z17" s="1">
-        <v>0.98987901608149198</v>
-      </c>
-      <c r="AA17" s="1">
-        <v>0.98891655802726697</v>
-      </c>
-      <c r="AB17" s="1">
-        <v>46.963905639648402</v>
-      </c>
-      <c r="AC17" s="2">
-        <v>45.852032043457001</v>
-      </c>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="2"/>
     </row>
     <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
@@ -5378,88 +5300,62 @@
       <c r="P18" s="11">
         <v>100</v>
       </c>
-      <c r="Q18" s="4">
-        <v>4.5256131484165903E-5</v>
-      </c>
-      <c r="R18" s="4">
-        <v>3.8013758665329002E-5</v>
-      </c>
-      <c r="S18" s="4">
-        <v>0.98969455003738405</v>
-      </c>
-      <c r="T18" s="4">
-        <v>0.98978726458549504</v>
-      </c>
-      <c r="U18" s="4">
-        <v>45.500738525390602</v>
-      </c>
-      <c r="V18" s="4">
-        <v>45.553018432617101</v>
-      </c>
-      <c r="W18" s="11">
-        <v>10</v>
-      </c>
-      <c r="X18" s="4">
-        <v>3.01593978929304E-5</v>
-      </c>
-      <c r="Y18" s="4">
-        <v>3.8595762001932601E-5</v>
-      </c>
-      <c r="Z18" s="4">
-        <v>0.98965702772140496</v>
-      </c>
-      <c r="AA18" s="4">
-        <v>0.98832294464111303</v>
-      </c>
-      <c r="AB18" s="4">
-        <v>46.934795570373502</v>
-      </c>
-      <c r="AC18" s="5">
-        <v>45.775898559570301</v>
-      </c>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="5"/>
     </row>
     <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="26" t="s">
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="22"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="27"/>
       <c r="P20" s="13" t="s">
         <v>13</v>
       </c>
       <c r="Q20" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="20"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="22"/>
-      <c r="W20" s="26" t="s">
+      <c r="R20" s="25"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="21"/>
-      <c r="AC20" s="22"/>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="26"/>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
+      <c r="AC20" s="27"/>
     </row>
     <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -5468,93 +5364,93 @@
       <c r="B21" s="11">
         <v>5</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="25"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
       <c r="P21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q21" s="5">
         <v>5</v>
       </c>
-      <c r="R21" s="23"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="25"/>
-      <c r="W21" s="27"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="24"/>
-      <c r="AC21" s="25"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="29"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="30"/>
     </row>
     <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30" t="s">
+      <c r="C22" s="35"/>
+      <c r="D22" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30" t="s">
+      <c r="E22" s="35"/>
+      <c r="F22" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="31" t="s">
+      <c r="G22" s="35"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30" t="s">
+      <c r="J22" s="35"/>
+      <c r="K22" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30" t="s">
+      <c r="L22" s="35"/>
+      <c r="M22" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="N22" s="32"/>
+      <c r="N22" s="37"/>
       <c r="P22" s="15"/>
-      <c r="Q22" s="29" t="s">
+      <c r="Q22" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="R22" s="30"/>
-      <c r="S22" s="30" t="s">
+      <c r="R22" s="35"/>
+      <c r="S22" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="T22" s="30"/>
-      <c r="U22" s="30" t="s">
+      <c r="T22" s="35"/>
+      <c r="U22" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="V22" s="30"/>
-      <c r="W22" s="27"/>
-      <c r="X22" s="31" t="s">
+      <c r="V22" s="35"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="Y22" s="30"/>
-      <c r="Z22" s="30" t="s">
+      <c r="Y22" s="35"/>
+      <c r="Z22" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AA22" s="30"/>
-      <c r="AB22" s="30" t="s">
+      <c r="AA22" s="35"/>
+      <c r="AB22" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="AC22" s="32"/>
+      <c r="AC22" s="37"/>
     </row>
     <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -5575,7 +5471,7 @@
       <c r="G23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="28"/>
+      <c r="H23" s="33"/>
       <c r="I23" s="3" t="s">
         <v>8</v>
       </c>
@@ -5615,7 +5511,7 @@
       <c r="V23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W23" s="28"/>
+      <c r="W23" s="33"/>
       <c r="X23" s="3" t="s">
         <v>8</v>
       </c>
@@ -5639,402 +5535,272 @@
       <c r="A24" s="15">
         <v>25</v>
       </c>
-      <c r="B24" s="15">
-        <v>1.0335394195863E-4</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1.32593137650474E-4</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0.972033457756042</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0.97174575626850102</v>
-      </c>
-      <c r="F24" s="1">
-        <v>40.792933502197201</v>
-      </c>
-      <c r="G24" s="1">
-        <v>39.996493787765502</v>
-      </c>
-      <c r="H24" s="10">
-        <v>15</v>
-      </c>
-      <c r="I24" s="1">
-        <v>3.5954642553406297E-5</v>
-      </c>
-      <c r="J24" s="1">
-        <v>4.7578173664533001E-5</v>
-      </c>
-      <c r="K24" s="1">
-        <v>0.983779838085174</v>
-      </c>
-      <c r="L24" s="1">
-        <v>0.98361665859818403</v>
-      </c>
-      <c r="M24" s="1">
-        <v>45.756995849609297</v>
-      </c>
-      <c r="N24" s="2">
-        <v>45.165402994155798</v>
-      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="2"/>
       <c r="P24" s="10">
         <v>25</v>
       </c>
-      <c r="Q24" s="1">
-        <v>1.87023348844377E-4</v>
+      <c r="Q24" s="15">
+        <v>1.0335394195863E-4</v>
       </c>
       <c r="R24" s="1">
-        <v>1.22301794988743E-4</v>
+        <v>1.32593137650474E-4</v>
       </c>
       <c r="S24" s="1">
-        <v>0.97240586042404098</v>
+        <v>0.972033457756042</v>
       </c>
       <c r="T24" s="1">
-        <v>0.97232422828674303</v>
+        <v>0.97174575626850102</v>
       </c>
       <c r="U24" s="1">
-        <v>39.379602890014603</v>
+        <v>40.792933502197201</v>
       </c>
       <c r="V24" s="1">
-        <v>40.267239433288502</v>
+        <v>39.996493787765502</v>
       </c>
       <c r="W24" s="10">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="X24" s="1">
-        <v>2.61555348333786E-5</v>
+        <v>3.5954642553406297E-5</v>
       </c>
       <c r="Y24" s="1">
-        <v>5.0274230328795899E-5</v>
+        <v>4.7578173664533001E-5</v>
       </c>
       <c r="Z24" s="1">
-        <v>0.98747579097747795</v>
+        <v>0.983779838085174</v>
       </c>
       <c r="AA24" s="1">
-        <v>0.986951784372329</v>
+        <v>0.98361665859818403</v>
       </c>
       <c r="AB24" s="1">
-        <v>46.992552947998</v>
+        <v>45.756995849609297</v>
       </c>
       <c r="AC24" s="2">
-        <v>45.924456985473597</v>
+        <v>45.165402994155798</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>50</v>
       </c>
-      <c r="B25" s="15">
-        <v>1.2837137142923799E-4</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1.1997246892406099E-4</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0.973419519662857</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0.97225018918514206</v>
-      </c>
-      <c r="F25" s="1">
-        <v>40.158833007812497</v>
-      </c>
-      <c r="G25" s="1">
-        <v>40.475180215835501</v>
-      </c>
-      <c r="H25" s="10">
-        <v>20</v>
-      </c>
-      <c r="I25" s="1">
-        <v>2.61542236421519E-5</v>
-      </c>
-      <c r="J25" s="1">
-        <v>3.00627074466319E-5</v>
-      </c>
-      <c r="K25" s="1">
-        <v>0.99003720998764</v>
-      </c>
-      <c r="L25" s="1">
-        <v>0.98952884152531595</v>
-      </c>
-      <c r="M25" s="1">
-        <v>48.122237396240202</v>
-      </c>
-      <c r="N25" s="2">
-        <v>47.562640924453703</v>
-      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="2"/>
       <c r="P25" s="10">
         <v>50</v>
       </c>
-      <c r="Q25" s="1">
-        <v>1.7721809726936E-4</v>
+      <c r="Q25" s="15">
+        <v>1.2837137142923799E-4</v>
       </c>
       <c r="R25" s="1">
-        <v>1.22301794988743E-4</v>
+        <v>1.1997246892406099E-4</v>
       </c>
       <c r="S25" s="1">
-        <v>0.97305006861686705</v>
+        <v>0.973419519662857</v>
       </c>
       <c r="T25" s="1">
-        <v>0.97232422828674303</v>
+        <v>0.97225018918514206</v>
       </c>
       <c r="U25" s="1">
-        <v>39.059421005249</v>
+        <v>40.158833007812497</v>
       </c>
       <c r="V25" s="1">
-        <v>40.267239433288502</v>
+        <v>40.475180215835501</v>
       </c>
       <c r="W25" s="10">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="X25" s="1">
-        <v>2.8246186520846E-5</v>
+        <v>2.61542236421519E-5</v>
       </c>
       <c r="Y25" s="1">
-        <v>3.7750013843833499E-5</v>
+        <v>3.00627074466319E-5</v>
       </c>
       <c r="Z25" s="1">
-        <v>0.98940120100975004</v>
+        <v>0.99003720998764</v>
       </c>
       <c r="AA25" s="1">
-        <v>0.98895520210266097</v>
+        <v>0.98952884152531595</v>
       </c>
       <c r="AB25" s="1">
-        <v>47.8213184356689</v>
+        <v>48.122237396240202</v>
       </c>
       <c r="AC25" s="2">
-        <v>46.968940277099598</v>
+        <v>47.562640924453703</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>75</v>
       </c>
-      <c r="B26" s="15">
-        <v>1.2182683548113901E-4</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1.26625652783332E-4</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0.97219605843226098</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0.97192650988698004</v>
-      </c>
-      <c r="F26" s="1">
-        <v>40.411686019897402</v>
-      </c>
-      <c r="G26" s="1">
-        <v>40.215824222564699</v>
-      </c>
-      <c r="H26" s="10">
-        <v>25</v>
-      </c>
-      <c r="I26" s="1">
-        <v>2.58598325490311E-5</v>
-      </c>
-      <c r="J26" s="1">
-        <v>2.6632548518819001E-5</v>
-      </c>
-      <c r="K26" s="1">
-        <v>0.99063826402028399</v>
-      </c>
-      <c r="L26" s="1">
-        <v>0.99046635508537295</v>
-      </c>
-      <c r="M26" s="1">
-        <v>48.085835418701102</v>
-      </c>
-      <c r="N26" s="2">
-        <v>47.838170747756898</v>
-      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="2"/>
       <c r="P26" s="10">
         <v>75</v>
       </c>
-      <c r="Q26" s="1">
-        <v>1.61925740151976E-4</v>
+      <c r="Q26" s="15">
+        <v>1.2182683548113901E-4</v>
       </c>
       <c r="R26" s="1">
-        <v>1.22301794988743E-4</v>
+        <v>1.26625652783332E-4</v>
       </c>
       <c r="S26" s="1">
-        <v>0.97214901447296098</v>
+        <v>0.97219605843226098</v>
       </c>
       <c r="T26" s="1">
-        <v>0.97232422828674303</v>
+        <v>0.97192650988698004</v>
       </c>
       <c r="U26" s="1">
-        <v>39.407296702067001</v>
+        <v>40.411686019897402</v>
       </c>
       <c r="V26" s="1">
-        <v>40.267239433288502</v>
+        <v>40.215824222564699</v>
       </c>
       <c r="W26" s="10">
-        <v>22</v>
-      </c>
-      <c r="X26" s="15">
-        <v>2.94253816173295E-5</v>
+        <v>25</v>
+      </c>
+      <c r="X26" s="1">
+        <v>2.58598325490311E-5</v>
       </c>
       <c r="Y26" s="1">
-        <v>3.2551214095292297E-5</v>
+        <v>2.6632548518819001E-5</v>
       </c>
       <c r="Z26" s="1">
-        <v>0.98908270676930699</v>
+        <v>0.99063826402028399</v>
       </c>
       <c r="AA26" s="1">
-        <v>0.988458636760711</v>
+        <v>0.99046635508537295</v>
       </c>
       <c r="AB26" s="1">
-        <v>47.706615549723303</v>
+        <v>48.085835418701102</v>
       </c>
       <c r="AC26" s="2">
-        <v>47.325179077148398</v>
+        <v>47.838170747756898</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>100</v>
       </c>
-      <c r="B27" s="3">
-        <v>1.2481739358918199E-4</v>
-      </c>
-      <c r="C27" s="4">
-        <v>1.27318583963642E-4</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.97236944019794402</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0.97191345453262301</v>
-      </c>
-      <c r="F27" s="4">
-        <v>40.242696590423499</v>
-      </c>
-      <c r="G27" s="4">
-        <v>40.189842977523803</v>
-      </c>
-      <c r="H27" s="11">
-        <v>30</v>
-      </c>
-      <c r="I27" s="35">
-        <v>2.4371969143430699E-5</v>
-      </c>
-      <c r="J27" s="4">
-        <v>2.62564474564896E-5</v>
-      </c>
-      <c r="K27" s="4">
-        <v>0.990291525125503</v>
-      </c>
-      <c r="L27" s="4">
-        <v>0.98999376922845805</v>
-      </c>
-      <c r="M27" s="4">
-        <v>48.127189064025799</v>
-      </c>
-      <c r="N27" s="5">
-        <v>47.923927621841401</v>
-      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="5"/>
       <c r="P27" s="11">
         <v>100</v>
       </c>
-      <c r="Q27" s="4">
-        <v>1.5695816919105701E-4</v>
+      <c r="Q27" s="3">
+        <v>1.2481739358918199E-4</v>
       </c>
       <c r="R27" s="4">
-        <v>1.22301794988743E-4</v>
+        <v>1.27318583963642E-4</v>
       </c>
       <c r="S27" s="4">
-        <v>0.97247086942195804</v>
+        <v>0.97236944019794402</v>
       </c>
       <c r="T27" s="4">
-        <v>0.97232422828674303</v>
+        <v>0.97191345453262301</v>
       </c>
       <c r="U27" s="4">
-        <v>39.453057918548502</v>
+        <v>40.242696590423499</v>
       </c>
       <c r="V27" s="4">
-        <v>40.267239433288502</v>
+        <v>40.189842977523803</v>
       </c>
       <c r="W27" s="11">
-        <v>13</v>
-      </c>
-      <c r="X27" s="3">
-        <v>2.9531874833992299E-5</v>
+        <v>30</v>
+      </c>
+      <c r="X27" s="22">
+        <v>2.4371969143430699E-5</v>
       </c>
       <c r="Y27" s="4">
-        <v>3.2329415906133299E-5</v>
+        <v>2.62564474564896E-5</v>
       </c>
       <c r="Z27" s="4">
-        <v>0.98975329101085596</v>
+        <v>0.990291525125503</v>
       </c>
       <c r="AA27" s="4">
-        <v>0.98950933218002302</v>
+        <v>0.98999376922845805</v>
       </c>
       <c r="AB27" s="4">
-        <v>47.705362815856901</v>
+        <v>48.127189064025799</v>
       </c>
       <c r="AC27" s="5">
-        <v>47.355676757812503</v>
+        <v>47.923927621841401</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I28" s="34"/>
-      <c r="K28" s="33"/>
+      <c r="I28" s="21"/>
+      <c r="K28" s="20"/>
     </row>
     <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
       <c r="P29" s="19">
         <v>200</v>
       </c>
-      <c r="Q29" s="17">
-        <v>1.0744010523922E-4</v>
-      </c>
-      <c r="R29" s="17">
-        <v>1.3207085607427801E-4</v>
-      </c>
-      <c r="S29" s="17">
-        <v>0.97247788453102102</v>
-      </c>
-      <c r="T29" s="17">
-        <v>0.97338824462890605</v>
-      </c>
-      <c r="U29" s="17">
-        <v>40.785670326232903</v>
-      </c>
-      <c r="V29" s="17">
-        <v>40.443220672607403</v>
-      </c>
-      <c r="W29" s="19">
-        <v>15</v>
-      </c>
-      <c r="X29" s="17">
-        <v>2.6981619124853701E-5</v>
-      </c>
-      <c r="Y29" s="17">
-        <v>2.8614148161068399E-5</v>
-      </c>
-      <c r="Z29" s="17">
-        <v>0.98452750730514504</v>
-      </c>
-      <c r="AA29" s="17">
-        <v>0.98452728366851805</v>
-      </c>
-      <c r="AB29" s="17">
-        <v>47.195258300781198</v>
-      </c>
-      <c r="AC29" s="18">
-        <v>47.304651504516599</v>
-      </c>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="17"/>
+      <c r="Y29" s="17"/>
+      <c r="Z29" s="17"/>
+      <c r="AA29" s="17"/>
+      <c r="AB29" s="17"/>
+      <c r="AC29" s="18"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J31" s="33"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="38" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I38" s="1"/>
@@ -6045,15 +5811,21 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C20:G21"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:N21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="R20:V21"/>
+    <mergeCell ref="W20:W23"/>
+    <mergeCell ref="X20:AC21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="R11:V12"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
@@ -6070,24 +5842,18 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="R11:V12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="R20:V21"/>
-    <mergeCell ref="W20:W23"/>
-    <mergeCell ref="X20:AC21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="C20:G21"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:N21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
   </mergeCells>
   <conditionalFormatting sqref="B4">
-    <cfRule type="colorScale" priority="60">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6097,7 +5863,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="58">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6107,7 +5873,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="colorScale" priority="57">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6117,7 +5883,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="colorScale" priority="61">
+    <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6127,7 +5893,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="63">
+    <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6137,7 +5903,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="colorScale" priority="65">
+    <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6147,7 +5913,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ7">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6157,7 +5923,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ7">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6167,7 +5933,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ6">
-    <cfRule type="colorScale" priority="66">
+    <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6177,6 +5943,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR2:AR7">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR2:AR6">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS2:AS7">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -6186,8 +5972,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AR2:AR6">
-    <cfRule type="colorScale" priority="67">
+  <conditionalFormatting sqref="AS2:AS6">
+    <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6196,98 +5982,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS2:AS7">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AS2:AS6">
-    <cfRule type="colorScale" priority="68">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q24:Q27">
-    <cfRule type="colorScale" priority="45">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S24:S27">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U24:U27">
-    <cfRule type="colorScale" priority="43">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X24:X27">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z24:Z27">
-    <cfRule type="colorScale" priority="41">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB24:AB27">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y24:Y27">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6297,7 +5993,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6307,7 +6003,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M38">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6317,6 +6013,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -6326,28 +6042,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
+  <conditionalFormatting sqref="D6">
     <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6357,7 +6053,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6366,7 +6062,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4 B6">
+  <conditionalFormatting sqref="B6 B4">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6 F4">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:B7 B4">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -6376,7 +6092,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4 F6">
+  <conditionalFormatting sqref="D6:D7 D4">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -6386,8 +6102,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B7 B4">
+  <conditionalFormatting sqref="F6:F7 F4">
     <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B8">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6396,17 +6122,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D7 D4">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F7 F4">
+  <conditionalFormatting sqref="D3:D8">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -6416,17 +6132,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B8">
+  <conditionalFormatting sqref="F3:F8">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
+  <conditionalFormatting sqref="I3:I8">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -6436,7 +6152,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F8">
+  <conditionalFormatting sqref="J3:J8">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -6446,28 +6162,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I8">
+  <conditionalFormatting sqref="C3:C8">
     <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J8">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C8">
-    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6477,7 +6173,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E8">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6487,7 +6183,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G8">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6496,6 +6192,26 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="X24:X27">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y24:Y27">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
updated -NM-AO-2 losses, SSIM dominantes
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A89D0E7-9C5C-44E3-9CD4-D7BDA82ABAC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324174C7-2980-4BA9-8DDC-95C08B412A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="19">
   <si>
     <t>Base Model</t>
   </si>
@@ -389,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -415,6 +415,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4108,16 +4109,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>370453</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>36239</xdr:rowOff>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>496891</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>61528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>59</xdr:col>
-      <xdr:colOff>40075</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>27940</xdr:rowOff>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>166513</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>53229</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4144,16 +4145,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>397653</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>41830</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>144777</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>50</xdr:col>
-      <xdr:colOff>161003</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>67122</xdr:rowOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>848</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25292</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4553,8 +4554,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AY38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4567,37 +4568,46 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="37" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="37" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="13" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="37"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
@@ -4748,35 +4758,35 @@
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
-        <v>3.1105838688745197E-5</v>
+      <c r="B6">
+        <v>2.9113601158314799E-5</v>
       </c>
       <c r="C6" s="1">
-        <v>3.1866090255334703E-5</v>
+        <v>2.95364080477611E-5</v>
       </c>
       <c r="D6" s="1">
-        <v>0.99037553977966297</v>
+        <v>0.99063221335411</v>
       </c>
       <c r="E6" s="1">
-        <v>0.99035752817988398</v>
+        <v>0.99068844288587499</v>
       </c>
       <c r="F6" s="1">
-        <v>46.641133148193298</v>
-      </c>
-      <c r="G6" s="2">
-        <v>46.648111543655297</v>
+        <v>46.891133316039998</v>
+      </c>
+      <c r="G6" s="1">
+        <v>47.021878166198697</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0.97614230172268368</v>
+        <v>0.98568522994527252</v>
       </c>
       <c r="J6">
         <f>(MIN(D6:E6)/MAX(D6:E6))</f>
-        <v>0.9999818133636631</v>
+        <v>0.99994324196252737</v>
       </c>
       <c r="K6">
         <f>(MIN(F6:G6)/MAX(F6:G6))</f>
-        <v>0.99985040347334386</v>
+        <v>0.99721948898560409</v>
       </c>
       <c r="AP6" s="8" t="s">
         <v>4</v>
@@ -4874,6 +4884,7 @@
       </c>
     </row>
     <row r="10" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="39"/>
       <c r="AQ10" t="s">
         <v>8</v>
       </c>
@@ -4894,40 +4905,40 @@
       <c r="B11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="31" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="25"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="27"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="28"/>
       <c r="P11" s="13" t="s">
         <v>13</v>
       </c>
       <c r="Q11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="R11" s="25"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="31" t="s">
+      <c r="R11" s="26"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="27"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="27"/>
+      <c r="AB11" s="27"/>
+      <c r="AC11" s="28"/>
       <c r="AP11" s="10">
         <v>25</v>
       </c>
@@ -4960,36 +4971,36 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="30"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="31"/>
       <c r="P12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
       </c>
-      <c r="R12" s="28"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="28"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="29"/>
-      <c r="AB12" s="29"/>
-      <c r="AC12" s="30"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="30"/>
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="31"/>
       <c r="AP12" s="10">
         <v>50</v>
       </c>
@@ -5017,57 +5028,57 @@
     </row>
     <row r="13" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15"/>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35" t="s">
+      <c r="C13" s="36"/>
+      <c r="D13" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35" t="s">
+      <c r="E13" s="36"/>
+      <c r="F13" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="35"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="36" t="s">
+      <c r="G13" s="36"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35" t="s">
+      <c r="J13" s="36"/>
+      <c r="K13" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35" t="s">
+      <c r="L13" s="36"/>
+      <c r="M13" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="37"/>
+      <c r="N13" s="38"/>
       <c r="P13" s="15"/>
-      <c r="Q13" s="34" t="s">
+      <c r="Q13" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35" t="s">
+      <c r="R13" s="36"/>
+      <c r="S13" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35" t="s">
+      <c r="T13" s="36"/>
+      <c r="U13" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="V13" s="35"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="36" t="s">
+      <c r="V13" s="36"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="35" t="s">
+      <c r="Y13" s="36"/>
+      <c r="Z13" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35" t="s">
+      <c r="AA13" s="36"/>
+      <c r="AB13" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="AC13" s="37"/>
+      <c r="AC13" s="38"/>
       <c r="AP13" s="10">
         <v>75</v>
       </c>
@@ -5115,7 +5126,7 @@
       <c r="G14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="33"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="4" t="s">
         <v>8</v>
       </c>
@@ -5155,7 +5166,7 @@
       <c r="V14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W14" s="33"/>
+      <c r="W14" s="34"/>
       <c r="X14" s="4" t="s">
         <v>8</v>
       </c>
@@ -5219,19 +5230,45 @@
       <c r="P15" s="10">
         <v>25</v>
       </c>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="2"/>
+      <c r="Q15" s="1">
+        <v>2.77512644606758E-5</v>
+      </c>
+      <c r="R15" s="1">
+        <v>3.1265178757848801E-5</v>
+      </c>
+      <c r="S15" s="1">
+        <v>0.98976352453231797</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0.98989894062280603</v>
+      </c>
+      <c r="U15" s="1">
+        <v>46.461437072753903</v>
+      </c>
+      <c r="V15" s="1">
+        <v>46.643888940811102</v>
+      </c>
+      <c r="W15" s="10">
+        <v>20</v>
+      </c>
+      <c r="X15" s="1">
+        <v>2.27695502144342E-5</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>3.2537159670482603E-5</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>0.99060320138931202</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>0.99029955714940998</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>47.047988891601499</v>
+      </c>
+      <c r="AC15" s="2">
+        <v>46.488731241226198</v>
+      </c>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
@@ -5253,21 +5290,47 @@
       <c r="P16" s="10">
         <v>50</v>
       </c>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="2"/>
+      <c r="Q16" s="1">
+        <v>2.54695100375101E-5</v>
+      </c>
+      <c r="R16" s="1">
+        <v>3.2729798145965103E-5</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.99048314452171304</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0.98997791945934299</v>
+      </c>
+      <c r="U16" s="1">
+        <v>47.164205703735298</v>
+      </c>
+      <c r="V16" s="1">
+        <v>46.457026739120401</v>
+      </c>
+      <c r="W16" s="10">
+        <v>10</v>
+      </c>
+      <c r="X16" s="1">
+        <v>2.3715251545581801E-5</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>3.0305313302960698E-5</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>0.99024703741073605</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>0.98945871308445899</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>47.417324676513601</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>46.849895143508903</v>
+      </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>75</v>
       </c>
@@ -5287,21 +5350,47 @@
       <c r="P17" s="10">
         <v>75</v>
       </c>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="2"/>
+      <c r="Q17" s="1">
+        <v>3.3553354593701998E-5</v>
+      </c>
+      <c r="R17" s="1">
+        <v>3.1094688805524097E-5</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0.98963750759760505</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0.989958387464284</v>
+      </c>
+      <c r="U17" s="1">
+        <v>46.817370707194002</v>
+      </c>
+      <c r="V17" s="1">
+        <v>46.688427810668898</v>
+      </c>
+      <c r="W17" s="10">
+        <v>25</v>
+      </c>
+      <c r="X17" s="1">
+        <v>3.11049654252807E-5</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>3.0239778110399101E-5</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>0.98999036073684599</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>0.99016795828938398</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>46.981024729410798</v>
+      </c>
+      <c r="AC17" s="2">
+        <v>46.849209213256799</v>
+      </c>
     </row>
-    <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>100</v>
       </c>
@@ -5321,156 +5410,246 @@
       <c r="P18" s="11">
         <v>100</v>
       </c>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="4"/>
-      <c r="AC18" s="5"/>
+      <c r="Q18" s="4">
+        <v>3.1133355314523201E-5</v>
+      </c>
+      <c r="R18" s="4">
+        <v>3.1063884883906198E-5</v>
+      </c>
+      <c r="S18" s="4">
+        <v>0.98994574248790701</v>
+      </c>
+      <c r="T18" s="4">
+        <v>0.98994714409112905</v>
+      </c>
+      <c r="U18" s="4">
+        <v>46.814664916992101</v>
+      </c>
+      <c r="V18" s="4">
+        <v>46.690697641372601</v>
+      </c>
+      <c r="W18" s="11">
+        <v>25</v>
+      </c>
+      <c r="X18" s="4">
+        <v>2.8949559105058099E-5</v>
+      </c>
+      <c r="Y18" s="4">
+        <v>2.9463366438449099E-5</v>
+      </c>
+      <c r="Z18" s="4">
+        <v>0.99025388300418804</v>
+      </c>
+      <c r="AA18" s="4">
+        <v>0.99022914797067596</v>
+      </c>
+      <c r="AB18" s="4">
+        <v>47.073031196594201</v>
+      </c>
+      <c r="AC18" s="5">
+        <v>46.950528669357297</v>
+      </c>
     </row>
-    <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="31" t="s">
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="25"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="27"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="28"/>
       <c r="P20" s="13" t="s">
         <v>13</v>
       </c>
       <c r="Q20" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="R20" s="25"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="31" t="s">
+      <c r="R20" s="26"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="X20" s="25"/>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="26"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
-      <c r="AC20" s="27"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="27"/>
+      <c r="AB20" s="27"/>
+      <c r="AC20" s="28"/>
+      <c r="AE20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF20" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG20" s="26"/>
+      <c r="AH20" s="27"/>
+      <c r="AI20" s="27"/>
+      <c r="AJ20" s="27"/>
+      <c r="AK20" s="28"/>
+      <c r="AL20" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM20" s="26"/>
+      <c r="AN20" s="27"/>
+      <c r="AO20" s="27"/>
+      <c r="AP20" s="27"/>
+      <c r="AQ20" s="27"/>
+      <c r="AR20" s="28"/>
     </row>
-    <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="11">
         <v>5</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="30"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="31"/>
       <c r="P21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="Q21" s="5">
         <v>5</v>
       </c>
-      <c r="R21" s="28"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="U21" s="29"/>
-      <c r="V21" s="30"/>
-      <c r="W21" s="32"/>
-      <c r="X21" s="28"/>
-      <c r="Y21" s="29"/>
-      <c r="Z21" s="29"/>
-      <c r="AA21" s="29"/>
-      <c r="AB21" s="29"/>
-      <c r="AC21" s="30"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="33"/>
+      <c r="X21" s="29"/>
+      <c r="Y21" s="30"/>
+      <c r="Z21" s="30"/>
+      <c r="AA21" s="30"/>
+      <c r="AB21" s="30"/>
+      <c r="AC21" s="31"/>
+      <c r="AE21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF21" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG21" s="29"/>
+      <c r="AH21" s="30"/>
+      <c r="AI21" s="30"/>
+      <c r="AJ21" s="30"/>
+      <c r="AK21" s="31"/>
+      <c r="AL21" s="33"/>
+      <c r="AM21" s="29"/>
+      <c r="AN21" s="30"/>
+      <c r="AO21" s="30"/>
+      <c r="AP21" s="30"/>
+      <c r="AQ21" s="30"/>
+      <c r="AR21" s="31"/>
     </row>
-    <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35" t="s">
+      <c r="C22" s="36"/>
+      <c r="D22" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35" t="s">
+      <c r="E22" s="36"/>
+      <c r="F22" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="35"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="36" t="s">
+      <c r="G22" s="36"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35" t="s">
+      <c r="J22" s="36"/>
+      <c r="K22" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35" t="s">
+      <c r="L22" s="36"/>
+      <c r="M22" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="N22" s="37"/>
+      <c r="N22" s="38"/>
       <c r="P22" s="15"/>
-      <c r="Q22" s="34" t="s">
+      <c r="Q22" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35" t="s">
+      <c r="R22" s="36"/>
+      <c r="S22" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35" t="s">
+      <c r="T22" s="36"/>
+      <c r="U22" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="V22" s="35"/>
-      <c r="W22" s="32"/>
-      <c r="X22" s="36" t="s">
+      <c r="V22" s="36"/>
+      <c r="W22" s="33"/>
+      <c r="X22" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="Y22" s="35"/>
-      <c r="Z22" s="35" t="s">
+      <c r="Y22" s="36"/>
+      <c r="Z22" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="AA22" s="35"/>
-      <c r="AB22" s="35" t="s">
+      <c r="AA22" s="36"/>
+      <c r="AB22" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="AC22" s="37"/>
+      <c r="AC22" s="38"/>
+      <c r="AE22" s="15"/>
+      <c r="AF22" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG22" s="36"/>
+      <c r="AH22" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI22" s="36"/>
+      <c r="AJ22" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK22" s="36"/>
+      <c r="AL22" s="33"/>
+      <c r="AM22" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN22" s="36"/>
+      <c r="AO22" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP22" s="36"/>
+      <c r="AQ22" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR22" s="38"/>
     </row>
-    <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
         <v>15</v>
       </c>
@@ -5492,7 +5671,7 @@
       <c r="G23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H23" s="33"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="3" t="s">
         <v>8</v>
       </c>
@@ -5532,7 +5711,7 @@
       <c r="V23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="W23" s="33"/>
+      <c r="W23" s="34"/>
       <c r="X23" s="3" t="s">
         <v>8</v>
       </c>
@@ -5551,8 +5730,48 @@
       <c r="AC23" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="AE23" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL23" s="34"/>
+      <c r="AM23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AN23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AP23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR23" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>25</v>
       </c>
@@ -5580,16 +5799,16 @@
       <c r="I24" s="13">
         <v>2.7744608341890799E-5</v>
       </c>
-      <c r="J24" s="38">
+      <c r="J24" s="25">
         <v>4.22422099313735E-5</v>
       </c>
-      <c r="K24" s="38">
+      <c r="K24" s="25">
         <v>0.98809633493423399</v>
       </c>
-      <c r="L24" s="38">
+      <c r="L24" s="25">
         <v>0.98773940578103003</v>
       </c>
-      <c r="M24" s="38">
+      <c r="M24" s="25">
         <v>46.455945434570303</v>
       </c>
       <c r="N24" s="14">
@@ -5637,8 +5856,48 @@
       <c r="AC24" s="2">
         <v>47.000839977264398</v>
       </c>
+      <c r="AE24" s="10">
+        <v>25</v>
+      </c>
+      <c r="AF24" s="1">
+        <v>9.2854484391864295E-5</v>
+      </c>
+      <c r="AG24" s="1">
+        <v>1.2343351113031499E-4</v>
+      </c>
+      <c r="AH24" s="1">
+        <v>0.975373094081878</v>
+      </c>
+      <c r="AI24" s="1">
+        <v>0.97568958029150898</v>
+      </c>
+      <c r="AJ24" s="1">
+        <v>41.184127807617102</v>
+      </c>
+      <c r="AK24" s="1">
+        <v>40.245421805381703</v>
+      </c>
+      <c r="AL24" s="10"/>
+      <c r="AM24" s="1">
+        <v>1.96451795272878E-5</v>
+      </c>
+      <c r="AN24" s="1">
+        <v>3.44599017898872E-5</v>
+      </c>
+      <c r="AO24" s="1">
+        <v>0.98993653059005704</v>
+      </c>
+      <c r="AP24" s="1">
+        <v>0.98928765535354601</v>
+      </c>
+      <c r="AQ24" s="1">
+        <v>48.063103942871003</v>
+      </c>
+      <c r="AR24" s="1">
+        <v>46.935824155807403</v>
+      </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>50</v>
       </c>
@@ -5723,8 +5982,24 @@
       <c r="AC25" s="2">
         <v>47.531822700500399</v>
       </c>
+      <c r="AE25" s="10">
+        <v>50</v>
+      </c>
+      <c r="AF25" s="15"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="10"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="1"/>
+      <c r="AR25" s="2"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>75</v>
       </c>
@@ -5809,8 +6084,24 @@
       <c r="AC26" s="2">
         <v>47.947384366989098</v>
       </c>
+      <c r="AE26" s="10">
+        <v>75</v>
+      </c>
+      <c r="AF26" s="15"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="10"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="1"/>
+      <c r="AR26" s="2"/>
     </row>
-    <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>100</v>
       </c>
@@ -5895,13 +6186,70 @@
       <c r="AC27" s="5">
         <v>47.923927621841401</v>
       </c>
+      <c r="AE27" s="11">
+        <v>100</v>
+      </c>
+      <c r="AF27" s="4">
+        <v>1.1494653263071E-4</v>
+      </c>
+      <c r="AG27" s="4">
+        <v>1.19207823468059E-4</v>
+      </c>
+      <c r="AH27" s="4">
+        <v>0.97659329891204805</v>
+      </c>
+      <c r="AI27" s="4">
+        <v>0.97592657163739205</v>
+      </c>
+      <c r="AJ27" s="4">
+        <v>40.558626155853197</v>
+      </c>
+      <c r="AK27" s="4">
+        <v>40.413001308441103</v>
+      </c>
+      <c r="AL27" s="11">
+        <v>35</v>
+      </c>
+      <c r="AM27" s="4">
+        <v>2.2430267690651801E-5</v>
+      </c>
+      <c r="AN27" s="4">
+        <v>2.4613124170400598E-5</v>
+      </c>
+      <c r="AO27" s="4">
+        <v>0.99106957435607901</v>
+      </c>
+      <c r="AP27" s="4">
+        <v>0.990855070054531</v>
+      </c>
+      <c r="AQ27" s="4">
+        <v>48.292446060180602</v>
+      </c>
+      <c r="AR27" s="5">
+        <v>48.0941442966461</v>
+      </c>
     </row>
-    <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="20"/>
       <c r="I28" s="21"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="N29" s="38"/>
       <c r="P29" s="19">
         <v>200</v>
       </c>
@@ -5919,17 +6267,124 @@
       <c r="AB29" s="17"/>
       <c r="AC29" s="18"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
+      <c r="I30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J31" s="20"/>
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="H31" s="15">
+        <v>25</v>
+      </c>
+      <c r="I31" s="1">
+        <v>2.2106023534433901E-5</v>
+      </c>
+      <c r="J31" s="1">
+        <v>3.6122786232226599E-5</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.98946617603302001</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0.98890163213014604</v>
+      </c>
+      <c r="M31" s="1">
+        <v>47.651081085205</v>
+      </c>
+      <c r="N31" s="2">
+        <v>47.000839977264398</v>
+      </c>
       <c r="W31" s="21"/>
       <c r="X31" s="21"/>
       <c r="Y31" s="20"/>
     </row>
-    <row r="38" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="H32" s="15">
+        <v>50</v>
+      </c>
+      <c r="I32" s="1">
+        <v>2.4145017250702901E-5</v>
+      </c>
+      <c r="J32" s="1">
+        <v>2.88026475823244E-5</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0.98924799889326098</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0.98952884152531595</v>
+      </c>
+      <c r="M32" s="1">
+        <v>48.197978820800699</v>
+      </c>
+      <c r="N32" s="2">
+        <v>47.531822700500399</v>
+      </c>
+    </row>
+    <row r="33" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H33" s="15">
+        <v>75</v>
+      </c>
+      <c r="I33" s="1">
+        <v>2.4419693569749699E-5</v>
+      </c>
+      <c r="J33" s="1">
+        <v>2.5516810550243401E-5</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.99079420646031702</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0.99062829300761202</v>
+      </c>
+      <c r="M33" s="1">
+        <v>48.232836761474601</v>
+      </c>
+      <c r="N33" s="2">
+        <v>47.947384366989098</v>
+      </c>
+    </row>
+    <row r="34" spans="8:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H34" s="3">
+        <v>100</v>
+      </c>
+      <c r="I34" s="22">
+        <v>2.4371969143430699E-5</v>
+      </c>
+      <c r="J34" s="4">
+        <v>2.62564474564896E-5</v>
+      </c>
+      <c r="K34" s="4">
+        <v>0.990291525125503</v>
+      </c>
+      <c r="L34" s="4">
+        <v>0.98999376922845805</v>
+      </c>
+      <c r="M34" s="4">
+        <v>48.127189064025799</v>
+      </c>
+      <c r="N34" s="5">
+        <v>47.923927621841401</v>
+      </c>
+    </row>
+    <row r="38" spans="8:14" x14ac:dyDescent="0.25">
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -5937,7 +6392,19 @@
       <c r="M38" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="52">
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="AG20:AK21"/>
+    <mergeCell ref="AL20:AL23"/>
+    <mergeCell ref="AM20:AR21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AO22:AP22"/>
+    <mergeCell ref="AQ22:AR22"/>
     <mergeCell ref="C20:G21"/>
     <mergeCell ref="H20:H23"/>
     <mergeCell ref="I20:N21"/>
@@ -5980,7 +6447,7 @@
     <mergeCell ref="AB22:AC22"/>
   </mergeCells>
   <conditionalFormatting sqref="B4">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5990,7 +6457,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="66">
+    <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6000,7 +6467,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="colorScale" priority="65">
+    <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6010,7 +6477,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="colorScale" priority="69">
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6020,7 +6487,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="71">
+    <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6030,7 +6497,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="colorScale" priority="73">
+    <cfRule type="colorScale" priority="98">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6040,7 +6507,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ7">
-    <cfRule type="colorScale" priority="60">
+    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6050,7 +6517,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ7">
-    <cfRule type="colorScale" priority="59">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6060,7 +6527,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ2:AQ6">
-    <cfRule type="colorScale" priority="74">
+    <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6070,7 +6537,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR2:AR7">
-    <cfRule type="colorScale" priority="57">
+    <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6080,7 +6547,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR2:AR6">
-    <cfRule type="colorScale" priority="75">
+    <cfRule type="colorScale" priority="100">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6090,6 +6557,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS2:AS7">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS2:AS6">
+    <cfRule type="colorScale" priority="101">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K38">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M38">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -6099,8 +6606,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS2:AS6">
-    <cfRule type="colorScale" priority="76">
+  <conditionalFormatting sqref="J38">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6109,8 +6636,88 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I38">
-    <cfRule type="colorScale" priority="28">
+  <conditionalFormatting sqref="B7 B4">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4 D7">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7 F4">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B5 B7:B8">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D5 D7:D8">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F5 F7:F8">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I8">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:K8">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C5 C7:C8">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6119,27 +6726,67 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K38">
+  <conditionalFormatting sqref="E3:E5 E10 E7:E8">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G5 G7:G8">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X24 X27">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y24 Y27">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y25">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M38">
+  <conditionalFormatting sqref="X25">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J38">
+  <conditionalFormatting sqref="X24:X25 X27">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -6149,7 +6796,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
+  <conditionalFormatting sqref="Y24:Y25 Y27">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X24:X27">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y24:Y27">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -6159,8 +6826,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="colorScale" priority="27">
+  <conditionalFormatting sqref="AN25">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6169,27 +6836,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="colorScale" priority="24">
+  <conditionalFormatting sqref="AM25">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6 B4">
+  <conditionalFormatting sqref="AM25">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -6199,17 +6856,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6 F4">
+  <conditionalFormatting sqref="AN25">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:B7 B4">
+  <conditionalFormatting sqref="AM25:AM26">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -6219,18 +6876,108 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D7 D4">
+  <conditionalFormatting sqref="AN25:AN26">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F7 F4">
+  <conditionalFormatting sqref="I34 I31">
     <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J34 J31">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31:I32 I34">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:J32 J34">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31:I34">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:J34">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:G6">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6240,96 +6987,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F8">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I8">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:K8">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C8">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E8">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G8">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X27 X24">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y27 Y24">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -6339,63 +6996,53 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y25">
+  <conditionalFormatting sqref="C3:C8">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X25">
+  <conditionalFormatting sqref="D3:D8">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X24:X25 X27">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y24:Y25 Y27">
+  <conditionalFormatting sqref="E3:E8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X24:X27">
+  <conditionalFormatting sqref="F3:F8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y24:Y27">
+  <conditionalFormatting sqref="G3:G8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
         <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added AOmap only model to the report
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A33BF0F-D540-49F7-842A-E6D11F43173B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644520A2-303A-4E89-BDB4-DFC1676F0DE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="17">
   <si>
     <t>Base Model</t>
   </si>
@@ -74,6 +74,9 @@
   <si>
     <t>epochs</t>
   </si>
+  <si>
+    <t>AO</t>
+  </si>
 </sst>
 </file>
 
@@ -102,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -240,52 +243,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -377,49 +334,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -431,18 +387,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,8 +714,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X17" zoomScale="126" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X33" sqref="X33"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,24 +750,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="28"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
+      <c r="A2" s="23"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -834,7 +788,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
@@ -869,16 +823,30 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
+      <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.3573738978011498E-5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.4275845818901801E-5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.98659012150764402</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.98670446947216905</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44.956761108398403</v>
+      </c>
+      <c r="G4" s="2">
+        <v>44.840311155319199</v>
+      </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1">
@@ -913,10 +881,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>2.9113601158314799E-5</v>
       </c>
       <c r="C6" s="1">
@@ -931,7 +899,7 @@
       <c r="F6" s="1">
         <v>46.891133316039998</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>47.021878166198697</v>
       </c>
       <c r="I6">
@@ -948,7 +916,7 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1">
@@ -983,25 +951,25 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>3.00520737182523E-5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>3.0312605779272401E-5</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>0.98983309078216497</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>0.98994339212775195</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>46.703372482299798</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="5">
         <v>46.899707784652698</v>
       </c>
       <c r="I8">
@@ -1018,49 +986,49 @@
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="25"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="35" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="31"/>
-      <c r="P11" s="13" t="s">
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="28"/>
+      <c r="P11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="29"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="35" t="s">
+      <c r="R11" s="26"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="30"/>
-      <c r="AA11" s="30"/>
-      <c r="AB11" s="30"/>
-      <c r="AC11" s="31"/>
+      <c r="X11" s="26"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="27"/>
+      <c r="AB11" s="27"/>
+      <c r="AC11" s="28"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1069,93 +1037,93 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="34"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="31"/>
       <c r="P12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
       </c>
-      <c r="R12" s="32"/>
-      <c r="S12" s="33"/>
-      <c r="T12" s="33"/>
-      <c r="U12" s="33"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="36"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="33"/>
-      <c r="Z12" s="33"/>
-      <c r="AA12" s="33"/>
-      <c r="AB12" s="33"/>
-      <c r="AC12" s="34"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="34"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="30"/>
+      <c r="AA12" s="30"/>
+      <c r="AB12" s="30"/>
+      <c r="AC12" s="31"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="38" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27" t="s">
+      <c r="C13" s="25"/>
+      <c r="D13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27" t="s">
+      <c r="E13" s="25"/>
+      <c r="F13" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="26" t="s">
+      <c r="G13" s="25"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27" t="s">
+      <c r="J13" s="25"/>
+      <c r="K13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27" t="s">
+      <c r="L13" s="25"/>
+      <c r="M13" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="28"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="38" t="s">
+      <c r="N13" s="32"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27" t="s">
+      <c r="R13" s="25"/>
+      <c r="S13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27" t="s">
+      <c r="T13" s="25"/>
+      <c r="U13" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="V13" s="27"/>
-      <c r="W13" s="36"/>
-      <c r="X13" s="26" t="s">
+      <c r="V13" s="25"/>
+      <c r="W13" s="34"/>
+      <c r="X13" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="Y13" s="27"/>
-      <c r="Z13" s="27" t="s">
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27" t="s">
+      <c r="AA13" s="25"/>
+      <c r="AB13" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="28"/>
+      <c r="AC13" s="32"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1176,7 +1144,7 @@
       <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="37"/>
+      <c r="H14" s="23"/>
       <c r="I14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1195,7 +1163,7 @@
       <c r="N14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P14" s="12" t="s">
+      <c r="P14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="Q14" s="4" t="s">
@@ -1216,7 +1184,7 @@
       <c r="V14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W14" s="37"/>
+      <c r="W14" s="23"/>
       <c r="X14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1237,7 +1205,7 @@
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="6">
         <v>25</v>
       </c>
       <c r="B15" s="1"/>
@@ -1246,14 +1214,14 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="10"/>
+      <c r="H15" s="6"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="2"/>
-      <c r="P15" s="10">
+      <c r="P15" s="6">
         <v>25</v>
       </c>
       <c r="Q15" s="1">
@@ -1274,7 +1242,7 @@
       <c r="V15" s="1">
         <v>46.643888940811102</v>
       </c>
-      <c r="W15" s="10">
+      <c r="W15" s="6">
         <v>20</v>
       </c>
       <c r="X15" s="1">
@@ -1297,7 +1265,7 @@
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="A16" s="6">
         <v>50</v>
       </c>
       <c r="B16" s="1"/>
@@ -1306,14 +1274,14 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="10"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="2"/>
-      <c r="P16" s="10">
+      <c r="P16" s="6">
         <v>50</v>
       </c>
       <c r="Q16" s="1">
@@ -1334,7 +1302,7 @@
       <c r="V16" s="1">
         <v>46.457026739120401</v>
       </c>
-      <c r="W16" s="10">
+      <c r="W16" s="6">
         <v>10</v>
       </c>
       <c r="X16" s="1">
@@ -1357,7 +1325,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="6">
         <v>75</v>
       </c>
       <c r="B17" s="1"/>
@@ -1366,14 +1334,14 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="10"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="2"/>
-      <c r="P17" s="10">
+      <c r="P17" s="6">
         <v>75</v>
       </c>
       <c r="Q17" s="1">
@@ -1394,7 +1362,7 @@
       <c r="V17" s="1">
         <v>46.688427810668898</v>
       </c>
-      <c r="W17" s="10">
+      <c r="W17" s="6">
         <v>25</v>
       </c>
       <c r="X17" s="1">
@@ -1417,7 +1385,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
+      <c r="A18" s="7">
         <v>100</v>
       </c>
       <c r="B18" s="4"/>
@@ -1426,14 +1394,14 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="11"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="5"/>
-      <c r="P18" s="11">
+      <c r="P18" s="7">
         <v>100</v>
       </c>
       <c r="Q18" s="4">
@@ -1454,7 +1422,7 @@
       <c r="V18" s="4">
         <v>46.690697641372601</v>
       </c>
-      <c r="W18" s="11">
+      <c r="W18" s="7">
         <v>25</v>
       </c>
       <c r="X18" s="4">
@@ -1478,205 +1446,205 @@
     </row>
     <row r="19" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="35" t="s">
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="31"/>
-      <c r="P20" s="13" t="s">
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="28"/>
+      <c r="P20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Q20" s="14" t="s">
+      <c r="Q20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R20" s="29"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="35" t="s">
+      <c r="R20" s="26"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="X20" s="29"/>
-      <c r="Y20" s="30"/>
-      <c r="Z20" s="30"/>
-      <c r="AA20" s="30"/>
-      <c r="AB20" s="30"/>
-      <c r="AC20" s="31"/>
-      <c r="AE20" s="13" t="s">
+      <c r="X20" s="26"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="27"/>
+      <c r="AB20" s="27"/>
+      <c r="AC20" s="28"/>
+      <c r="AE20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AF20" s="14" t="s">
+      <c r="AF20" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AG20" s="29"/>
-      <c r="AH20" s="30"/>
-      <c r="AI20" s="30"/>
-      <c r="AJ20" s="30"/>
-      <c r="AK20" s="31"/>
-      <c r="AL20" s="35" t="s">
+      <c r="AG20" s="26"/>
+      <c r="AH20" s="27"/>
+      <c r="AI20" s="27"/>
+      <c r="AJ20" s="27"/>
+      <c r="AK20" s="28"/>
+      <c r="AL20" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="AM20" s="29"/>
-      <c r="AN20" s="30"/>
-      <c r="AO20" s="30"/>
-      <c r="AP20" s="30"/>
-      <c r="AQ20" s="30"/>
-      <c r="AR20" s="31"/>
+      <c r="AM20" s="26"/>
+      <c r="AN20" s="27"/>
+      <c r="AO20" s="27"/>
+      <c r="AP20" s="27"/>
+      <c r="AQ20" s="27"/>
+      <c r="AR20" s="28"/>
     </row>
     <row r="21" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="7">
         <v>5</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="34"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="31"/>
       <c r="P21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q21" s="5">
         <v>5</v>
       </c>
-      <c r="R21" s="32"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="33"/>
-      <c r="V21" s="34"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="32"/>
-      <c r="Y21" s="33"/>
-      <c r="Z21" s="33"/>
-      <c r="AA21" s="33"/>
-      <c r="AB21" s="33"/>
-      <c r="AC21" s="34"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="29"/>
+      <c r="Y21" s="30"/>
+      <c r="Z21" s="30"/>
+      <c r="AA21" s="30"/>
+      <c r="AB21" s="30"/>
+      <c r="AC21" s="31"/>
       <c r="AE21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AF21" s="5">
         <v>5</v>
       </c>
-      <c r="AG21" s="32"/>
-      <c r="AH21" s="33"/>
-      <c r="AI21" s="33"/>
-      <c r="AJ21" s="33"/>
-      <c r="AK21" s="34"/>
-      <c r="AL21" s="36"/>
-      <c r="AM21" s="32"/>
-      <c r="AN21" s="33"/>
-      <c r="AO21" s="33"/>
-      <c r="AP21" s="33"/>
-      <c r="AQ21" s="33"/>
-      <c r="AR21" s="34"/>
+      <c r="AG21" s="29"/>
+      <c r="AH21" s="30"/>
+      <c r="AI21" s="30"/>
+      <c r="AJ21" s="30"/>
+      <c r="AK21" s="31"/>
+      <c r="AL21" s="34"/>
+      <c r="AM21" s="29"/>
+      <c r="AN21" s="30"/>
+      <c r="AO21" s="30"/>
+      <c r="AP21" s="30"/>
+      <c r="AQ21" s="30"/>
+      <c r="AR21" s="31"/>
     </row>
     <row r="22" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="38" t="s">
+      <c r="A22" s="11"/>
+      <c r="B22" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27" t="s">
+      <c r="C22" s="25"/>
+      <c r="D22" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27" t="s">
+      <c r="E22" s="25"/>
+      <c r="F22" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="26" t="s">
+      <c r="G22" s="25"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27" t="s">
+      <c r="J22" s="25"/>
+      <c r="K22" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27" t="s">
+      <c r="L22" s="25"/>
+      <c r="M22" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="28"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="38" t="s">
+      <c r="N22" s="32"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27" t="s">
+      <c r="R22" s="25"/>
+      <c r="S22" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27" t="s">
+      <c r="T22" s="25"/>
+      <c r="U22" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="V22" s="27"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="26" t="s">
+      <c r="V22" s="25"/>
+      <c r="W22" s="34"/>
+      <c r="X22" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="27"/>
-      <c r="Z22" s="27" t="s">
+      <c r="Y22" s="25"/>
+      <c r="Z22" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AA22" s="27"/>
-      <c r="AB22" s="27" t="s">
+      <c r="AA22" s="25"/>
+      <c r="AB22" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AC22" s="28"/>
-      <c r="AE22" s="15"/>
-      <c r="AF22" s="38" t="s">
+      <c r="AC22" s="32"/>
+      <c r="AE22" s="11"/>
+      <c r="AF22" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AG22" s="27"/>
-      <c r="AH22" s="27" t="s">
+      <c r="AG22" s="25"/>
+      <c r="AH22" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AI22" s="27"/>
-      <c r="AJ22" s="27" t="s">
+      <c r="AI22" s="25"/>
+      <c r="AJ22" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AK22" s="27"/>
-      <c r="AL22" s="36"/>
-      <c r="AM22" s="26" t="s">
+      <c r="AK22" s="25"/>
+      <c r="AL22" s="34"/>
+      <c r="AM22" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AN22" s="27"/>
-      <c r="AO22" s="27" t="s">
+      <c r="AN22" s="25"/>
+      <c r="AO22" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AP22" s="27"/>
-      <c r="AQ22" s="27" t="s">
+      <c r="AP22" s="25"/>
+      <c r="AQ22" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AR22" s="28"/>
+      <c r="AR22" s="32"/>
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1697,7 +1665,7 @@
       <c r="G23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="37"/>
+      <c r="H23" s="23"/>
       <c r="I23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1716,7 +1684,7 @@
       <c r="N23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P23" s="12" t="s">
+      <c r="P23" s="8" t="s">
         <v>14</v>
       </c>
       <c r="Q23" s="4" t="s">
@@ -1737,7 +1705,7 @@
       <c r="V23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W23" s="37"/>
+      <c r="W23" s="23"/>
       <c r="X23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1756,7 +1724,7 @@
       <c r="AC23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AE23" s="12" t="s">
+      <c r="AE23" s="8" t="s">
         <v>14</v>
       </c>
       <c r="AF23" s="4" t="s">
@@ -1777,7 +1745,7 @@
       <c r="AK23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AL23" s="37"/>
+      <c r="AL23" s="23"/>
       <c r="AM23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1798,10 +1766,10 @@
       </c>
     </row>
     <row r="24" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="A24" s="11">
         <v>25</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="11">
         <v>1.19287510897265E-4</v>
       </c>
       <c r="C24" s="1">
@@ -1819,31 +1787,31 @@
       <c r="G24" s="1">
         <v>39.089947509765601</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="6">
         <v>60</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="9">
         <v>2.7744608341890799E-5</v>
       </c>
-      <c r="J24" s="24">
+      <c r="J24" s="20">
         <v>4.22422099313735E-5</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="20">
         <v>0.98809633493423399</v>
       </c>
-      <c r="L24" s="24">
+      <c r="L24" s="20">
         <v>0.98773940578103003</v>
       </c>
-      <c r="M24" s="24">
+      <c r="M24" s="20">
         <v>46.455945434570303</v>
       </c>
-      <c r="N24" s="14">
+      <c r="N24" s="10">
         <v>45.520264139175403</v>
       </c>
-      <c r="P24" s="10">
+      <c r="P24" s="6">
         <v>25</v>
       </c>
-      <c r="Q24" s="15">
+      <c r="Q24" s="11">
         <v>1.0335394195863E-4</v>
       </c>
       <c r="R24" s="1">
@@ -1861,10 +1829,10 @@
       <c r="V24" s="1">
         <v>39.996493787765502</v>
       </c>
-      <c r="W24" s="10">
+      <c r="W24" s="6">
         <v>30</v>
       </c>
-      <c r="X24" s="15">
+      <c r="X24" s="11">
         <v>2.2106023534433901E-5</v>
       </c>
       <c r="Y24" s="1">
@@ -1882,7 +1850,7 @@
       <c r="AC24" s="2">
         <v>47.000839977264398</v>
       </c>
-      <c r="AE24" s="10">
+      <c r="AE24" s="6">
         <v>25</v>
       </c>
       <c r="AF24" s="1">
@@ -1903,7 +1871,7 @@
       <c r="AK24" s="1">
         <v>40.245421805381703</v>
       </c>
-      <c r="AL24" s="10"/>
+      <c r="AL24" s="6"/>
       <c r="AM24" s="1">
         <v>1.96451795272878E-5</v>
       </c>
@@ -1924,10 +1892,10 @@
       </c>
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="A25" s="11">
         <v>50</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="11">
         <v>1.4365710536367199E-4</v>
       </c>
       <c r="C25" s="1">
@@ -1945,10 +1913,10 @@
       <c r="G25" s="1">
         <v>39.538470983505199</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="6">
         <v>55</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="11">
         <v>2.8793881119781799E-5</v>
       </c>
       <c r="J25" s="1">
@@ -1966,10 +1934,10 @@
       <c r="N25" s="2">
         <v>46.554669828414902</v>
       </c>
-      <c r="P25" s="10">
+      <c r="P25" s="6">
         <v>50</v>
       </c>
-      <c r="Q25" s="15">
+      <c r="Q25" s="11">
         <v>1.2837137142923799E-4</v>
       </c>
       <c r="R25" s="1">
@@ -1987,10 +1955,10 @@
       <c r="V25" s="1">
         <v>40.475180215835501</v>
       </c>
-      <c r="W25" s="10">
+      <c r="W25" s="6">
         <v>35</v>
       </c>
-      <c r="X25" s="15">
+      <c r="X25" s="11">
         <v>2.4145017250702901E-5</v>
       </c>
       <c r="Y25" s="1">
@@ -2008,16 +1976,16 @@
       <c r="AC25" s="2">
         <v>47.531822700500399</v>
       </c>
-      <c r="AE25" s="10">
+      <c r="AE25" s="6">
         <v>50</v>
       </c>
-      <c r="AF25" s="15"/>
+      <c r="AF25" s="11"/>
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
-      <c r="AL25" s="10"/>
+      <c r="AL25" s="6"/>
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
@@ -2026,10 +1994,10 @@
       <c r="AR25" s="2"/>
     </row>
     <row r="26" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="A26" s="11">
         <v>75</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="11">
         <v>1.39489508728729E-4</v>
       </c>
       <c r="C26" s="1">
@@ -2047,10 +2015,10 @@
       <c r="G26" s="1">
         <v>39.292952666282602</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="6">
         <v>55</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="11">
         <v>2.8770537234474102E-5</v>
       </c>
       <c r="J26" s="1">
@@ -2068,10 +2036,10 @@
       <c r="N26" s="2">
         <v>46.846222772598203</v>
       </c>
-      <c r="P26" s="10">
+      <c r="P26" s="6">
         <v>75</v>
       </c>
-      <c r="Q26" s="15">
+      <c r="Q26" s="11">
         <v>1.2182683548113901E-4</v>
       </c>
       <c r="R26" s="1">
@@ -2089,10 +2057,10 @@
       <c r="V26" s="1">
         <v>40.215824222564699</v>
       </c>
-      <c r="W26" s="10">
+      <c r="W26" s="6">
         <v>25</v>
       </c>
-      <c r="X26" s="15">
+      <c r="X26" s="11">
         <v>2.4419693569749699E-5</v>
       </c>
       <c r="Y26" s="1">
@@ -2110,16 +2078,16 @@
       <c r="AC26" s="2">
         <v>47.947384366989098</v>
       </c>
-      <c r="AE26" s="10">
+      <c r="AE26" s="6">
         <v>75</v>
       </c>
-      <c r="AF26" s="15"/>
+      <c r="AF26" s="11"/>
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
-      <c r="AL26" s="10"/>
+      <c r="AL26" s="6"/>
       <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
       <c r="AO26" s="1"/>
@@ -2149,7 +2117,7 @@
       <c r="G27" s="4">
         <v>39.269116249084398</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="7">
         <v>55</v>
       </c>
       <c r="I27" s="3">
@@ -2170,7 +2138,7 @@
       <c r="N27" s="5">
         <v>46.9667868614196</v>
       </c>
-      <c r="P27" s="11">
+      <c r="P27" s="7">
         <v>100</v>
       </c>
       <c r="Q27" s="3">
@@ -2191,7 +2159,7 @@
       <c r="V27" s="4">
         <v>40.189842977523803</v>
       </c>
-      <c r="W27" s="11">
+      <c r="W27" s="7">
         <v>35</v>
       </c>
       <c r="X27" s="3">
@@ -2212,7 +2180,7 @@
       <c r="AC27" s="5">
         <v>48.0322548866272</v>
       </c>
-      <c r="AE27" s="11">
+      <c r="AE27" s="7">
         <v>100</v>
       </c>
       <c r="AF27" s="4">
@@ -2233,7 +2201,7 @@
       <c r="AK27" s="4">
         <v>40.413001308441103</v>
       </c>
-      <c r="AL27" s="11">
+      <c r="AL27" s="7">
         <v>35</v>
       </c>
       <c r="AM27" s="4">
@@ -2256,46 +2224,46 @@
       </c>
     </row>
     <row r="28" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="19"/>
-      <c r="I28" s="20"/>
-      <c r="K28" s="19"/>
+      <c r="C28" s="15"/>
+      <c r="I28" s="16"/>
+      <c r="K28" s="15"/>
     </row>
     <row r="29" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G29" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="26" t="s">
+      <c r="I29" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27" t="s">
+      <c r="J29" s="25"/>
+      <c r="K29" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27" t="s">
+      <c r="L29" s="25"/>
+      <c r="M29" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="28"/>
-      <c r="P29" s="18">
+      <c r="N29" s="32"/>
+      <c r="P29" s="14">
         <v>200</v>
       </c>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="18"/>
-      <c r="X29" s="16"/>
-      <c r="Y29" s="16"/>
-      <c r="Z29" s="16"/>
-      <c r="AA29" s="16"/>
-      <c r="AB29" s="16"/>
-      <c r="AC29" s="17"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="14"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="13"/>
     </row>
     <row r="30" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
       <c r="I30" s="3" t="s">
         <v>7</v>
       </c>
@@ -2316,7 +2284,7 @@
       </c>
     </row>
     <row r="31" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="H31" s="15">
+      <c r="H31" s="11">
         <v>25</v>
       </c>
       <c r="I31" s="1">
@@ -2337,12 +2305,12 @@
       <c r="N31" s="2">
         <v>47.000839977264398</v>
       </c>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
-      <c r="Y31" s="19"/>
+      <c r="W31" s="16"/>
+      <c r="X31" s="16"/>
+      <c r="Y31" s="15"/>
     </row>
     <row r="32" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="H32" s="15">
+      <c r="H32" s="11">
         <v>50</v>
       </c>
       <c r="I32" s="1">
@@ -2365,7 +2333,7 @@
       </c>
     </row>
     <row r="33" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H33" s="15">
+      <c r="H33" s="11">
         <v>75</v>
       </c>
       <c r="I33" s="1">
@@ -2391,7 +2359,7 @@
       <c r="H34" s="3">
         <v>100</v>
       </c>
-      <c r="I34" s="21">
+      <c r="I34" s="17">
         <v>2.4371969143430699E-5</v>
       </c>
       <c r="J34" s="4">
@@ -2419,12 +2387,36 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="R11:V12"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="AG20:AK21"/>
+    <mergeCell ref="AL20:AL23"/>
+    <mergeCell ref="R20:V21"/>
+    <mergeCell ref="W20:W23"/>
+    <mergeCell ref="X20:AC21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="AM20:AR21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AO22:AP22"/>
+    <mergeCell ref="AQ22:AR22"/>
+    <mergeCell ref="C20:G21"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:N21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
@@ -2441,99 +2433,15 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="C20:G21"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:N21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="AM20:AR21"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="AO22:AP22"/>
-    <mergeCell ref="AQ22:AR22"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="AG20:AK21"/>
-    <mergeCell ref="AL20:AL23"/>
-    <mergeCell ref="R20:V21"/>
-    <mergeCell ref="W20:W23"/>
-    <mergeCell ref="X20:AC21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="R11:V12"/>
+    <mergeCell ref="M13:N13"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4">
-    <cfRule type="colorScale" priority="114">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="112">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
-    <cfRule type="colorScale" priority="111">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
-    <cfRule type="colorScale" priority="115">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="colorScale" priority="117">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
-    <cfRule type="colorScale" priority="119">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="colorScale" priority="74">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2543,7 +2451,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38">
-    <cfRule type="colorScale" priority="77">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2553,7 +2461,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M38">
-    <cfRule type="colorScale" priority="76">
+    <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2563,26 +2471,76 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38">
-    <cfRule type="colorScale" priority="75">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4">
+    <cfRule type="colorScale" priority="82">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3 B7 B5">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3 D7 D5">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3 F7 F5">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I8">
     <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
@@ -2592,108 +2550,318 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4 B7">
+  <conditionalFormatting sqref="J3:K8">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7 D4">
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7 C3 C5">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7 F4">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3 E10 E7 E5">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B5 B7">
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3 G7 G5">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D5 D7">
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X24">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F5 F7">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y24">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I8">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y25">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:K8">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X25">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C5 C7">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X24:X25">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y24:Y25">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X24:X26">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y24:Y26">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN25">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM25">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM25">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN25">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM25:AM26">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN25:AN26">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34 I31">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J34 J31">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J32">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31:I32 I34">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:J32 J34">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31:I34">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31:J34">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E5 E10 E7">
-    <cfRule type="colorScale" priority="56">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
+  <conditionalFormatting sqref="D6:G6">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B7 B3">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C7 C3">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G5 G7">
-    <cfRule type="colorScale" priority="55">
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D7 D3">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E7 E3">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2702,267 +2870,47 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X24">
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y24">
-    <cfRule type="colorScale" priority="53">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y25">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X25">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X24:X25">
-    <cfRule type="colorScale" priority="50">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y24:Y25">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X24:X26">
-    <cfRule type="colorScale" priority="48">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y24:Y26">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN25">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM25">
-    <cfRule type="colorScale" priority="43">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM25">
-    <cfRule type="colorScale" priority="42">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN25">
-    <cfRule type="colorScale" priority="41">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM25:AM26">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN25:AN26">
-    <cfRule type="colorScale" priority="39">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I34 I31">
-    <cfRule type="colorScale" priority="38">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J34 J31">
-    <cfRule type="colorScale" priority="37">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J32">
-    <cfRule type="colorScale" priority="36">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31:I32 I34">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J31:J32 J34">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I31:I34">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J31:J34">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
+  <conditionalFormatting sqref="F5:F7 F3">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G7 G3">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6:G6">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B7">
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C7">
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D7">
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -2972,27 +2920,37 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E7">
+  <conditionalFormatting sqref="F8">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F7">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G7">
+  <conditionalFormatting sqref="E8">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3002,87 +2960,87 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
+  <conditionalFormatting sqref="D8">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E8 E3">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
+  <conditionalFormatting sqref="B8:C8">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:C8">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B8 B3">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C8 C3">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D8 D3">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -3092,8 +3050,58 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="F5:F8 F3">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G8 G3">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X24:X27">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y24:Y27">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G8">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F8">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3112,8 +3120,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:C8">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="D3:D8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C8">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3122,78 +3140,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:C8">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C8">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F8">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G8">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X24:X27">
     <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y24:Y27">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
report.xlsx was updated 200 sample NM-AO-2
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644520A2-303A-4E89-BDB4-DFC1676F0DE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA34008-2942-43A4-A601-5D61D3558753}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -357,16 +357,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -387,16 +385,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,8 +714,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="N7" zoomScale="126" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,24 +750,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="32"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -788,7 +788,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
@@ -1000,7 +1000,7 @@
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
       <c r="G11" s="28"/>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="26"/>
@@ -1020,7 +1020,7 @@
       <c r="T11" s="27"/>
       <c r="U11" s="27"/>
       <c r="V11" s="28"/>
-      <c r="W11" s="22" t="s">
+      <c r="W11" s="32" t="s">
         <v>15</v>
       </c>
       <c r="X11" s="26"/>
@@ -1042,7 +1042,7 @@
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="31"/>
-      <c r="H12" s="34"/>
+      <c r="H12" s="33"/>
       <c r="I12" s="29"/>
       <c r="J12" s="30"/>
       <c r="K12" s="30"/>
@@ -1060,7 +1060,7 @@
       <c r="T12" s="30"/>
       <c r="U12" s="30"/>
       <c r="V12" s="31"/>
-      <c r="W12" s="34"/>
+      <c r="W12" s="33"/>
       <c r="X12" s="29"/>
       <c r="Y12" s="30"/>
       <c r="Z12" s="30"/>
@@ -1070,57 +1070,57 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25" t="s">
+      <c r="C13" s="24"/>
+      <c r="D13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25" t="s">
+      <c r="E13" s="24"/>
+      <c r="F13" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="33" t="s">
+      <c r="G13" s="24"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25" t="s">
+      <c r="J13" s="24"/>
+      <c r="K13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25" t="s">
+      <c r="L13" s="24"/>
+      <c r="M13" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="32"/>
+      <c r="N13" s="25"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="24" t="s">
+      <c r="Q13" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25" t="s">
+      <c r="R13" s="24"/>
+      <c r="S13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25" t="s">
+      <c r="T13" s="24"/>
+      <c r="U13" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="V13" s="25"/>
-      <c r="W13" s="34"/>
-      <c r="X13" s="33" t="s">
+      <c r="V13" s="24"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25" t="s">
+      <c r="Y13" s="24"/>
+      <c r="Z13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="25" t="s">
+      <c r="AA13" s="24"/>
+      <c r="AB13" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="32"/>
+      <c r="AC13" s="25"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1144,7 +1144,7 @@
       <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="23"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1184,7 @@
       <c r="V14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W14" s="23"/>
+      <c r="W14" s="34"/>
       <c r="X14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1457,7 +1457,7 @@
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
       <c r="G20" s="28"/>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="32" t="s">
         <v>15</v>
       </c>
       <c r="I20" s="26"/>
@@ -1477,7 +1477,7 @@
       <c r="T20" s="27"/>
       <c r="U20" s="27"/>
       <c r="V20" s="28"/>
-      <c r="W20" s="22" t="s">
+      <c r="W20" s="32" t="s">
         <v>15</v>
       </c>
       <c r="X20" s="26"/>
@@ -1497,7 +1497,7 @@
       <c r="AI20" s="27"/>
       <c r="AJ20" s="27"/>
       <c r="AK20" s="28"/>
-      <c r="AL20" s="22" t="s">
+      <c r="AL20" s="32" t="s">
         <v>15</v>
       </c>
       <c r="AM20" s="26"/>
@@ -1519,7 +1519,7 @@
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
       <c r="G21" s="31"/>
-      <c r="H21" s="34"/>
+      <c r="H21" s="33"/>
       <c r="I21" s="29"/>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
@@ -1537,7 +1537,7 @@
       <c r="T21" s="30"/>
       <c r="U21" s="30"/>
       <c r="V21" s="31"/>
-      <c r="W21" s="34"/>
+      <c r="W21" s="33"/>
       <c r="X21" s="29"/>
       <c r="Y21" s="30"/>
       <c r="Z21" s="30"/>
@@ -1555,7 +1555,7 @@
       <c r="AI21" s="30"/>
       <c r="AJ21" s="30"/>
       <c r="AK21" s="31"/>
-      <c r="AL21" s="34"/>
+      <c r="AL21" s="33"/>
       <c r="AM21" s="29"/>
       <c r="AN21" s="30"/>
       <c r="AO21" s="30"/>
@@ -1565,83 +1565,83 @@
     </row>
     <row r="22" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25" t="s">
+      <c r="C22" s="24"/>
+      <c r="D22" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25" t="s">
+      <c r="E22" s="24"/>
+      <c r="F22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="25"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="33" t="s">
+      <c r="G22" s="24"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25" t="s">
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25" t="s">
+      <c r="L22" s="24"/>
+      <c r="M22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="32"/>
+      <c r="N22" s="25"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="24" t="s">
+      <c r="Q22" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25" t="s">
+      <c r="R22" s="24"/>
+      <c r="S22" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="25"/>
-      <c r="U22" s="25" t="s">
+      <c r="T22" s="24"/>
+      <c r="U22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="V22" s="25"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="33" t="s">
+      <c r="V22" s="24"/>
+      <c r="W22" s="33"/>
+      <c r="X22" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="25"/>
-      <c r="Z22" s="25" t="s">
+      <c r="Y22" s="24"/>
+      <c r="Z22" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AA22" s="25"/>
-      <c r="AB22" s="25" t="s">
+      <c r="AA22" s="24"/>
+      <c r="AB22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AC22" s="32"/>
+      <c r="AC22" s="25"/>
       <c r="AE22" s="11"/>
-      <c r="AF22" s="24" t="s">
+      <c r="AF22" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AG22" s="25"/>
-      <c r="AH22" s="25" t="s">
+      <c r="AG22" s="24"/>
+      <c r="AH22" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AI22" s="25"/>
-      <c r="AJ22" s="25" t="s">
+      <c r="AI22" s="24"/>
+      <c r="AJ22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AK22" s="25"/>
-      <c r="AL22" s="34"/>
-      <c r="AM22" s="33" t="s">
+      <c r="AK22" s="24"/>
+      <c r="AL22" s="33"/>
+      <c r="AM22" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="AN22" s="25"/>
-      <c r="AO22" s="25" t="s">
+      <c r="AN22" s="24"/>
+      <c r="AO22" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AP22" s="25"/>
-      <c r="AQ22" s="25" t="s">
+      <c r="AP22" s="24"/>
+      <c r="AQ22" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="AR22" s="32"/>
+      <c r="AR22" s="25"/>
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
@@ -1665,7 +1665,7 @@
       <c r="G23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="23"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1705,7 +1705,7 @@
       <c r="V23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W23" s="23"/>
+      <c r="W23" s="34"/>
       <c r="X23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1745,7 +1745,7 @@
       <c r="AK23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AL23" s="23"/>
+      <c r="AL23" s="34"/>
       <c r="AM23" s="3" t="s">
         <v>7</v>
       </c>
@@ -2232,34 +2232,60 @@
       <c r="G29" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="33" t="s">
+      <c r="I29" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25" t="s">
+      <c r="J29" s="24"/>
+      <c r="K29" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25" t="s">
+      <c r="L29" s="24"/>
+      <c r="M29" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="32"/>
+      <c r="N29" s="25"/>
       <c r="P29" s="14">
         <v>200</v>
       </c>
-      <c r="Q29" s="12"/>
-      <c r="R29" s="12"/>
-      <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
-      <c r="U29" s="12"/>
-      <c r="V29" s="12"/>
-      <c r="W29" s="14"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="12"/>
-      <c r="Z29" s="12"/>
-      <c r="AA29" s="12"/>
-      <c r="AB29" s="12"/>
-      <c r="AC29" s="13"/>
+      <c r="Q29" s="18">
+        <v>1.02994677297829E-4</v>
+      </c>
+      <c r="R29" s="12">
+        <v>1.26044154662849E-4</v>
+      </c>
+      <c r="S29" s="12">
+        <v>0.97093703746795601</v>
+      </c>
+      <c r="T29" s="12">
+        <v>0.97067702367901798</v>
+      </c>
+      <c r="U29" s="12">
+        <v>40.880678009033197</v>
+      </c>
+      <c r="V29" s="13">
+        <v>40.129889388084401</v>
+      </c>
+      <c r="W29" s="14">
+        <v>25</v>
+      </c>
+      <c r="X29" s="18">
+        <v>2.10001648902107E-5</v>
+      </c>
+      <c r="Y29" s="12">
+        <v>2.25852938717707E-5</v>
+      </c>
+      <c r="Z29" s="12">
+        <v>0.99081480550765899</v>
+      </c>
+      <c r="AA29" s="12">
+        <v>0.99073930859565695</v>
+      </c>
+      <c r="AB29" s="12">
+        <v>48.4266024627685</v>
+      </c>
+      <c r="AC29" s="13">
+        <v>48.509353599548298</v>
+      </c>
     </row>
     <row r="30" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="15"/>
@@ -2387,36 +2413,12 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="AG20:AK21"/>
-    <mergeCell ref="AL20:AL23"/>
-    <mergeCell ref="R20:V21"/>
-    <mergeCell ref="W20:W23"/>
-    <mergeCell ref="X20:AC21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="AM20:AR21"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="AO22:AP22"/>
-    <mergeCell ref="AQ22:AR22"/>
-    <mergeCell ref="C20:G21"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:N21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="R11:V12"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
@@ -2433,12 +2435,36 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="R11:V12"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="C20:G21"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:N21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="AM20:AR21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AO22:AP22"/>
+    <mergeCell ref="AQ22:AR22"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="AG20:AK21"/>
+    <mergeCell ref="AL20:AL23"/>
+    <mergeCell ref="R20:V21"/>
+    <mergeCell ref="W20:W23"/>
+    <mergeCell ref="X20:AC21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
   </mergeCells>
   <conditionalFormatting sqref="I38">
     <cfRule type="colorScale" priority="81">
@@ -2510,7 +2536,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3 B7 B5">
+  <conditionalFormatting sqref="B7 B3 B5">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -2520,7 +2546,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3 D7 D5">
+  <conditionalFormatting sqref="D7 D3 D5">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -2530,7 +2556,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3 F7 F5">
+  <conditionalFormatting sqref="F7 F3 F5">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
@@ -2560,7 +2586,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7 C3 C5">
+  <conditionalFormatting sqref="C3 C7 C5">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -2570,7 +2596,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3 E10 E7 E5">
+  <conditionalFormatting sqref="E10 E3 E7 E5">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -2580,7 +2606,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3 G7 G5">
+  <conditionalFormatting sqref="G7 G3 G5">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -2730,7 +2756,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I34 I31">
+  <conditionalFormatting sqref="I31 I34">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -2740,7 +2766,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34 J31">
+  <conditionalFormatting sqref="J31 J34">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
updated report.xlsx for base model and AO improvement
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6ABA73-D540-43A1-A1A5-EAE5EF1ED403}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B010219-3BC9-4EFA-82F3-3F749A4CF149}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -367,16 +367,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -397,13 +394,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -723,8 +723,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P11" zoomScale="139" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,24 +762,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="29"/>
+      <c r="F1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="38"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -804,38 +804,38 @@
         <v>0</v>
       </c>
       <c r="B3" s="24">
-        <v>4.4384981214534402E-5</v>
+        <v>4.1144312133837898E-5</v>
       </c>
       <c r="C3" s="24">
-        <v>4.3598451313755497E-5</v>
+        <v>4.0423539585390199E-5</v>
       </c>
       <c r="D3" s="24">
-        <v>0.98570186853408803</v>
+        <v>0.98695401430130003</v>
       </c>
       <c r="E3" s="24">
-        <v>0.98624380275607104</v>
+        <v>0.98747133150696698</v>
       </c>
       <c r="F3" s="24">
-        <v>44.889844085693298</v>
+        <v>45.2277616729736</v>
       </c>
       <c r="G3" s="25">
-        <v>45.043708372116001</v>
+        <v>45.398860187530502</v>
       </c>
       <c r="I3">
         <f>(MIN(B3:C3)/MAX(B3:C3))</f>
-        <v>0.98227936839767438</v>
+        <v>0.9824818422992927</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J8" si="0">(MIN(D3:E3)/MAX(D3:E3))</f>
-        <v>0.99945050684174785</v>
+        <v>0.99947611926629054</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K8" si="1">(MIN(F3:G3)/MAX(F3:G3))</f>
-        <v>0.99658411147786508</v>
+        <v>0.99623121563294448</v>
       </c>
       <c r="L3" s="23">
         <f>(1-E3/MAX(E$3:E$8))*100</f>
-        <v>0.44864156453230386</v>
+        <v>0.32473492569838891</v>
       </c>
       <c r="N3">
         <f>MIN(B3:C8)</f>
@@ -843,11 +843,11 @@
       </c>
       <c r="O3">
         <f>MIN(D3:E8)</f>
-        <v>0.98570186853408803</v>
+        <v>0.98695401430130003</v>
       </c>
       <c r="P3">
         <f>MIN(F3:G8)</f>
-        <v>44.840311155319199</v>
+        <v>45.2277616729736</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -855,42 +855,42 @@
         <v>16</v>
       </c>
       <c r="B4" s="24">
-        <v>4.3573738978011498E-5</v>
+        <v>4.04361183318542E-5</v>
       </c>
       <c r="C4" s="24">
-        <v>4.4275845818901801E-5</v>
+        <v>3.9570047426877803E-5</v>
       </c>
       <c r="D4" s="24">
-        <v>0.98659012150764402</v>
+        <v>0.98800736880302398</v>
       </c>
       <c r="E4" s="24">
-        <v>0.98670446947216905</v>
+        <v>0.98831831634044598</v>
       </c>
       <c r="F4" s="24">
-        <v>44.956761108398403</v>
+        <v>45.337396545410101</v>
       </c>
       <c r="G4" s="25">
-        <v>44.840311155319199</v>
+        <v>45.483137578964197</v>
       </c>
       <c r="I4">
         <f>(MIN(B4:C4)/MAX(B4:C4))</f>
-        <v>0.98414244091999781</v>
+        <v>0.97858174966576517</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0.99988411123283327</v>
+        <v>0.99968537713783001</v>
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>0.99740973437124569</v>
+        <v>0.99679571284410462</v>
       </c>
       <c r="L4" s="23">
         <f t="shared" ref="L4:L8" si="2">(1-E4/MAX(E$3:E$8))*100</f>
-        <v>0.40214190872164268</v>
+        <v>0.23924035477035366</v>
       </c>
       <c r="N4">
         <f>MAX(B3:C8)</f>
-        <v>4.4384981214534402E-5</v>
+        <v>4.1144312133837898E-5</v>
       </c>
       <c r="O4">
         <f>MAX(D3:E8)</f>
@@ -1067,40 +1067,40 @@
       <c r="B11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="28" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="32"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="34"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="33"/>
       <c r="P11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="32"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="34"/>
-      <c r="W11" s="28" t="s">
+      <c r="R11" s="31"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="33"/>
-      <c r="Z11" s="33"/>
-      <c r="AA11" s="33"/>
-      <c r="AB11" s="33"/>
-      <c r="AC11" s="34"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="32"/>
+      <c r="AA11" s="32"/>
+      <c r="AB11" s="32"/>
+      <c r="AC11" s="33"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1109,90 +1109,90 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="37"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="36"/>
       <c r="P12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
       </c>
-      <c r="R12" s="35"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="37"/>
-      <c r="W12" s="40"/>
-      <c r="X12" s="35"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="36"/>
-      <c r="AA12" s="36"/>
-      <c r="AB12" s="36"/>
-      <c r="AC12" s="37"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="34"/>
+      <c r="Y12" s="35"/>
+      <c r="Z12" s="35"/>
+      <c r="AA12" s="35"/>
+      <c r="AB12" s="35"/>
+      <c r="AC12" s="36"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31" t="s">
+      <c r="C13" s="29"/>
+      <c r="D13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31" t="s">
+      <c r="E13" s="29"/>
+      <c r="F13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="39" t="s">
+      <c r="G13" s="29"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31" t="s">
+      <c r="J13" s="29"/>
+      <c r="K13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31" t="s">
+      <c r="L13" s="29"/>
+      <c r="M13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="38"/>
+      <c r="N13" s="30"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="30" t="s">
+      <c r="Q13" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31" t="s">
+      <c r="R13" s="29"/>
+      <c r="S13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="31"/>
-      <c r="U13" s="31" t="s">
+      <c r="T13" s="29"/>
+      <c r="U13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="V13" s="31"/>
-      <c r="W13" s="40"/>
-      <c r="X13" s="39" t="s">
+      <c r="V13" s="29"/>
+      <c r="W13" s="38"/>
+      <c r="X13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="Y13" s="31"/>
-      <c r="Z13" s="31" t="s">
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="AA13" s="31"/>
-      <c r="AB13" s="31" t="s">
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="38"/>
+      <c r="AC13" s="30"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1216,7 +1216,7 @@
       <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="29"/>
+      <c r="H14" s="39"/>
       <c r="I14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1256,7 +1256,7 @@
       <c r="V14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W14" s="29"/>
+      <c r="W14" s="39"/>
       <c r="X14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1524,60 +1524,60 @@
       <c r="B20" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="28" t="s">
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="32"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="34"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="33"/>
       <c r="P20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R20" s="32"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="28" t="s">
+      <c r="R20" s="31"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="X20" s="32"/>
-      <c r="Y20" s="33"/>
-      <c r="Z20" s="33"/>
-      <c r="AA20" s="33"/>
-      <c r="AB20" s="33"/>
-      <c r="AC20" s="34"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="32"/>
+      <c r="AA20" s="32"/>
+      <c r="AB20" s="32"/>
+      <c r="AC20" s="33"/>
       <c r="AE20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="AF20" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AG20" s="32"/>
-      <c r="AH20" s="33"/>
-      <c r="AI20" s="33"/>
-      <c r="AJ20" s="33"/>
-      <c r="AK20" s="34"/>
-      <c r="AL20" s="28" t="s">
+      <c r="AG20" s="31"/>
+      <c r="AH20" s="32"/>
+      <c r="AI20" s="32"/>
+      <c r="AJ20" s="32"/>
+      <c r="AK20" s="33"/>
+      <c r="AL20" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="AM20" s="32"/>
-      <c r="AN20" s="33"/>
-      <c r="AO20" s="33"/>
-      <c r="AP20" s="33"/>
-      <c r="AQ20" s="33"/>
-      <c r="AR20" s="34"/>
+      <c r="AM20" s="31"/>
+      <c r="AN20" s="32"/>
+      <c r="AO20" s="32"/>
+      <c r="AP20" s="32"/>
+      <c r="AQ20" s="32"/>
+      <c r="AR20" s="33"/>
     </row>
     <row r="21" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1586,134 +1586,134 @@
       <c r="B21" s="7">
         <v>5</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="37"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="36"/>
       <c r="P21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q21" s="5">
         <v>5</v>
       </c>
-      <c r="R21" s="35"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="40"/>
-      <c r="X21" s="35"/>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="36"/>
-      <c r="AA21" s="36"/>
-      <c r="AB21" s="36"/>
-      <c r="AC21" s="37"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="38"/>
+      <c r="X21" s="34"/>
+      <c r="Y21" s="35"/>
+      <c r="Z21" s="35"/>
+      <c r="AA21" s="35"/>
+      <c r="AB21" s="35"/>
+      <c r="AC21" s="36"/>
       <c r="AE21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AF21" s="5">
         <v>5</v>
       </c>
-      <c r="AG21" s="35"/>
-      <c r="AH21" s="36"/>
-      <c r="AI21" s="36"/>
-      <c r="AJ21" s="36"/>
-      <c r="AK21" s="37"/>
-      <c r="AL21" s="40"/>
-      <c r="AM21" s="35"/>
-      <c r="AN21" s="36"/>
-      <c r="AO21" s="36"/>
-      <c r="AP21" s="36"/>
-      <c r="AQ21" s="36"/>
-      <c r="AR21" s="37"/>
+      <c r="AG21" s="34"/>
+      <c r="AH21" s="35"/>
+      <c r="AI21" s="35"/>
+      <c r="AJ21" s="35"/>
+      <c r="AK21" s="36"/>
+      <c r="AL21" s="38"/>
+      <c r="AM21" s="34"/>
+      <c r="AN21" s="35"/>
+      <c r="AO21" s="35"/>
+      <c r="AP21" s="35"/>
+      <c r="AQ21" s="35"/>
+      <c r="AR21" s="36"/>
     </row>
     <row r="22" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31" t="s">
+      <c r="C22" s="29"/>
+      <c r="D22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31" t="s">
+      <c r="E22" s="29"/>
+      <c r="F22" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="39" t="s">
+      <c r="G22" s="29"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31" t="s">
+      <c r="J22" s="29"/>
+      <c r="K22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31" t="s">
+      <c r="L22" s="29"/>
+      <c r="M22" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="38"/>
+      <c r="N22" s="30"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="30" t="s">
+      <c r="Q22" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31" t="s">
+      <c r="R22" s="29"/>
+      <c r="S22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31" t="s">
+      <c r="T22" s="29"/>
+      <c r="U22" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="V22" s="31"/>
-      <c r="W22" s="40"/>
-      <c r="X22" s="39" t="s">
+      <c r="V22" s="29"/>
+      <c r="W22" s="38"/>
+      <c r="X22" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="31"/>
-      <c r="Z22" s="31" t="s">
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="31" t="s">
+      <c r="AA22" s="29"/>
+      <c r="AB22" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="AC22" s="38"/>
+      <c r="AC22" s="30"/>
       <c r="AE22" s="11"/>
-      <c r="AF22" s="30" t="s">
+      <c r="AF22" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="AG22" s="31"/>
-      <c r="AH22" s="31" t="s">
+      <c r="AG22" s="29"/>
+      <c r="AH22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="AI22" s="31"/>
-      <c r="AJ22" s="31" t="s">
+      <c r="AI22" s="29"/>
+      <c r="AJ22" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="AK22" s="31"/>
-      <c r="AL22" s="40"/>
-      <c r="AM22" s="39" t="s">
+      <c r="AK22" s="29"/>
+      <c r="AL22" s="38"/>
+      <c r="AM22" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AN22" s="31"/>
-      <c r="AO22" s="31" t="s">
+      <c r="AN22" s="29"/>
+      <c r="AO22" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="AP22" s="31"/>
-      <c r="AQ22" s="31" t="s">
+      <c r="AP22" s="29"/>
+      <c r="AQ22" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="AR22" s="38"/>
+      <c r="AR22" s="30"/>
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
@@ -1737,7 +1737,7 @@
       <c r="G23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="29"/>
+      <c r="H23" s="39"/>
       <c r="I23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1777,7 +1777,7 @@
       <c r="V23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W23" s="29"/>
+      <c r="W23" s="39"/>
       <c r="X23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1817,7 +1817,7 @@
       <c r="AK23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AL23" s="29"/>
+      <c r="AL23" s="39"/>
       <c r="AM23" s="3" t="s">
         <v>7</v>
       </c>
@@ -2304,18 +2304,18 @@
       <c r="G29" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="39" t="s">
+      <c r="I29" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31" t="s">
+      <c r="J29" s="29"/>
+      <c r="K29" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31" t="s">
+      <c r="L29" s="29"/>
+      <c r="M29" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="38"/>
+      <c r="N29" s="30"/>
       <c r="P29" s="14">
         <v>200</v>
       </c>
@@ -2485,36 +2485,12 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="AG20:AK21"/>
-    <mergeCell ref="AL20:AL23"/>
-    <mergeCell ref="R20:V21"/>
-    <mergeCell ref="W20:W23"/>
-    <mergeCell ref="X20:AC21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="AM20:AR21"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="AO22:AP22"/>
-    <mergeCell ref="AQ22:AR22"/>
-    <mergeCell ref="C20:G21"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:N21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="R11:V12"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
@@ -2531,12 +2507,36 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="R11:V12"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="C20:G21"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:N21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="AM20:AR21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AO22:AP22"/>
+    <mergeCell ref="AQ22:AR22"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="AG20:AK21"/>
+    <mergeCell ref="AL20:AL23"/>
+    <mergeCell ref="R20:V21"/>
+    <mergeCell ref="W20:W23"/>
+    <mergeCell ref="X20:AC21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
   </mergeCells>
   <conditionalFormatting sqref="I38">
     <cfRule type="colorScale" priority="81">
@@ -2608,7 +2608,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7 B3 B5">
+  <conditionalFormatting sqref="B3 B7 B5">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -2618,7 +2618,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 D3 D5">
+  <conditionalFormatting sqref="D3 D7 D5">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -2628,7 +2628,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7 F3 F5">
+  <conditionalFormatting sqref="F3 F7 F5">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
@@ -2658,7 +2658,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7 C3 C5">
+  <conditionalFormatting sqref="C3 C7 C5">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -2668,7 +2668,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 E3 E7 E5">
+  <conditionalFormatting sqref="E3 E10 E7 E5">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -2678,7 +2678,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7 G3 G5">
+  <conditionalFormatting sqref="G3 G7 G5">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -2828,7 +2828,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I34 I31">
+  <conditionalFormatting sqref="I31 I34">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -2838,7 +2838,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34 J31">
+  <conditionalFormatting sqref="J31 J34">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Added new worksheet for new normalized data
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B010219-3BC9-4EFA-82F3-3F749A4CF149}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A33A749-7FB2-4735-8B7A-7044790FB8AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Old data" sheetId="1" r:id="rId1"/>
+    <sheet name="Normalized Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="20">
   <si>
     <t>Base Model</t>
   </si>
@@ -77,6 +78,15 @@
   <si>
     <t>AO</t>
   </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
 </sst>
 </file>
 
@@ -338,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -367,13 +377,17 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -394,16 +408,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -723,8 +734,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J3" sqref="I3:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,24 +773,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="30"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39"/>
+      <c r="A2" s="30"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1067,40 +1078,40 @@
       <c r="B11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="37" t="s">
+      <c r="C11" s="33"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="35"/>
       <c r="P11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="31"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="32"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="37" t="s">
+      <c r="R11" s="33"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="X11" s="31"/>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="32"/>
-      <c r="AA11" s="32"/>
-      <c r="AB11" s="32"/>
-      <c r="AC11" s="33"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="34"/>
+      <c r="Z11" s="34"/>
+      <c r="AA11" s="34"/>
+      <c r="AB11" s="34"/>
+      <c r="AC11" s="35"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1109,90 +1120,90 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="38"/>
       <c r="P12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
       </c>
-      <c r="R12" s="34"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="36"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="35"/>
-      <c r="AA12" s="35"/>
-      <c r="AB12" s="35"/>
-      <c r="AC12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="38"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="37"/>
+      <c r="Z12" s="37"/>
+      <c r="AA12" s="37"/>
+      <c r="AB12" s="37"/>
+      <c r="AC12" s="38"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29" t="s">
+      <c r="C13" s="32"/>
+      <c r="D13" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29" t="s">
+      <c r="E13" s="32"/>
+      <c r="F13" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="29"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="28" t="s">
+      <c r="G13" s="32"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29" t="s">
+      <c r="J13" s="32"/>
+      <c r="K13" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29" t="s">
+      <c r="L13" s="32"/>
+      <c r="M13" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="30"/>
+      <c r="N13" s="39"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="40" t="s">
+      <c r="Q13" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29" t="s">
+      <c r="R13" s="32"/>
+      <c r="S13" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29" t="s">
+      <c r="T13" s="32"/>
+      <c r="U13" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="V13" s="29"/>
-      <c r="W13" s="38"/>
-      <c r="X13" s="28" t="s">
+      <c r="V13" s="32"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="Y13" s="29"/>
-      <c r="Z13" s="29" t="s">
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AA13" s="29"/>
-      <c r="AB13" s="29" t="s">
+      <c r="AA13" s="32"/>
+      <c r="AB13" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="30"/>
+      <c r="AC13" s="39"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1216,7 +1227,7 @@
       <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="39"/>
+      <c r="H14" s="30"/>
       <c r="I14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1256,7 +1267,7 @@
       <c r="V14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W14" s="39"/>
+      <c r="W14" s="30"/>
       <c r="X14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1524,60 +1535,60 @@
       <c r="B20" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="37" t="s">
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="35"/>
       <c r="P20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R20" s="31"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="37" t="s">
+      <c r="R20" s="33"/>
+      <c r="S20" s="34"/>
+      <c r="T20" s="34"/>
+      <c r="U20" s="34"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="X20" s="31"/>
-      <c r="Y20" s="32"/>
-      <c r="Z20" s="32"/>
-      <c r="AA20" s="32"/>
-      <c r="AB20" s="32"/>
-      <c r="AC20" s="33"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="34"/>
+      <c r="Z20" s="34"/>
+      <c r="AA20" s="34"/>
+      <c r="AB20" s="34"/>
+      <c r="AC20" s="35"/>
       <c r="AE20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="AF20" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AG20" s="31"/>
-      <c r="AH20" s="32"/>
-      <c r="AI20" s="32"/>
-      <c r="AJ20" s="32"/>
-      <c r="AK20" s="33"/>
-      <c r="AL20" s="37" t="s">
+      <c r="AG20" s="33"/>
+      <c r="AH20" s="34"/>
+      <c r="AI20" s="34"/>
+      <c r="AJ20" s="34"/>
+      <c r="AK20" s="35"/>
+      <c r="AL20" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AM20" s="31"/>
-      <c r="AN20" s="32"/>
-      <c r="AO20" s="32"/>
-      <c r="AP20" s="32"/>
-      <c r="AQ20" s="32"/>
-      <c r="AR20" s="33"/>
+      <c r="AM20" s="33"/>
+      <c r="AN20" s="34"/>
+      <c r="AO20" s="34"/>
+      <c r="AP20" s="34"/>
+      <c r="AQ20" s="34"/>
+      <c r="AR20" s="35"/>
     </row>
     <row r="21" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1586,134 +1597,134 @@
       <c r="B21" s="7">
         <v>5</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="38"/>
       <c r="P21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q21" s="5">
         <v>5</v>
       </c>
-      <c r="R21" s="34"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="38"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="35"/>
-      <c r="Z21" s="35"/>
-      <c r="AA21" s="35"/>
-      <c r="AB21" s="35"/>
-      <c r="AC21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="37"/>
+      <c r="Z21" s="37"/>
+      <c r="AA21" s="37"/>
+      <c r="AB21" s="37"/>
+      <c r="AC21" s="38"/>
       <c r="AE21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AF21" s="5">
         <v>5</v>
       </c>
-      <c r="AG21" s="34"/>
-      <c r="AH21" s="35"/>
-      <c r="AI21" s="35"/>
-      <c r="AJ21" s="35"/>
-      <c r="AK21" s="36"/>
-      <c r="AL21" s="38"/>
-      <c r="AM21" s="34"/>
-      <c r="AN21" s="35"/>
-      <c r="AO21" s="35"/>
-      <c r="AP21" s="35"/>
-      <c r="AQ21" s="35"/>
-      <c r="AR21" s="36"/>
+      <c r="AG21" s="36"/>
+      <c r="AH21" s="37"/>
+      <c r="AI21" s="37"/>
+      <c r="AJ21" s="37"/>
+      <c r="AK21" s="38"/>
+      <c r="AL21" s="41"/>
+      <c r="AM21" s="36"/>
+      <c r="AN21" s="37"/>
+      <c r="AO21" s="37"/>
+      <c r="AP21" s="37"/>
+      <c r="AQ21" s="37"/>
+      <c r="AR21" s="38"/>
     </row>
     <row r="22" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29" t="s">
+      <c r="E22" s="32"/>
+      <c r="F22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="29"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="28" t="s">
+      <c r="G22" s="32"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29" t="s">
+      <c r="J22" s="32"/>
+      <c r="K22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29" t="s">
+      <c r="L22" s="32"/>
+      <c r="M22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="30"/>
+      <c r="N22" s="39"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="40" t="s">
+      <c r="Q22" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29" t="s">
+      <c r="R22" s="32"/>
+      <c r="S22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="29"/>
-      <c r="U22" s="29" t="s">
+      <c r="T22" s="32"/>
+      <c r="U22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="V22" s="29"/>
-      <c r="W22" s="38"/>
-      <c r="X22" s="28" t="s">
+      <c r="V22" s="32"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="29"/>
-      <c r="Z22" s="29" t="s">
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AA22" s="29"/>
-      <c r="AB22" s="29" t="s">
+      <c r="AA22" s="32"/>
+      <c r="AB22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AC22" s="30"/>
+      <c r="AC22" s="39"/>
       <c r="AE22" s="11"/>
-      <c r="AF22" s="40" t="s">
+      <c r="AF22" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="AG22" s="29"/>
-      <c r="AH22" s="29" t="s">
+      <c r="AG22" s="32"/>
+      <c r="AH22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AI22" s="29"/>
-      <c r="AJ22" s="29" t="s">
+      <c r="AI22" s="32"/>
+      <c r="AJ22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AK22" s="29"/>
-      <c r="AL22" s="38"/>
-      <c r="AM22" s="28" t="s">
+      <c r="AK22" s="32"/>
+      <c r="AL22" s="41"/>
+      <c r="AM22" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="AN22" s="29"/>
-      <c r="AO22" s="29" t="s">
+      <c r="AN22" s="32"/>
+      <c r="AO22" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AP22" s="29"/>
-      <c r="AQ22" s="29" t="s">
+      <c r="AP22" s="32"/>
+      <c r="AQ22" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AR22" s="30"/>
+      <c r="AR22" s="39"/>
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
@@ -1737,7 +1748,7 @@
       <c r="G23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="39"/>
+      <c r="H23" s="30"/>
       <c r="I23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1777,7 +1788,7 @@
       <c r="V23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W23" s="39"/>
+      <c r="W23" s="30"/>
       <c r="X23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1817,7 +1828,7 @@
       <c r="AK23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AL23" s="39"/>
+      <c r="AL23" s="30"/>
       <c r="AM23" s="3" t="s">
         <v>7</v>
       </c>
@@ -2304,18 +2315,18 @@
       <c r="G29" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29" t="s">
+      <c r="J29" s="32"/>
+      <c r="K29" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29" t="s">
+      <c r="L29" s="32"/>
+      <c r="M29" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="30"/>
+      <c r="N29" s="39"/>
       <c r="P29" s="14">
         <v>200</v>
       </c>
@@ -2485,12 +2496,36 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="R11:V12"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="AG20:AK21"/>
+    <mergeCell ref="AL20:AL23"/>
+    <mergeCell ref="R20:V21"/>
+    <mergeCell ref="W20:W23"/>
+    <mergeCell ref="X20:AC21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="AM20:AR21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AO22:AP22"/>
+    <mergeCell ref="AQ22:AR22"/>
+    <mergeCell ref="C20:G21"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:N21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
@@ -2507,36 +2542,12 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="C20:G21"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:N21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="AM20:AR21"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="AO22:AP22"/>
-    <mergeCell ref="AQ22:AR22"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="AG20:AK21"/>
-    <mergeCell ref="AL20:AL23"/>
-    <mergeCell ref="R20:V21"/>
-    <mergeCell ref="W20:W23"/>
-    <mergeCell ref="X20:AC21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="R11:V12"/>
+    <mergeCell ref="M13:N13"/>
   </mergeCells>
   <conditionalFormatting sqref="I38">
     <cfRule type="colorScale" priority="81">
@@ -2608,7 +2619,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3 B7 B5">
+  <conditionalFormatting sqref="B7 B3 B5">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -2618,7 +2629,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3 D7 D5">
+  <conditionalFormatting sqref="D7 D3 D5">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -2628,7 +2639,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3 F7 F5">
+  <conditionalFormatting sqref="F7 F3 F5">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
@@ -2658,7 +2669,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3 C7 C5">
+  <conditionalFormatting sqref="C7 C3 C5">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -2668,7 +2679,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3 E10 E7 E5">
+  <conditionalFormatting sqref="E10 E3 E7 E5">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -2678,7 +2689,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3 G7 G5">
+  <conditionalFormatting sqref="G7 G3 G5">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -2828,7 +2839,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31 I34">
+  <conditionalFormatting sqref="I34 I31">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -2838,7 +2849,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J31 J34">
+  <conditionalFormatting sqref="J34 J31">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -3251,4 +3262,685 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A37A8E-CDB1-4DEE-B664-FA66341E80CD}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="39"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="24">
+        <v>2.24666097710724E-4</v>
+      </c>
+      <c r="C3" s="24">
+        <v>2.5044871725185601E-4</v>
+      </c>
+      <c r="D3" s="24">
+        <v>0.98166596442460996</v>
+      </c>
+      <c r="E3" s="24">
+        <v>0.98212377816438601</v>
+      </c>
+      <c r="F3" s="24">
+        <v>37.120959625244097</v>
+      </c>
+      <c r="G3" s="25">
+        <v>36.5967915201187</v>
+      </c>
+      <c r="I3">
+        <f>(MIN(B3:C3)/MAX(B3:C3))</f>
+        <v>0.8970542958892278</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J5" si="0">(MIN(D3:E3)/MAX(D3:E3))</f>
+        <v>0.99953385331874189</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K5" si="1">(MIN(F3:G3)/MAX(F3:G3))</f>
+        <v>0.98587945703944202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="24">
+        <v>1.9500122456520301E-4</v>
+      </c>
+      <c r="C4" s="24">
+        <v>2.1797288509333099E-4</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0.98218990951776497</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0.98240298330783804</v>
+      </c>
+      <c r="F4" s="24">
+        <v>37.798613090515097</v>
+      </c>
+      <c r="G4" s="25">
+        <v>37.295324578285197</v>
+      </c>
+      <c r="I4">
+        <f>(MIN(B4:C4)/MAX(B4:C4))</f>
+        <v>0.89461230226735755</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0.99978310958568584</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>0.98668500055743602</v>
+      </c>
+      <c r="M4" s="28">
+        <f>(C$3-C4)/C$3</f>
+        <v>0.12967058691646924</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="24">
+        <v>2.4308788826601799E-4</v>
+      </c>
+      <c r="C5" s="24">
+        <v>2.7886579895493899E-4</v>
+      </c>
+      <c r="D5" s="24">
+        <v>0.98379539966583196</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0.98392467290162999</v>
+      </c>
+      <c r="F5" s="24">
+        <v>37.178017253875701</v>
+      </c>
+      <c r="G5" s="25">
+        <v>36.509374628067</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5" si="2">(MIN(B5:C5)/MAX(B5:C5))</f>
+        <v>0.87170204871662216</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0.99986861470256982</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>0.98201510798053659</v>
+      </c>
+      <c r="M5" s="28">
+        <f>(C$3-C5)/C$3</f>
+        <v>-0.11346467258806607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="24">
+        <v>2.2841662463179001E-4</v>
+      </c>
+      <c r="C6" s="24">
+        <v>2.3231557313920301E-4</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0.98487747460603703</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0.98535418227314897</v>
+      </c>
+      <c r="F6" s="24">
+        <v>37.299269056320099</v>
+      </c>
+      <c r="G6" s="25">
+        <v>37.225104932785001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="24">
+        <v>2.39534612046554E-4</v>
+      </c>
+      <c r="C7" s="24">
+        <v>2.6282198745320698E-4</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0.98356195926666201</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.98410001799464197</v>
+      </c>
+      <c r="F7" s="24">
+        <v>37.126828088760298</v>
+      </c>
+      <c r="G7" s="25">
+        <v>36.708566784858697</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D9" s="15"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I11" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7 B3 B5">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7 D3 D5">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7 F3 F5">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7 C3 C5">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 E3 E5">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7 G3 G5">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:G6">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B7 B3">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C7 C3">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D7 D3">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E7 E3">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F7 F3">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G7 G3">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E8 E3">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:C8">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:C8">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B8 B3">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C8 C3">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D8 D3">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F8 F3">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G8 G3">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G8">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F8">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E8">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D8">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C8">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L8">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:K8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New staggering performance of UNet with 512 filter size
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A33A749-7FB2-4735-8B7A-7044790FB8AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B37AE-A85A-4219-B348-042D2EDD20E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="26">
   <si>
     <t>Base Model</t>
   </si>
@@ -87,16 +87,36 @@
   <si>
     <t>R</t>
   </si>
+  <si>
+    <t>Unet-512-NM</t>
+  </si>
+  <si>
+    <t>SSIM+PSNR</t>
+  </si>
+  <si>
+    <t>No. of Parameters</t>
+  </si>
+  <si>
+    <t>Speed (s)</t>
+  </si>
+  <si>
+    <t>5 Epochs</t>
+  </si>
+  <si>
+    <t>Improvement</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +129,13 @@
       <color rgb="FFD4D4D4"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -345,10 +372,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -378,16 +407,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -408,18 +434,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,24 +824,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="39"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
+      <c r="A2" s="40"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1078,40 +1129,40 @@
       <c r="B11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="29" t="s">
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="35"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="34"/>
       <c r="P11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="33"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="34"/>
-      <c r="U11" s="34"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="29" t="s">
+      <c r="R11" s="32"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="34"/>
+      <c r="W11" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="X11" s="33"/>
-      <c r="Y11" s="34"/>
-      <c r="Z11" s="34"/>
-      <c r="AA11" s="34"/>
-      <c r="AB11" s="34"/>
-      <c r="AC11" s="35"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="33"/>
+      <c r="Z11" s="33"/>
+      <c r="AA11" s="33"/>
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="34"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1120,90 +1171,90 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="38"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="37"/>
       <c r="P12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
       </c>
-      <c r="R12" s="36"/>
-      <c r="S12" s="37"/>
-      <c r="T12" s="37"/>
-      <c r="U12" s="37"/>
-      <c r="V12" s="38"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="37"/>
-      <c r="Z12" s="37"/>
-      <c r="AA12" s="37"/>
-      <c r="AB12" s="37"/>
-      <c r="AC12" s="38"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="35"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="36"/>
+      <c r="AA12" s="36"/>
+      <c r="AB12" s="36"/>
+      <c r="AC12" s="37"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32" t="s">
+      <c r="E13" s="30"/>
+      <c r="F13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="40" t="s">
+      <c r="G13" s="30"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32" t="s">
+      <c r="J13" s="30"/>
+      <c r="K13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32" t="s">
+      <c r="L13" s="30"/>
+      <c r="M13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="39"/>
+      <c r="N13" s="31"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="31" t="s">
+      <c r="Q13" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32" t="s">
+      <c r="R13" s="30"/>
+      <c r="S13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32" t="s">
+      <c r="T13" s="30"/>
+      <c r="U13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="V13" s="32"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="40" t="s">
+      <c r="V13" s="30"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32" t="s">
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="AA13" s="32"/>
-      <c r="AB13" s="32" t="s">
+      <c r="AA13" s="30"/>
+      <c r="AB13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="39"/>
+      <c r="AC13" s="31"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1227,7 +1278,7 @@
       <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="30"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1267,7 +1318,7 @@
       <c r="V14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W14" s="30"/>
+      <c r="W14" s="40"/>
       <c r="X14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1535,60 +1586,60 @@
       <c r="B20" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="29" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="35"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="34"/>
       <c r="P20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R20" s="33"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="29" t="s">
+      <c r="R20" s="32"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="34"/>
+      <c r="W20" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="X20" s="33"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="34"/>
-      <c r="AA20" s="34"/>
-      <c r="AB20" s="34"/>
-      <c r="AC20" s="35"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="33"/>
+      <c r="Z20" s="33"/>
+      <c r="AA20" s="33"/>
+      <c r="AB20" s="33"/>
+      <c r="AC20" s="34"/>
       <c r="AE20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="AF20" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AG20" s="33"/>
-      <c r="AH20" s="34"/>
-      <c r="AI20" s="34"/>
-      <c r="AJ20" s="34"/>
-      <c r="AK20" s="35"/>
-      <c r="AL20" s="29" t="s">
+      <c r="AG20" s="32"/>
+      <c r="AH20" s="33"/>
+      <c r="AI20" s="33"/>
+      <c r="AJ20" s="33"/>
+      <c r="AK20" s="34"/>
+      <c r="AL20" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="AM20" s="33"/>
-      <c r="AN20" s="34"/>
-      <c r="AO20" s="34"/>
-      <c r="AP20" s="34"/>
-      <c r="AQ20" s="34"/>
-      <c r="AR20" s="35"/>
+      <c r="AM20" s="32"/>
+      <c r="AN20" s="33"/>
+      <c r="AO20" s="33"/>
+      <c r="AP20" s="33"/>
+      <c r="AQ20" s="33"/>
+      <c r="AR20" s="34"/>
     </row>
     <row r="21" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1597,134 +1648,134 @@
       <c r="B21" s="7">
         <v>5</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="38"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="37"/>
       <c r="P21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q21" s="5">
         <v>5</v>
       </c>
-      <c r="R21" s="36"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="37"/>
-      <c r="V21" s="38"/>
-      <c r="W21" s="41"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="37"/>
-      <c r="AA21" s="37"/>
-      <c r="AB21" s="37"/>
-      <c r="AC21" s="38"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="36"/>
+      <c r="Z21" s="36"/>
+      <c r="AA21" s="36"/>
+      <c r="AB21" s="36"/>
+      <c r="AC21" s="37"/>
       <c r="AE21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AF21" s="5">
         <v>5</v>
       </c>
-      <c r="AG21" s="36"/>
-      <c r="AH21" s="37"/>
-      <c r="AI21" s="37"/>
-      <c r="AJ21" s="37"/>
-      <c r="AK21" s="38"/>
-      <c r="AL21" s="41"/>
-      <c r="AM21" s="36"/>
-      <c r="AN21" s="37"/>
-      <c r="AO21" s="37"/>
-      <c r="AP21" s="37"/>
-      <c r="AQ21" s="37"/>
-      <c r="AR21" s="38"/>
+      <c r="AG21" s="35"/>
+      <c r="AH21" s="36"/>
+      <c r="AI21" s="36"/>
+      <c r="AJ21" s="36"/>
+      <c r="AK21" s="37"/>
+      <c r="AL21" s="39"/>
+      <c r="AM21" s="35"/>
+      <c r="AN21" s="36"/>
+      <c r="AO21" s="36"/>
+      <c r="AP21" s="36"/>
+      <c r="AQ21" s="36"/>
+      <c r="AR21" s="37"/>
     </row>
     <row r="22" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32" t="s">
+      <c r="E22" s="30"/>
+      <c r="F22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="40" t="s">
+      <c r="G22" s="30"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32" t="s">
+      <c r="J22" s="30"/>
+      <c r="K22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32" t="s">
+      <c r="L22" s="30"/>
+      <c r="M22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="39"/>
+      <c r="N22" s="31"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="31" t="s">
+      <c r="Q22" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="R22" s="32"/>
-      <c r="S22" s="32" t="s">
+      <c r="R22" s="30"/>
+      <c r="S22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="32"/>
-      <c r="U22" s="32" t="s">
+      <c r="T22" s="30"/>
+      <c r="U22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="V22" s="32"/>
-      <c r="W22" s="41"/>
-      <c r="X22" s="40" t="s">
+      <c r="V22" s="30"/>
+      <c r="W22" s="39"/>
+      <c r="X22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="32"/>
-      <c r="Z22" s="32" t="s">
+      <c r="Y22" s="30"/>
+      <c r="Z22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="AA22" s="32"/>
-      <c r="AB22" s="32" t="s">
+      <c r="AA22" s="30"/>
+      <c r="AB22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AC22" s="39"/>
+      <c r="AC22" s="31"/>
       <c r="AE22" s="11"/>
-      <c r="AF22" s="31" t="s">
+      <c r="AF22" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AG22" s="32"/>
-      <c r="AH22" s="32" t="s">
+      <c r="AG22" s="30"/>
+      <c r="AH22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="AI22" s="32"/>
-      <c r="AJ22" s="32" t="s">
+      <c r="AI22" s="30"/>
+      <c r="AJ22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AK22" s="32"/>
-      <c r="AL22" s="41"/>
-      <c r="AM22" s="40" t="s">
+      <c r="AK22" s="30"/>
+      <c r="AL22" s="39"/>
+      <c r="AM22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="AN22" s="32"/>
-      <c r="AO22" s="32" t="s">
+      <c r="AN22" s="30"/>
+      <c r="AO22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="AP22" s="32"/>
-      <c r="AQ22" s="32" t="s">
+      <c r="AP22" s="30"/>
+      <c r="AQ22" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AR22" s="39"/>
+      <c r="AR22" s="31"/>
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
@@ -1748,7 +1799,7 @@
       <c r="G23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="30"/>
+      <c r="H23" s="40"/>
       <c r="I23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1788,7 +1839,7 @@
       <c r="V23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W23" s="30"/>
+      <c r="W23" s="40"/>
       <c r="X23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1828,7 +1879,7 @@
       <c r="AK23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AL23" s="30"/>
+      <c r="AL23" s="40"/>
       <c r="AM23" s="3" t="s">
         <v>7</v>
       </c>
@@ -2315,18 +2366,18 @@
       <c r="G29" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="40" t="s">
+      <c r="I29" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32" t="s">
+      <c r="J29" s="30"/>
+      <c r="K29" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32" t="s">
+      <c r="L29" s="30"/>
+      <c r="M29" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="39"/>
+      <c r="N29" s="31"/>
       <c r="P29" s="14">
         <v>200</v>
       </c>
@@ -2496,36 +2547,12 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="AG20:AK21"/>
-    <mergeCell ref="AL20:AL23"/>
-    <mergeCell ref="R20:V21"/>
-    <mergeCell ref="W20:W23"/>
-    <mergeCell ref="X20:AC21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="AM20:AR21"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="AO22:AP22"/>
-    <mergeCell ref="AQ22:AR22"/>
-    <mergeCell ref="C20:G21"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:N21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="R11:V12"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
@@ -2542,12 +2569,36 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="R11:V12"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="C20:G21"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:N21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="AM20:AR21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AO22:AP22"/>
+    <mergeCell ref="AQ22:AR22"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="AG20:AK21"/>
+    <mergeCell ref="AL20:AL23"/>
+    <mergeCell ref="R20:V21"/>
+    <mergeCell ref="W20:W23"/>
+    <mergeCell ref="X20:AC21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
   </mergeCells>
   <conditionalFormatting sqref="I38">
     <cfRule type="colorScale" priority="81">
@@ -2619,7 +2670,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7 B3 B5">
+  <conditionalFormatting sqref="B3 B7 B5">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -2629,7 +2680,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 D3 D5">
+  <conditionalFormatting sqref="D3 D7 D5">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -2639,7 +2690,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7 F3 F5">
+  <conditionalFormatting sqref="F3 F7 F5">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
@@ -2669,7 +2720,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7 C3 C5">
+  <conditionalFormatting sqref="C3 C7 C5">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -2679,7 +2730,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 E3 E7 E5">
+  <conditionalFormatting sqref="E3 E10 E7 E5">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -2689,7 +2740,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7 G3 G5">
+  <conditionalFormatting sqref="G3 G7 G5">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -2839,7 +2890,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I34 I31">
+  <conditionalFormatting sqref="I31 I34">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -2849,7 +2900,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34 J31">
+  <conditionalFormatting sqref="J31 J34">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -3266,39 +3317,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A37A8E-CDB1-4DEE-B664-FA66341E80CD}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="179" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="39"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="33"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="40"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3317,8 +3382,27 @@
       <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H2" s="50"/>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
@@ -3328,32 +3412,57 @@
       <c r="C3" s="24">
         <v>2.5044871725185601E-4</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="46">
         <v>0.98166596442460996</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="46">
         <v>0.98212377816438601</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="42">
         <v>37.120959625244097</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="43">
         <v>36.5967915201187</v>
       </c>
-      <c r="I3">
+      <c r="H3" s="6">
+        <f>H5-(H4-H5)/2</f>
+        <v>1688601</v>
+      </c>
+      <c r="I3" s="11">
+        <v>154.21816682815501</v>
+      </c>
+      <c r="J3" s="1">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="K3" s="2">
+        <v>24</v>
+      </c>
+      <c r="L3" s="51">
+        <f>(C$3-C3)/C$3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="46">
+        <f>(E3-E$3)/E$3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="52">
+        <f>(G3-G$3)/G$3</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="48">
         <f>(MIN(B3:C3)/MAX(B3:C3))</f>
         <v>0.8970542958892278</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J5" si="0">(MIN(D3:E3)/MAX(D3:E3))</f>
+      <c r="W3" s="48">
+        <f>(MIN(D3:E3)/MAX(D3:E3))</f>
         <v>0.99953385331874189</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K5" si="1">(MIN(F3:G3)/MAX(F3:G3))</f>
+      <c r="X3" s="48">
+        <f>(MIN(F3:G3)/MAX(F3:G3))</f>
         <v>0.98587945703944202</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -3363,36 +3472,52 @@
       <c r="C4" s="24">
         <v>2.1797288509333099E-4</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="46">
         <v>0.98218990951776497</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="46">
         <v>0.98240298330783804</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="42">
         <v>37.798613090515097</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="43">
         <v>37.295324578285197</v>
       </c>
-      <c r="I4">
+      <c r="H4" s="6">
+        <v>1690401</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="51">
+        <f>(C$3-C4)/C$3</f>
+        <v>0.12967058691646924</v>
+      </c>
+      <c r="M4" s="46">
+        <f>(E4-E$3)/E$3</f>
+        <v>2.8428712313011508E-4</v>
+      </c>
+      <c r="N4" s="52">
+        <f>(G4-G$3)/G$3</f>
+        <v>1.9087275937358761E-2</v>
+      </c>
+      <c r="Q4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="V4" s="48">
         <f>(MIN(B4:C4)/MAX(B4:C4))</f>
         <v>0.89461230226735755</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
+      <c r="W4" s="48">
+        <f>(MIN(D4:E4)/MAX(D4:E4))</f>
         <v>0.99978310958568584</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
+      <c r="X4" s="48">
+        <f>(MIN(F4:G4)/MAX(F4:G4))</f>
         <v>0.98668500055743602</v>
       </c>
-      <c r="M4" s="28">
-        <f>(C$3-C4)/C$3</f>
-        <v>0.12967058691646924</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -3402,36 +3527,50 @@
       <c r="C5" s="24">
         <v>2.7886579895493899E-4</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="46">
         <v>0.98379539966583196</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="46">
         <v>0.98392467290162999</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="42">
         <v>37.178017253875701</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="43">
         <v>36.509374628067</v>
       </c>
-      <c r="I5">
-        <f t="shared" ref="I5" si="2">(MIN(B5:C5)/MAX(B5:C5))</f>
-        <v>0.87170204871662216</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>0.99986861470256982</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>0.98201510798053659</v>
-      </c>
-      <c r="M5" s="28">
+      <c r="H5" s="6">
+        <v>1689201</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="51">
         <f>(C$3-C5)/C$3</f>
         <v>-0.11346467258806607</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" s="46">
+        <f>(E5-E$3)/E$3</f>
+        <v>1.8336738986300717E-3</v>
+      </c>
+      <c r="N5" s="52">
+        <f>(G5-G$3)/G$3</f>
+        <v>-2.3886490706061712E-3</v>
+      </c>
+      <c r="V5" s="48">
+        <f>(MIN(B5:C5)/MAX(B5:C5))</f>
+        <v>0.87170204871662216</v>
+      </c>
+      <c r="W5" s="48">
+        <f>(MIN(D5:E5)/MAX(D5:E5))</f>
+        <v>0.99986861470256982</v>
+      </c>
+      <c r="X5" s="48">
+        <f>(MIN(F5:G5)/MAX(F5:G5))</f>
+        <v>0.98201510798053659</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -3441,20 +3580,50 @@
       <c r="C6" s="24">
         <v>2.3231557313920301E-4</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="46">
         <v>0.98487747460603703</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="46">
         <v>0.98535418227314897</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="42">
         <v>37.299269056320099</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="43">
         <v>37.225104932785001</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H6" s="6">
+        <v>1689201</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="51">
+        <f>(C$3-C6)/C$3</f>
+        <v>7.2402623226127227E-2</v>
+      </c>
+      <c r="M6" s="46">
+        <f>(E6-E$3)/E$3</f>
+        <v>3.2892026245415515E-3</v>
+      </c>
+      <c r="N6" s="52">
+        <f>(G6-G$3)/G$3</f>
+        <v>1.7168538185127317E-2</v>
+      </c>
+      <c r="V6" s="48">
+        <f>(MIN(B6:C6)/MAX(B6:C6))</f>
+        <v>0.98321701617016966</v>
+      </c>
+      <c r="W6" s="48">
+        <f>(MIN(D6:E6)/MAX(D6:E6))</f>
+        <v>0.99951620678565323</v>
+      </c>
+      <c r="X6" s="48">
+        <f>(MIN(F6:G6)/MAX(F6:G6))</f>
+        <v>0.99801164673165277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -3464,83 +3633,235 @@
       <c r="C7" s="24">
         <v>2.6282198745320698E-4</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="46">
         <v>0.98356195926666201</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="46">
         <v>0.98410001799464197</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="42">
         <v>37.126828088760298</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="43">
         <v>36.708566784858697</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H7" s="6">
+        <v>1689201</v>
+      </c>
+      <c r="I7" s="11">
+        <v>156.81576633453301</v>
+      </c>
+      <c r="J7" s="1">
+        <v>20.704391002655001</v>
+      </c>
+      <c r="K7" s="2">
+        <v>24.351212739944401</v>
+      </c>
+      <c r="L7" s="51">
+        <f>(C$3-C7)/C$3</f>
+        <v>-4.9404406367584523E-2</v>
+      </c>
+      <c r="M7" s="46">
+        <f>(E7-E$3)/E$3</f>
+        <v>2.0122105524719171E-3</v>
+      </c>
+      <c r="N7" s="52">
+        <f>(G7-G$3)/G$3</f>
+        <v>3.054236726696369E-3</v>
+      </c>
+      <c r="V7" s="48">
+        <f>(MIN(B7:C7)/MAX(B7:C7))</f>
+        <v>0.91139487364694294</v>
+      </c>
+      <c r="W7" s="48">
+        <f>(MIN(D7:E7)/MAX(D7:E7))</f>
+        <v>0.99945324792384782</v>
+      </c>
+      <c r="X7" s="48">
+        <f>(MIN(F7:G7)/MAX(F7:G7))</f>
+        <v>0.98873425699330819</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1.5743178133561701E-4</v>
+      </c>
+      <c r="C8" s="26">
+        <v>1.68062711854872E-4</v>
+      </c>
+      <c r="D8" s="47">
+        <v>0.98499482691287998</v>
+      </c>
+      <c r="E8" s="47">
+        <v>0.98527451008558198</v>
+      </c>
+      <c r="F8" s="44">
+        <v>38.884887685775702</v>
+      </c>
+      <c r="G8" s="45">
+        <v>38.678806848526001</v>
+      </c>
+      <c r="H8" s="7">
+        <v>2545505</v>
+      </c>
+      <c r="I8" s="3">
+        <v>77.299384355545001</v>
+      </c>
+      <c r="J8" s="4">
+        <v>10.3</v>
+      </c>
+      <c r="K8" s="5">
+        <v>13.8</v>
+      </c>
+      <c r="L8" s="53">
+        <f>(C$3-C8)/C$3</f>
+        <v>0.32895359297901722</v>
+      </c>
+      <c r="M8" s="47">
+        <f>(E8-E$3)/E$3</f>
+        <v>3.2080802758739512E-3</v>
+      </c>
+      <c r="N8" s="54">
+        <f>(G8-G$3)/G$3</f>
+        <v>5.6890651937690648E-2</v>
+      </c>
+      <c r="V8" s="48">
+        <f>(MIN(B8:C8)/MAX(B8:C8))</f>
+        <v>0.93674426407902323</v>
+      </c>
+      <c r="W8" s="48">
+        <f>(MIN(D8:E8)/MAX(D8:E8))</f>
+        <v>0.99971613680264837</v>
+      </c>
+      <c r="X8" s="48">
+        <f>(MIN(F8:G8)/MAX(F8:G8))</f>
+        <v>0.99470023318788992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D9" s="15"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I11" s="15"/>
     </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F13" s="28"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3 B7 B5">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3 D7 D5">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3 F7 F5">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3 C7 C5">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3 E7 E5">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7">
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3 G7 G5">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7 B3 B5">
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7 D3 D5">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6:G6">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -3550,17 +3871,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7 F3 F5">
+  <conditionalFormatting sqref="B5:B7 B3">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7 C3 C5">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C7 C3">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -3570,17 +3891,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 E3 E5">
+  <conditionalFormatting sqref="D5:D7 D3">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G7 G3 G5">
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E7 E3">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -3590,47 +3911,47 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
+  <conditionalFormatting sqref="F5:F7 F3">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6:G6">
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G7 G3">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B7 B3">
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C7 C3">
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D7 D3">
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -3640,17 +3961,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E7 E3">
+  <conditionalFormatting sqref="F8">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F7 F3">
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -3660,7 +3981,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G7 G3">
+  <conditionalFormatting sqref="E8">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -3670,7 +3991,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
+  <conditionalFormatting sqref="E8">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -3680,17 +4001,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
+  <conditionalFormatting sqref="D8">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -3700,7 +4021,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
+  <conditionalFormatting sqref="D8">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -3710,47 +4031,57 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
+  <conditionalFormatting sqref="E5:E8 E3">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:C8">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:C8">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B8 B3">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C8 C3">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D8 D3">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -3760,107 +4091,87 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E8 E3">
+  <conditionalFormatting sqref="F5:F8 F3">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G8 G3">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G8">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F8">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E8">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D8">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C8">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:C8">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:C8">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B8 B3">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C8 C3">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D8 D3">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F8 F3">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B8">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G8 G3">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G8">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F8">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12:L17">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3870,73 +4181,83 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E8">
+  <conditionalFormatting sqref="V3:V8 I15:I17">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W3:X8 J15:K17">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M8">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C8">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B8">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L8">
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N8">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I8">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:K8">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
DenseNet results were added
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B37AE-A85A-4219-B348-042D2EDD20E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428ABA6A-7AFE-49DE-AB3C-99486AE277E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="27">
   <si>
     <t>Base Model</t>
   </si>
@@ -105,6 +105,9 @@
   <si>
     <t>Improvement</t>
   </si>
+  <si>
+    <t>DenseNet128-NM</t>
+  </si>
 </sst>
 </file>
 
@@ -114,7 +117,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
-    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -377,7 +380,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -407,6 +410,21 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -446,26 +464,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -824,24 +828,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="45"/>
+      <c r="F1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="31"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
+      <c r="A2" s="55"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1129,40 +1133,40 @@
       <c r="B11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="38" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="32"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="34"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="49"/>
       <c r="P11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="32"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="34"/>
-      <c r="W11" s="38" t="s">
+      <c r="R11" s="47"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="33"/>
-      <c r="Z11" s="33"/>
-      <c r="AA11" s="33"/>
-      <c r="AB11" s="33"/>
-      <c r="AC11" s="34"/>
+      <c r="X11" s="47"/>
+      <c r="Y11" s="48"/>
+      <c r="Z11" s="48"/>
+      <c r="AA11" s="48"/>
+      <c r="AB11" s="48"/>
+      <c r="AC11" s="49"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1171,90 +1175,90 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="37"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="52"/>
       <c r="P12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
       </c>
-      <c r="R12" s="35"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="37"/>
-      <c r="W12" s="39"/>
-      <c r="X12" s="35"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="36"/>
-      <c r="AA12" s="36"/>
-      <c r="AB12" s="36"/>
-      <c r="AC12" s="37"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="51"/>
+      <c r="U12" s="51"/>
+      <c r="V12" s="52"/>
+      <c r="W12" s="54"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="51"/>
+      <c r="Z12" s="51"/>
+      <c r="AA12" s="51"/>
+      <c r="AB12" s="51"/>
+      <c r="AC12" s="52"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30" t="s">
+      <c r="C13" s="45"/>
+      <c r="D13" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30" t="s">
+      <c r="E13" s="45"/>
+      <c r="F13" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="29" t="s">
+      <c r="G13" s="45"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30" t="s">
+      <c r="J13" s="45"/>
+      <c r="K13" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30" t="s">
+      <c r="L13" s="45"/>
+      <c r="M13" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="31"/>
+      <c r="N13" s="46"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="41" t="s">
+      <c r="Q13" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30" t="s">
+      <c r="R13" s="45"/>
+      <c r="S13" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30" t="s">
+      <c r="T13" s="45"/>
+      <c r="U13" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="V13" s="30"/>
-      <c r="W13" s="39"/>
-      <c r="X13" s="29" t="s">
+      <c r="V13" s="45"/>
+      <c r="W13" s="54"/>
+      <c r="X13" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="30" t="s">
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="AA13" s="30"/>
-      <c r="AB13" s="30" t="s">
+      <c r="AA13" s="45"/>
+      <c r="AB13" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="31"/>
+      <c r="AC13" s="46"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1278,7 +1282,7 @@
       <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="40"/>
+      <c r="H14" s="55"/>
       <c r="I14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1318,7 +1322,7 @@
       <c r="V14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W14" s="40"/>
+      <c r="W14" s="55"/>
       <c r="X14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1586,60 +1590,60 @@
       <c r="B20" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="38" t="s">
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="32"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="34"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="49"/>
       <c r="P20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R20" s="32"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="38" t="s">
+      <c r="R20" s="47"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="49"/>
+      <c r="W20" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="X20" s="32"/>
-      <c r="Y20" s="33"/>
-      <c r="Z20" s="33"/>
-      <c r="AA20" s="33"/>
-      <c r="AB20" s="33"/>
-      <c r="AC20" s="34"/>
+      <c r="X20" s="47"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="49"/>
       <c r="AE20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="AF20" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AG20" s="32"/>
-      <c r="AH20" s="33"/>
-      <c r="AI20" s="33"/>
-      <c r="AJ20" s="33"/>
-      <c r="AK20" s="34"/>
-      <c r="AL20" s="38" t="s">
+      <c r="AG20" s="47"/>
+      <c r="AH20" s="48"/>
+      <c r="AI20" s="48"/>
+      <c r="AJ20" s="48"/>
+      <c r="AK20" s="49"/>
+      <c r="AL20" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="AM20" s="32"/>
-      <c r="AN20" s="33"/>
-      <c r="AO20" s="33"/>
-      <c r="AP20" s="33"/>
-      <c r="AQ20" s="33"/>
-      <c r="AR20" s="34"/>
+      <c r="AM20" s="47"/>
+      <c r="AN20" s="48"/>
+      <c r="AO20" s="48"/>
+      <c r="AP20" s="48"/>
+      <c r="AQ20" s="48"/>
+      <c r="AR20" s="49"/>
     </row>
     <row r="21" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1648,134 +1652,134 @@
       <c r="B21" s="7">
         <v>5</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="37"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="52"/>
       <c r="P21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q21" s="5">
         <v>5</v>
       </c>
-      <c r="R21" s="35"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="39"/>
-      <c r="X21" s="35"/>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="36"/>
-      <c r="AA21" s="36"/>
-      <c r="AB21" s="36"/>
-      <c r="AC21" s="37"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="51"/>
+      <c r="V21" s="52"/>
+      <c r="W21" s="54"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="51"/>
+      <c r="AB21" s="51"/>
+      <c r="AC21" s="52"/>
       <c r="AE21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AF21" s="5">
         <v>5</v>
       </c>
-      <c r="AG21" s="35"/>
-      <c r="AH21" s="36"/>
-      <c r="AI21" s="36"/>
-      <c r="AJ21" s="36"/>
-      <c r="AK21" s="37"/>
-      <c r="AL21" s="39"/>
-      <c r="AM21" s="35"/>
-      <c r="AN21" s="36"/>
-      <c r="AO21" s="36"/>
-      <c r="AP21" s="36"/>
-      <c r="AQ21" s="36"/>
-      <c r="AR21" s="37"/>
+      <c r="AG21" s="50"/>
+      <c r="AH21" s="51"/>
+      <c r="AI21" s="51"/>
+      <c r="AJ21" s="51"/>
+      <c r="AK21" s="52"/>
+      <c r="AL21" s="54"/>
+      <c r="AM21" s="50"/>
+      <c r="AN21" s="51"/>
+      <c r="AO21" s="51"/>
+      <c r="AP21" s="51"/>
+      <c r="AQ21" s="51"/>
+      <c r="AR21" s="52"/>
     </row>
     <row r="22" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30" t="s">
+      <c r="C22" s="45"/>
+      <c r="D22" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30" t="s">
+      <c r="E22" s="45"/>
+      <c r="F22" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="29" t="s">
+      <c r="G22" s="45"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30" t="s">
+      <c r="J22" s="45"/>
+      <c r="K22" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30" t="s">
+      <c r="L22" s="45"/>
+      <c r="M22" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="31"/>
+      <c r="N22" s="46"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="41" t="s">
+      <c r="Q22" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="R22" s="30"/>
-      <c r="S22" s="30" t="s">
+      <c r="R22" s="45"/>
+      <c r="S22" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="30"/>
-      <c r="U22" s="30" t="s">
+      <c r="T22" s="45"/>
+      <c r="U22" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="V22" s="30"/>
-      <c r="W22" s="39"/>
-      <c r="X22" s="29" t="s">
+      <c r="V22" s="45"/>
+      <c r="W22" s="54"/>
+      <c r="X22" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="30"/>
-      <c r="Z22" s="30" t="s">
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="AA22" s="30"/>
-      <c r="AB22" s="30" t="s">
+      <c r="AA22" s="45"/>
+      <c r="AB22" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="AC22" s="31"/>
+      <c r="AC22" s="46"/>
       <c r="AE22" s="11"/>
-      <c r="AF22" s="41" t="s">
+      <c r="AF22" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="AG22" s="30"/>
-      <c r="AH22" s="30" t="s">
+      <c r="AG22" s="45"/>
+      <c r="AH22" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="AI22" s="30"/>
-      <c r="AJ22" s="30" t="s">
+      <c r="AI22" s="45"/>
+      <c r="AJ22" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="AK22" s="30"/>
-      <c r="AL22" s="39"/>
-      <c r="AM22" s="29" t="s">
+      <c r="AK22" s="45"/>
+      <c r="AL22" s="54"/>
+      <c r="AM22" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="AN22" s="30"/>
-      <c r="AO22" s="30" t="s">
+      <c r="AN22" s="45"/>
+      <c r="AO22" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="AP22" s="30"/>
-      <c r="AQ22" s="30" t="s">
+      <c r="AP22" s="45"/>
+      <c r="AQ22" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="AR22" s="31"/>
+      <c r="AR22" s="46"/>
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
@@ -1799,7 +1803,7 @@
       <c r="G23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="40"/>
+      <c r="H23" s="55"/>
       <c r="I23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1839,7 +1843,7 @@
       <c r="V23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W23" s="40"/>
+      <c r="W23" s="55"/>
       <c r="X23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1879,7 +1883,7 @@
       <c r="AK23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AL23" s="40"/>
+      <c r="AL23" s="55"/>
       <c r="AM23" s="3" t="s">
         <v>7</v>
       </c>
@@ -2366,18 +2370,18 @@
       <c r="G29" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="29" t="s">
+      <c r="I29" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30" t="s">
+      <c r="J29" s="45"/>
+      <c r="K29" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="30"/>
-      <c r="M29" s="30" t="s">
+      <c r="L29" s="45"/>
+      <c r="M29" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="31"/>
+      <c r="N29" s="46"/>
       <c r="P29" s="14">
         <v>200</v>
       </c>
@@ -3320,12 +3324,12 @@
   <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
@@ -3333,37 +3337,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="45"/>
+      <c r="F1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="49" t="s">
+      <c r="G1" s="46"/>
+      <c r="H1" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="32" t="s">
+      <c r="J1" s="48"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="49"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
+      <c r="A2" s="55"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3382,8 +3386,8 @@
       <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="58"/>
+      <c r="I2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -3392,13 +3396,13 @@
       <c r="K2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="56" t="s">
+      <c r="M2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="57" t="s">
+      <c r="N2" s="42" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3412,23 +3416,23 @@
       <c r="C3" s="24">
         <v>2.5044871725185601E-4</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="33">
         <v>0.98166596442460996</v>
       </c>
-      <c r="E3" s="46">
+      <c r="E3" s="33">
         <v>0.98212377816438601</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="29">
         <v>37.120959625244097</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="30">
         <v>36.5967915201187</v>
       </c>
       <c r="H3" s="6">
         <f>H5-(H4-H5)/2</f>
         <v>1688601</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="1">
         <v>154.21816682815501</v>
       </c>
       <c r="J3" s="1">
@@ -3437,28 +3441,28 @@
       <c r="K3" s="2">
         <v>24</v>
       </c>
-      <c r="L3" s="51">
-        <f>(C$3-C3)/C$3</f>
+      <c r="L3" s="36">
+        <f t="shared" ref="L3:L8" si="0">(C$3-C3)/C$3</f>
         <v>0</v>
       </c>
-      <c r="M3" s="46">
-        <f>(E3-E$3)/E$3</f>
+      <c r="M3" s="33">
+        <f t="shared" ref="M3:M8" si="1">(E3-E$3)/E$3</f>
         <v>0</v>
       </c>
-      <c r="N3" s="52">
-        <f>(G3-G$3)/G$3</f>
+      <c r="N3" s="37">
+        <f t="shared" ref="N3:N8" si="2">(G3-G$3)/G$3</f>
         <v>0</v>
       </c>
-      <c r="V3" s="48">
-        <f>(MIN(B3:C3)/MAX(B3:C3))</f>
+      <c r="V3" s="35">
+        <f t="shared" ref="V3:V8" si="3">(MIN(B3:C3)/MAX(B3:C3))</f>
         <v>0.8970542958892278</v>
       </c>
-      <c r="W3" s="48">
-        <f>(MIN(D3:E3)/MAX(D3:E3))</f>
+      <c r="W3" s="35">
+        <f t="shared" ref="W3:W8" si="4">(MIN(D3:E3)/MAX(D3:E3))</f>
         <v>0.99953385331874189</v>
       </c>
-      <c r="X3" s="48">
-        <f>(MIN(F3:G3)/MAX(F3:G3))</f>
+      <c r="X3" s="35">
+        <f t="shared" ref="X3:X8" si="5">(MIN(F3:G3)/MAX(F3:G3))</f>
         <v>0.98587945703944202</v>
       </c>
     </row>
@@ -3472,48 +3476,48 @@
       <c r="C4" s="24">
         <v>2.1797288509333099E-4</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="33">
         <v>0.98218990951776497</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="33">
         <v>0.98240298330783804</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="29">
         <v>37.798613090515097</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="30">
         <v>37.295324578285197</v>
       </c>
       <c r="H4" s="6">
         <v>1690401</v>
       </c>
-      <c r="I4" s="11"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="51">
-        <f>(C$3-C4)/C$3</f>
+      <c r="L4" s="36">
+        <f t="shared" si="0"/>
         <v>0.12967058691646924</v>
       </c>
-      <c r="M4" s="46">
-        <f>(E4-E$3)/E$3</f>
+      <c r="M4" s="33">
+        <f t="shared" si="1"/>
         <v>2.8428712313011508E-4</v>
       </c>
-      <c r="N4" s="52">
-        <f>(G4-G$3)/G$3</f>
+      <c r="N4" s="37">
+        <f t="shared" si="2"/>
         <v>1.9087275937358761E-2</v>
       </c>
-      <c r="Q4" s="48"/>
-      <c r="S4" s="48"/>
-      <c r="V4" s="48">
-        <f>(MIN(B4:C4)/MAX(B4:C4))</f>
+      <c r="Q4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="V4" s="35">
+        <f t="shared" si="3"/>
         <v>0.89461230226735755</v>
       </c>
-      <c r="W4" s="48">
-        <f>(MIN(D4:E4)/MAX(D4:E4))</f>
+      <c r="W4" s="35">
+        <f t="shared" si="4"/>
         <v>0.99978310958568584</v>
       </c>
-      <c r="X4" s="48">
-        <f>(MIN(F4:G4)/MAX(F4:G4))</f>
+      <c r="X4" s="35">
+        <f t="shared" si="5"/>
         <v>0.98668500055743602</v>
       </c>
     </row>
@@ -3527,46 +3531,46 @@
       <c r="C5" s="24">
         <v>2.7886579895493899E-4</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="33">
         <v>0.98379539966583196</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="33">
         <v>0.98392467290162999</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="29">
         <v>37.178017253875701</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="30">
         <v>36.509374628067</v>
       </c>
       <c r="H5" s="6">
         <v>1689201</v>
       </c>
-      <c r="I5" s="11"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="51">
-        <f>(C$3-C5)/C$3</f>
+      <c r="L5" s="36">
+        <f t="shared" si="0"/>
         <v>-0.11346467258806607</v>
       </c>
-      <c r="M5" s="46">
-        <f>(E5-E$3)/E$3</f>
+      <c r="M5" s="33">
+        <f t="shared" si="1"/>
         <v>1.8336738986300717E-3</v>
       </c>
-      <c r="N5" s="52">
-        <f>(G5-G$3)/G$3</f>
+      <c r="N5" s="37">
+        <f t="shared" si="2"/>
         <v>-2.3886490706061712E-3</v>
       </c>
-      <c r="V5" s="48">
-        <f>(MIN(B5:C5)/MAX(B5:C5))</f>
+      <c r="V5" s="35">
+        <f t="shared" si="3"/>
         <v>0.87170204871662216</v>
       </c>
-      <c r="W5" s="48">
-        <f>(MIN(D5:E5)/MAX(D5:E5))</f>
+      <c r="W5" s="35">
+        <f t="shared" si="4"/>
         <v>0.99986861470256982</v>
       </c>
-      <c r="X5" s="48">
-        <f>(MIN(F5:G5)/MAX(F5:G5))</f>
+      <c r="X5" s="35">
+        <f t="shared" si="5"/>
         <v>0.98201510798053659</v>
       </c>
     </row>
@@ -3580,46 +3584,46 @@
       <c r="C6" s="24">
         <v>2.3231557313920301E-4</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="33">
         <v>0.98487747460603703</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="33">
         <v>0.98535418227314897</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="29">
         <v>37.299269056320099</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="30">
         <v>37.225104932785001</v>
       </c>
       <c r="H6" s="6">
         <v>1689201</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="51">
-        <f>(C$3-C6)/C$3</f>
+      <c r="L6" s="36">
+        <f t="shared" si="0"/>
         <v>7.2402623226127227E-2</v>
       </c>
-      <c r="M6" s="46">
-        <f>(E6-E$3)/E$3</f>
+      <c r="M6" s="33">
+        <f t="shared" si="1"/>
         <v>3.2892026245415515E-3</v>
       </c>
-      <c r="N6" s="52">
-        <f>(G6-G$3)/G$3</f>
+      <c r="N6" s="37">
+        <f t="shared" si="2"/>
         <v>1.7168538185127317E-2</v>
       </c>
-      <c r="V6" s="48">
-        <f>(MIN(B6:C6)/MAX(B6:C6))</f>
+      <c r="V6" s="35">
+        <f t="shared" si="3"/>
         <v>0.98321701617016966</v>
       </c>
-      <c r="W6" s="48">
-        <f>(MIN(D6:E6)/MAX(D6:E6))</f>
+      <c r="W6" s="35">
+        <f t="shared" si="4"/>
         <v>0.99951620678565323</v>
       </c>
-      <c r="X6" s="48">
-        <f>(MIN(F6:G6)/MAX(F6:G6))</f>
+      <c r="X6" s="35">
+        <f t="shared" si="5"/>
         <v>0.99801164673165277</v>
       </c>
     </row>
@@ -3633,22 +3637,22 @@
       <c r="C7" s="24">
         <v>2.6282198745320698E-4</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="33">
         <v>0.98356195926666201</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="33">
         <v>0.98410001799464197</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="29">
         <v>37.126828088760298</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="30">
         <v>36.708566784858697</v>
       </c>
       <c r="H7" s="6">
         <v>1689201</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="1">
         <v>156.81576633453301</v>
       </c>
       <c r="J7" s="1">
@@ -3657,95 +3661,139 @@
       <c r="K7" s="2">
         <v>24.351212739944401</v>
       </c>
-      <c r="L7" s="51">
-        <f>(C$3-C7)/C$3</f>
+      <c r="L7" s="36">
+        <f t="shared" si="0"/>
         <v>-4.9404406367584523E-2</v>
       </c>
-      <c r="M7" s="46">
-        <f>(E7-E$3)/E$3</f>
+      <c r="M7" s="33">
+        <f t="shared" si="1"/>
         <v>2.0122105524719171E-3</v>
       </c>
-      <c r="N7" s="52">
-        <f>(G7-G$3)/G$3</f>
+      <c r="N7" s="37">
+        <f t="shared" si="2"/>
         <v>3.054236726696369E-3</v>
       </c>
-      <c r="V7" s="48">
-        <f>(MIN(B7:C7)/MAX(B7:C7))</f>
+      <c r="V7" s="35">
+        <f t="shared" si="3"/>
         <v>0.91139487364694294</v>
       </c>
-      <c r="W7" s="48">
-        <f>(MIN(D7:E7)/MAX(D7:E7))</f>
+      <c r="W7" s="35">
+        <f t="shared" si="4"/>
         <v>0.99945324792384782</v>
       </c>
-      <c r="X7" s="48">
-        <f>(MIN(F7:G7)/MAX(F7:G7))</f>
+      <c r="X7" s="35">
+        <f t="shared" si="5"/>
         <v>0.98873425699330819</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="24">
+        <v>2.27021457831142E-4</v>
+      </c>
+      <c r="C8" s="24">
+        <v>2.41102768250129E-4</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0.98064835458993904</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0.98107850506901695</v>
+      </c>
+      <c r="F8" s="29">
+        <v>37.095721302032402</v>
+      </c>
+      <c r="G8" s="30">
+        <v>36.814777007102897</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1384460</v>
+      </c>
+      <c r="I8">
+        <v>241.57</v>
+      </c>
+      <c r="J8">
+        <v>29.43</v>
+      </c>
+      <c r="K8">
+        <v>34.67</v>
+      </c>
+      <c r="L8" s="36">
+        <f t="shared" si="0"/>
+        <v>3.731681720824527E-2</v>
+      </c>
+      <c r="M8" s="33">
+        <f t="shared" si="1"/>
+        <v>-1.0642987356672099E-3</v>
+      </c>
+      <c r="N8" s="37">
+        <f t="shared" si="2"/>
+        <v>5.9564097815613774E-3</v>
+      </c>
+      <c r="V8" s="35">
+        <f>(MIN(B9:C9)/MAX(B9:C9))</f>
+        <v>0.93674426407902323</v>
+      </c>
+      <c r="W8" s="35">
+        <f>(MIN(D9:E9)/MAX(D9:E9))</f>
+        <v>0.99971613680264837</v>
+      </c>
+      <c r="X8" s="35">
+        <f>(MIN(F9:G9)/MAX(F9:G9))</f>
+        <v>0.99470023318788992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B9" s="26">
         <v>1.5743178133561701E-4</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C9" s="26">
         <v>1.68062711854872E-4</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D9" s="34">
         <v>0.98499482691287998</v>
       </c>
-      <c r="E8" s="47">
+      <c r="E9" s="34">
         <v>0.98527451008558198</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F9" s="31">
         <v>38.884887685775702</v>
       </c>
-      <c r="G8" s="45">
+      <c r="G9" s="32">
         <v>38.678806848526001</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H9" s="7">
         <v>2545505</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I9" s="4">
         <v>77.299384355545001</v>
       </c>
-      <c r="J8" s="4">
-        <v>10.3</v>
-      </c>
-      <c r="K8" s="5">
+      <c r="J9" s="43">
+        <v>10.25</v>
+      </c>
+      <c r="K9" s="5">
         <v>13.8</v>
       </c>
-      <c r="L8" s="53">
-        <f>(C$3-C8)/C$3</f>
+      <c r="L9" s="38">
+        <f>(C$3-C9)/C$3</f>
         <v>0.32895359297901722</v>
       </c>
-      <c r="M8" s="47">
-        <f>(E8-E$3)/E$3</f>
+      <c r="M9" s="34">
+        <f>(E9-E$3)/E$3</f>
         <v>3.2080802758739512E-3</v>
       </c>
-      <c r="N8" s="54">
-        <f>(G8-G$3)/G$3</f>
+      <c r="N9" s="39">
+        <f>(G9-G$3)/G$3</f>
         <v>5.6890651937690648E-2</v>
       </c>
-      <c r="V8" s="48">
-        <f>(MIN(B8:C8)/MAX(B8:C8))</f>
-        <v>0.93674426407902323</v>
-      </c>
-      <c r="W8" s="48">
-        <f>(MIN(D8:E8)/MAX(D8:E8))</f>
-        <v>0.99971613680264837</v>
-      </c>
-      <c r="X8" s="48">
-        <f>(MIN(F8:G8)/MAX(F8:G8))</f>
-        <v>0.99470023318788992</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="15"/>
-      <c r="I9" s="15"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C11" s="15"/>
       <c r="I11" s="15"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -3762,7 +3810,7 @@
     <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="115">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3772,7 +3820,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="114">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3782,7 +3830,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="113">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3792,7 +3840,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3 B7 B5">
-    <cfRule type="colorScale" priority="48">
+    <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3802,7 +3850,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3 D7 D5">
-    <cfRule type="colorScale" priority="47">
+    <cfRule type="colorScale" priority="111">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3812,7 +3860,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3 F7 F5">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3822,7 +3870,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 C7 C5">
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3832,7 +3880,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3 E7 E5">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3842,7 +3890,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3 G7 G5">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="107">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3852,7 +3900,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="106">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3862,7 +3910,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:G6">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="105">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3872,7 +3920,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B7 B3">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="104">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3882,7 +3930,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:C7 C3">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3892,7 +3940,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D7 D3">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="102">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3902,7 +3950,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E7 E3">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3912,7 +3960,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F7 F3">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="100">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3922,7 +3970,357 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G7 G3">
-    <cfRule type="colorScale" priority="35">
+    <cfRule type="colorScale" priority="99">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="colorScale" priority="98">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="colorScale" priority="97">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="colorScale" priority="96">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="colorScale" priority="95">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="colorScale" priority="94">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="colorScale" priority="93">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="colorScale" priority="92">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="colorScale" priority="91">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="colorScale" priority="90">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="colorScale" priority="89">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:C9">
+    <cfRule type="colorScale" priority="88">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:C9">
+    <cfRule type="colorScale" priority="87">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12:L17">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V8 I15:I17">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W3:X8 J15:K17">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E7 E9 E3">
+    <cfRule type="colorScale" priority="149">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B7 B9 B3">
+    <cfRule type="colorScale" priority="152">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C7 C9 C3">
+    <cfRule type="colorScale" priority="155">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D7 D9 D3">
+    <cfRule type="colorScale" priority="158">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F7 F9 F3">
+    <cfRule type="colorScale" priority="161">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G7 G9 G3">
+    <cfRule type="colorScale" priority="164">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G7 G9">
+    <cfRule type="colorScale" priority="167">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F7 F9">
+    <cfRule type="colorScale" priority="169">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E7 E9">
+    <cfRule type="colorScale" priority="171">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D7 D9">
+    <cfRule type="colorScale" priority="173">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C7 C9">
+    <cfRule type="colorScale" priority="175">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B7 B9">
+    <cfRule type="colorScale" priority="177">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3932,37 +4330,107 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3981,18 +4449,38 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4002,186 +4490,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E8 E3">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:C8">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:C8">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B8 B3">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C8 C3">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D8 D3">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F8 F3">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G8 G3">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G8">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F8">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E8">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D8">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C8">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B8">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L12:L17">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B9">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C9">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V8 I15:I17">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -4191,27 +4549,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W3:X8 J15:K17">
+  <conditionalFormatting sqref="E3:E9">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L8">
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F9">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M8">
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -4221,17 +4579,77 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N8">
+  <conditionalFormatting sqref="L3:L9">
+    <cfRule type="colorScale" priority="182">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M9">
+    <cfRule type="colorScale" priority="184">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N9">
+    <cfRule type="colorScale" priority="186">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I7 I9">
+    <cfRule type="colorScale" priority="188">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J7 J9">
+    <cfRule type="colorScale" priority="190">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K7 K9">
+    <cfRule type="colorScale" priority="192">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I9">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I8">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -4241,17 +4659,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J8">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K8">
+  <conditionalFormatting sqref="K3:K9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Updated report.xlsx for TL 100 samples
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B78C11-42BF-456D-9FF2-2A025C89FC28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF23F73E-B2E3-4E16-8082-17DE40519C41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -469,13 +469,16 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -496,25 +499,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -875,24 +875,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="58"/>
+      <c r="G1" s="66"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1180,40 +1180,40 @@
       <c r="B11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="65" t="s">
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="59"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="61"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="62"/>
       <c r="P11" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="59"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="60"/>
-      <c r="V11" s="61"/>
-      <c r="W11" s="65" t="s">
+      <c r="R11" s="60"/>
+      <c r="S11" s="61"/>
+      <c r="T11" s="61"/>
+      <c r="U11" s="61"/>
+      <c r="V11" s="62"/>
+      <c r="W11" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="X11" s="59"/>
-      <c r="Y11" s="60"/>
-      <c r="Z11" s="60"/>
-      <c r="AA11" s="60"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="61"/>
+      <c r="X11" s="60"/>
+      <c r="Y11" s="61"/>
+      <c r="Z11" s="61"/>
+      <c r="AA11" s="61"/>
+      <c r="AB11" s="61"/>
+      <c r="AC11" s="62"/>
     </row>
     <row r="12" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1222,90 +1222,90 @@
       <c r="B12" s="5">
         <v>3</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="63"/>
-      <c r="L12" s="63"/>
-      <c r="M12" s="63"/>
-      <c r="N12" s="64"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="65"/>
       <c r="P12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q12" s="5">
         <v>3</v>
       </c>
-      <c r="R12" s="62"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="63"/>
-      <c r="U12" s="63"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="66"/>
-      <c r="X12" s="62"/>
-      <c r="Y12" s="63"/>
-      <c r="Z12" s="63"/>
-      <c r="AA12" s="63"/>
-      <c r="AB12" s="63"/>
-      <c r="AC12" s="64"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="64"/>
+      <c r="T12" s="64"/>
+      <c r="U12" s="64"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="68"/>
+      <c r="X12" s="63"/>
+      <c r="Y12" s="64"/>
+      <c r="Z12" s="64"/>
+      <c r="AA12" s="64"/>
+      <c r="AB12" s="64"/>
+      <c r="AC12" s="65"/>
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57" t="s">
+      <c r="C13" s="59"/>
+      <c r="D13" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57" t="s">
+      <c r="E13" s="59"/>
+      <c r="F13" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="56" t="s">
+      <c r="G13" s="59"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="57"/>
-      <c r="K13" s="57" t="s">
+      <c r="J13" s="59"/>
+      <c r="K13" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="57"/>
-      <c r="M13" s="57" t="s">
+      <c r="L13" s="59"/>
+      <c r="M13" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="58"/>
+      <c r="N13" s="66"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="68" t="s">
+      <c r="Q13" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="57"/>
-      <c r="S13" s="57" t="s">
+      <c r="R13" s="59"/>
+      <c r="S13" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57" t="s">
+      <c r="T13" s="59"/>
+      <c r="U13" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="V13" s="57"/>
-      <c r="W13" s="66"/>
-      <c r="X13" s="56" t="s">
+      <c r="V13" s="59"/>
+      <c r="W13" s="68"/>
+      <c r="X13" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="Y13" s="57"/>
-      <c r="Z13" s="57" t="s">
+      <c r="Y13" s="59"/>
+      <c r="Z13" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AA13" s="57"/>
-      <c r="AB13" s="57" t="s">
+      <c r="AA13" s="59"/>
+      <c r="AB13" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="58"/>
+      <c r="AC13" s="66"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1329,7 +1329,7 @@
       <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="67"/>
+      <c r="H14" s="57"/>
       <c r="I14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1369,7 +1369,7 @@
       <c r="V14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W14" s="67"/>
+      <c r="W14" s="57"/>
       <c r="X14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1637,60 +1637,60 @@
       <c r="B20" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="65" t="s">
+      <c r="C20" s="60"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="59"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="61"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="62"/>
       <c r="P20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="Q20" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="R20" s="59"/>
-      <c r="S20" s="60"/>
-      <c r="T20" s="60"/>
-      <c r="U20" s="60"/>
-      <c r="V20" s="61"/>
-      <c r="W20" s="65" t="s">
+      <c r="R20" s="60"/>
+      <c r="S20" s="61"/>
+      <c r="T20" s="61"/>
+      <c r="U20" s="61"/>
+      <c r="V20" s="62"/>
+      <c r="W20" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="X20" s="59"/>
-      <c r="Y20" s="60"/>
-      <c r="Z20" s="60"/>
-      <c r="AA20" s="60"/>
-      <c r="AB20" s="60"/>
-      <c r="AC20" s="61"/>
+      <c r="X20" s="60"/>
+      <c r="Y20" s="61"/>
+      <c r="Z20" s="61"/>
+      <c r="AA20" s="61"/>
+      <c r="AB20" s="61"/>
+      <c r="AC20" s="62"/>
       <c r="AE20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="AF20" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="AG20" s="59"/>
-      <c r="AH20" s="60"/>
-      <c r="AI20" s="60"/>
-      <c r="AJ20" s="60"/>
-      <c r="AK20" s="61"/>
-      <c r="AL20" s="65" t="s">
+      <c r="AG20" s="60"/>
+      <c r="AH20" s="61"/>
+      <c r="AI20" s="61"/>
+      <c r="AJ20" s="61"/>
+      <c r="AK20" s="62"/>
+      <c r="AL20" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AM20" s="59"/>
-      <c r="AN20" s="60"/>
-      <c r="AO20" s="60"/>
-      <c r="AP20" s="60"/>
-      <c r="AQ20" s="60"/>
-      <c r="AR20" s="61"/>
+      <c r="AM20" s="60"/>
+      <c r="AN20" s="61"/>
+      <c r="AO20" s="61"/>
+      <c r="AP20" s="61"/>
+      <c r="AQ20" s="61"/>
+      <c r="AR20" s="62"/>
     </row>
     <row r="21" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1699,134 +1699,134 @@
       <c r="B21" s="7">
         <v>5</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="63"/>
-      <c r="K21" s="63"/>
-      <c r="L21" s="63"/>
-      <c r="M21" s="63"/>
-      <c r="N21" s="64"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="65"/>
       <c r="P21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q21" s="5">
         <v>5</v>
       </c>
-      <c r="R21" s="62"/>
-      <c r="S21" s="63"/>
-      <c r="T21" s="63"/>
-      <c r="U21" s="63"/>
-      <c r="V21" s="64"/>
-      <c r="W21" s="66"/>
-      <c r="X21" s="62"/>
-      <c r="Y21" s="63"/>
-      <c r="Z21" s="63"/>
-      <c r="AA21" s="63"/>
-      <c r="AB21" s="63"/>
-      <c r="AC21" s="64"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="64"/>
+      <c r="T21" s="64"/>
+      <c r="U21" s="64"/>
+      <c r="V21" s="65"/>
+      <c r="W21" s="68"/>
+      <c r="X21" s="63"/>
+      <c r="Y21" s="64"/>
+      <c r="Z21" s="64"/>
+      <c r="AA21" s="64"/>
+      <c r="AB21" s="64"/>
+      <c r="AC21" s="65"/>
       <c r="AE21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AF21" s="5">
         <v>5</v>
       </c>
-      <c r="AG21" s="62"/>
-      <c r="AH21" s="63"/>
-      <c r="AI21" s="63"/>
-      <c r="AJ21" s="63"/>
-      <c r="AK21" s="64"/>
-      <c r="AL21" s="66"/>
-      <c r="AM21" s="62"/>
-      <c r="AN21" s="63"/>
-      <c r="AO21" s="63"/>
-      <c r="AP21" s="63"/>
-      <c r="AQ21" s="63"/>
-      <c r="AR21" s="64"/>
+      <c r="AG21" s="63"/>
+      <c r="AH21" s="64"/>
+      <c r="AI21" s="64"/>
+      <c r="AJ21" s="64"/>
+      <c r="AK21" s="65"/>
+      <c r="AL21" s="68"/>
+      <c r="AM21" s="63"/>
+      <c r="AN21" s="64"/>
+      <c r="AO21" s="64"/>
+      <c r="AP21" s="64"/>
+      <c r="AQ21" s="64"/>
+      <c r="AR21" s="65"/>
     </row>
     <row r="22" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57" t="s">
+      <c r="C22" s="59"/>
+      <c r="D22" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57" t="s">
+      <c r="E22" s="59"/>
+      <c r="F22" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="57"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="56" t="s">
+      <c r="G22" s="59"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57" t="s">
+      <c r="J22" s="59"/>
+      <c r="K22" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="57"/>
-      <c r="M22" s="57" t="s">
+      <c r="L22" s="59"/>
+      <c r="M22" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="58"/>
+      <c r="N22" s="66"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="68" t="s">
+      <c r="Q22" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="R22" s="57"/>
-      <c r="S22" s="57" t="s">
+      <c r="R22" s="59"/>
+      <c r="S22" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="57"/>
-      <c r="U22" s="57" t="s">
+      <c r="T22" s="59"/>
+      <c r="U22" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="V22" s="57"/>
-      <c r="W22" s="66"/>
-      <c r="X22" s="56" t="s">
+      <c r="V22" s="59"/>
+      <c r="W22" s="68"/>
+      <c r="X22" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="57"/>
-      <c r="Z22" s="57" t="s">
+      <c r="Y22" s="59"/>
+      <c r="Z22" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AA22" s="57"/>
-      <c r="AB22" s="57" t="s">
+      <c r="AA22" s="59"/>
+      <c r="AB22" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="AC22" s="58"/>
+      <c r="AC22" s="66"/>
       <c r="AE22" s="11"/>
-      <c r="AF22" s="68" t="s">
+      <c r="AF22" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="AG22" s="57"/>
-      <c r="AH22" s="57" t="s">
+      <c r="AG22" s="59"/>
+      <c r="AH22" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AI22" s="57"/>
-      <c r="AJ22" s="57" t="s">
+      <c r="AI22" s="59"/>
+      <c r="AJ22" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="AK22" s="57"/>
-      <c r="AL22" s="66"/>
-      <c r="AM22" s="56" t="s">
+      <c r="AK22" s="59"/>
+      <c r="AL22" s="68"/>
+      <c r="AM22" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="AN22" s="57"/>
-      <c r="AO22" s="57" t="s">
+      <c r="AN22" s="59"/>
+      <c r="AO22" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AP22" s="57"/>
-      <c r="AQ22" s="57" t="s">
+      <c r="AP22" s="59"/>
+      <c r="AQ22" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="AR22" s="58"/>
+      <c r="AR22" s="66"/>
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
@@ -1850,7 +1850,7 @@
       <c r="G23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="67"/>
+      <c r="H23" s="57"/>
       <c r="I23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1890,7 +1890,7 @@
       <c r="V23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W23" s="67"/>
+      <c r="W23" s="57"/>
       <c r="X23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="AK23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AL23" s="67"/>
+      <c r="AL23" s="57"/>
       <c r="AM23" s="3" t="s">
         <v>7</v>
       </c>
@@ -2417,18 +2417,18 @@
       <c r="G29" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="56" t="s">
+      <c r="I29" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57" t="s">
+      <c r="J29" s="59"/>
+      <c r="K29" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="57"/>
-      <c r="M29" s="57" t="s">
+      <c r="L29" s="59"/>
+      <c r="M29" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="58"/>
+      <c r="N29" s="66"/>
       <c r="P29" s="14">
         <v>200</v>
       </c>
@@ -2598,12 +2598,36 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="R11:V12"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="AG20:AK21"/>
+    <mergeCell ref="AL20:AL23"/>
+    <mergeCell ref="R20:V21"/>
+    <mergeCell ref="W20:W23"/>
+    <mergeCell ref="X20:AC21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="AM20:AR21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AO22:AP22"/>
+    <mergeCell ref="AQ22:AR22"/>
+    <mergeCell ref="C20:G21"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:N21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
@@ -2620,36 +2644,12 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="C20:G21"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:N21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="AM20:AR21"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="AO22:AP22"/>
-    <mergeCell ref="AQ22:AR22"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="AG20:AK21"/>
-    <mergeCell ref="AL20:AL23"/>
-    <mergeCell ref="R20:V21"/>
-    <mergeCell ref="W20:W23"/>
-    <mergeCell ref="X20:AC21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="AB22:AC22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="R11:V12"/>
+    <mergeCell ref="M13:N13"/>
   </mergeCells>
   <conditionalFormatting sqref="I38">
     <cfRule type="colorScale" priority="81">
@@ -2721,7 +2721,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7 B3 B5">
+  <conditionalFormatting sqref="B3 B7 B5">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -2731,7 +2731,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 D3 D5">
+  <conditionalFormatting sqref="D3 D7 D5">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -2741,7 +2741,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7 F3 F5">
+  <conditionalFormatting sqref="F3 F7 F5">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
@@ -2771,7 +2771,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7 C3 C5">
+  <conditionalFormatting sqref="C3 C7 C5">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -2781,7 +2781,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 E3 E7 E5">
+  <conditionalFormatting sqref="E3 E10 E7 E5">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -2791,7 +2791,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7 G3 G5">
+  <conditionalFormatting sqref="G3 G7 G5">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -2941,7 +2941,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I34 I31">
+  <conditionalFormatting sqref="I31 I34">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -2951,7 +2951,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34 J31">
+  <conditionalFormatting sqref="J31 J34">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -3370,8 +3370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A37A8E-CDB1-4DEE-B664-FA66341E80CD}">
   <dimension ref="A1:CS13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" zoomScale="139" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="BV12" sqref="BV12"/>
+    <sheetView tabSelected="1" topLeftCell="BZ1" zoomScale="139" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="CJ15" sqref="CJ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3385,202 +3385,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="58"/>
+      <c r="G1" s="66"/>
       <c r="H1" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="60"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="59" t="s">
+      <c r="J1" s="61"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="59" t="s">
+      <c r="M1" s="61"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
       <c r="R1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="57" t="s">
+      <c r="S1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57" t="s">
+      <c r="T1" s="59"/>
+      <c r="U1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57" t="s">
+      <c r="V1" s="59"/>
+      <c r="W1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="58"/>
+      <c r="X1" s="66"/>
       <c r="Y1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="57" t="s">
+      <c r="Z1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57" t="s">
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="57" t="s">
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="AE1" s="58"/>
-      <c r="AF1" s="59" t="s">
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" s="60"/>
-      <c r="AH1" s="60"/>
-      <c r="AI1" s="59" t="s">
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="61"/>
+      <c r="AI1" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="60"/>
-      <c r="AK1" s="61"/>
+      <c r="AJ1" s="61"/>
+      <c r="AK1" s="62"/>
       <c r="AL1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="57" t="s">
+      <c r="AM1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="AN1" s="57"/>
-      <c r="AO1" s="57" t="s">
+      <c r="AN1" s="59"/>
+      <c r="AO1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AP1" s="57"/>
-      <c r="AQ1" s="57" t="s">
+      <c r="AP1" s="59"/>
+      <c r="AQ1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="58"/>
+      <c r="AR1" s="66"/>
       <c r="AS1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="AT1" s="57" t="s">
+      <c r="AT1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="AU1" s="57"/>
-      <c r="AV1" s="57" t="s">
+      <c r="AU1" s="59"/>
+      <c r="AV1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="57"/>
-      <c r="AX1" s="57" t="s">
+      <c r="AW1" s="59"/>
+      <c r="AX1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="AY1" s="58"/>
-      <c r="AZ1" s="59" t="s">
+      <c r="AY1" s="66"/>
+      <c r="AZ1" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="BA1" s="60"/>
-      <c r="BB1" s="60"/>
-      <c r="BC1" s="59" t="s">
+      <c r="BA1" s="61"/>
+      <c r="BB1" s="61"/>
+      <c r="BC1" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="BD1" s="60"/>
-      <c r="BE1" s="61"/>
+      <c r="BD1" s="61"/>
+      <c r="BE1" s="62"/>
       <c r="BF1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="BG1" s="57" t="s">
+      <c r="BG1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="BH1" s="57"/>
-      <c r="BI1" s="57" t="s">
+      <c r="BH1" s="59"/>
+      <c r="BI1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="BJ1" s="57"/>
-      <c r="BK1" s="57" t="s">
+      <c r="BJ1" s="59"/>
+      <c r="BK1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="BL1" s="58"/>
+      <c r="BL1" s="66"/>
       <c r="BM1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="BN1" s="57" t="s">
+      <c r="BN1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="BO1" s="57"/>
-      <c r="BP1" s="57" t="s">
+      <c r="BO1" s="59"/>
+      <c r="BP1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="BQ1" s="57"/>
-      <c r="BR1" s="57" t="s">
+      <c r="BQ1" s="59"/>
+      <c r="BR1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="BS1" s="58"/>
-      <c r="BT1" s="59" t="s">
+      <c r="BS1" s="66"/>
+      <c r="BT1" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="BU1" s="60"/>
-      <c r="BV1" s="60"/>
-      <c r="BW1" s="59" t="s">
+      <c r="BU1" s="61"/>
+      <c r="BV1" s="61"/>
+      <c r="BW1" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="BX1" s="60"/>
-      <c r="BY1" s="61"/>
+      <c r="BX1" s="61"/>
+      <c r="BY1" s="62"/>
       <c r="BZ1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="CA1" s="57" t="s">
+      <c r="CA1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="CB1" s="57"/>
-      <c r="CC1" s="57" t="s">
+      <c r="CB1" s="59"/>
+      <c r="CC1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="CD1" s="57"/>
-      <c r="CE1" s="57" t="s">
+      <c r="CD1" s="59"/>
+      <c r="CE1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="CF1" s="58"/>
+      <c r="CF1" s="66"/>
       <c r="CG1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="CH1" s="57" t="s">
+      <c r="CH1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="CI1" s="57"/>
-      <c r="CJ1" s="57" t="s">
+      <c r="CI1" s="59"/>
+      <c r="CJ1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="CK1" s="57"/>
-      <c r="CL1" s="57" t="s">
+      <c r="CK1" s="59"/>
+      <c r="CL1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="CM1" s="58"/>
-      <c r="CN1" s="59" t="s">
+      <c r="CM1" s="66"/>
+      <c r="CN1" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="CO1" s="60"/>
-      <c r="CP1" s="60"/>
-      <c r="CQ1" s="59" t="s">
+      <c r="CO1" s="61"/>
+      <c r="CP1" s="61"/>
+      <c r="CQ1" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="CR1" s="60"/>
-      <c r="CS1" s="61"/>
+      <c r="CR1" s="61"/>
+      <c r="CS1" s="62"/>
     </row>
     <row r="2" spans="1:97" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3599,7 +3599,7 @@
       <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="71"/>
+      <c r="H2" s="70"/>
       <c r="I2" s="4" t="s">
         <v>24</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="X2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="70"/>
+      <c r="Y2" s="71"/>
       <c r="Z2" s="4" t="s">
         <v>7</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="AR2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AS2" s="70"/>
+      <c r="AS2" s="71"/>
       <c r="AT2" s="4" t="s">
         <v>7</v>
       </c>
@@ -3764,7 +3764,7 @@
       <c r="BL2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BM2" s="70"/>
+      <c r="BM2" s="71"/>
       <c r="BN2" s="4" t="s">
         <v>7</v>
       </c>
@@ -3822,7 +3822,7 @@
       <c r="CF2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="CG2" s="70"/>
+      <c r="CG2" s="71"/>
       <c r="CH2" s="4" t="s">
         <v>7</v>
       </c>
@@ -5305,43 +5305,43 @@
         <v>5</v>
       </c>
       <c r="CH9" s="17">
-        <v>1.7546647170092901E-4</v>
+        <v>1.6494510913616899E-4</v>
       </c>
       <c r="CI9" s="47">
-        <v>2.1413359618236401E-4</v>
+        <v>1.7596745269656799E-4</v>
       </c>
       <c r="CJ9" s="34">
-        <v>0.98700532674789399</v>
+        <v>0.98793016672134404</v>
       </c>
       <c r="CK9" s="34">
-        <v>0.98757469698786704</v>
+        <v>0.98766421332955301</v>
       </c>
       <c r="CL9" s="4">
-        <v>38.064488220214798</v>
+        <v>38.482702484130797</v>
       </c>
       <c r="CM9" s="5">
-        <v>37.393007526397703</v>
+        <v>38.382000861167903</v>
       </c>
       <c r="CN9" s="3">
-        <v>9.58</v>
+        <v>37.54</v>
       </c>
       <c r="CO9" s="42">
-        <v>7.44</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="CP9" s="4">
-        <v>10.3</v>
+        <v>11.56</v>
       </c>
       <c r="CQ9" s="44">
         <f t="shared" ref="CQ9" si="24">(MIN(CH9:CI9)/MAX(CH9:CI9))</f>
-        <v>0.8194252318608396</v>
+        <v>0.93736146434189993</v>
       </c>
       <c r="CR9" s="34">
         <f t="shared" ref="CR9" si="25">(MIN(CJ9:CK9)/MAX(CJ9:CK9))</f>
-        <v>0.99942346615227218</v>
+        <v>0.99973079737743642</v>
       </c>
       <c r="CS9" s="38">
         <f t="shared" ref="CS9" si="26">(MIN(CL9:CM9)/MAX(CL9:CM9))</f>
-        <v>0.98235939256736171</v>
+        <v>0.99738319773658257</v>
       </c>
     </row>
     <row r="10" spans="1:97" ht="60" x14ac:dyDescent="0.25">
@@ -5401,13 +5401,27 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="CH1:CI1"/>
+    <mergeCell ref="CJ1:CK1"/>
+    <mergeCell ref="CL1:CM1"/>
+    <mergeCell ref="CN1:CP1"/>
+    <mergeCell ref="CQ1:CS1"/>
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="CA1:CB1"/>
+    <mergeCell ref="CC1:CD1"/>
+    <mergeCell ref="CE1:CF1"/>
+    <mergeCell ref="CG1:CG2"/>
+    <mergeCell ref="BN1:BO1"/>
+    <mergeCell ref="BP1:BQ1"/>
+    <mergeCell ref="BR1:BS1"/>
+    <mergeCell ref="BT1:BV1"/>
+    <mergeCell ref="BW1:BY1"/>
+    <mergeCell ref="BC1:BE1"/>
+    <mergeCell ref="BG1:BH1"/>
+    <mergeCell ref="BI1:BJ1"/>
+    <mergeCell ref="BK1:BL1"/>
+    <mergeCell ref="BM1:BM2"/>
+    <mergeCell ref="AS1:AS2"/>
     <mergeCell ref="AT1:AU1"/>
     <mergeCell ref="AV1:AW1"/>
     <mergeCell ref="AX1:AY1"/>
@@ -5424,27 +5438,13 @@
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="CA1:CB1"/>
-    <mergeCell ref="CC1:CD1"/>
-    <mergeCell ref="CE1:CF1"/>
-    <mergeCell ref="CG1:CG2"/>
-    <mergeCell ref="BN1:BO1"/>
-    <mergeCell ref="BP1:BQ1"/>
-    <mergeCell ref="BR1:BS1"/>
-    <mergeCell ref="BT1:BV1"/>
-    <mergeCell ref="BW1:BY1"/>
-    <mergeCell ref="BC1:BE1"/>
-    <mergeCell ref="BG1:BH1"/>
-    <mergeCell ref="BI1:BJ1"/>
-    <mergeCell ref="BK1:BL1"/>
-    <mergeCell ref="BM1:BM2"/>
-    <mergeCell ref="AS1:AS2"/>
-    <mergeCell ref="CH1:CI1"/>
-    <mergeCell ref="CJ1:CK1"/>
-    <mergeCell ref="CL1:CM1"/>
-    <mergeCell ref="CN1:CP1"/>
-    <mergeCell ref="CQ1:CS1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="colorScale" priority="208">
@@ -5476,7 +5476,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7 B3 B5">
+  <conditionalFormatting sqref="B3 B7 B5">
     <cfRule type="colorScale" priority="205">
       <colorScale>
         <cfvo type="min"/>
@@ -5486,7 +5486,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 D3 D5">
+  <conditionalFormatting sqref="D3 D7 D5">
     <cfRule type="colorScale" priority="204">
       <colorScale>
         <cfvo type="min"/>
@@ -5496,7 +5496,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7 F3 F5">
+  <conditionalFormatting sqref="F3 F7 F5">
     <cfRule type="colorScale" priority="203">
       <colorScale>
         <cfvo type="min"/>
@@ -5506,7 +5506,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7 C3 C5">
+  <conditionalFormatting sqref="C3 C7 C5">
     <cfRule type="colorScale" priority="202">
       <colorScale>
         <cfvo type="min"/>
@@ -5516,7 +5516,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 E3 E5">
+  <conditionalFormatting sqref="E3 E7 E5">
     <cfRule type="colorScale" priority="201">
       <colorScale>
         <cfvo type="min"/>
@@ -5526,7 +5526,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7 G3 G5">
+  <conditionalFormatting sqref="G3 G7 G5">
     <cfRule type="colorScale" priority="200">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
report.xlsx was updated: 4141 annual samples
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qorba\Documents\Master-Building science\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF23F73E-B2E3-4E16-8082-17DE40519C41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F26C978-8BD1-432C-8C17-3EC38BA900A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{C760A067-8455-42A1-8018-2B10D7DC26ED}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="42">
   <si>
     <t>Base Model</t>
   </si>
@@ -137,6 +137,21 @@
   </si>
   <si>
     <t>TL 100 samples</t>
+  </si>
+  <si>
+    <t>All samples</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>duration: (s)</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>DGP</t>
   </si>
 </sst>
 </file>
@@ -410,7 +425,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -469,16 +484,14 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -499,22 +512,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -875,24 +894,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59" t="s">
+      <c r="E1" s="58"/>
+      <c r="F1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="66"/>
+      <c r="G1" s="59"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
+      <c r="A2" s="68"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1204,7 @@
       <c r="E11" s="61"/>
       <c r="F11" s="61"/>
       <c r="G11" s="62"/>
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="66" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="60"/>
@@ -1205,7 +1224,7 @@
       <c r="T11" s="61"/>
       <c r="U11" s="61"/>
       <c r="V11" s="62"/>
-      <c r="W11" s="56" t="s">
+      <c r="W11" s="66" t="s">
         <v>15</v>
       </c>
       <c r="X11" s="60"/>
@@ -1227,7 +1246,7 @@
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
       <c r="G12" s="65"/>
-      <c r="H12" s="68"/>
+      <c r="H12" s="67"/>
       <c r="I12" s="63"/>
       <c r="J12" s="64"/>
       <c r="K12" s="64"/>
@@ -1245,7 +1264,7 @@
       <c r="T12" s="64"/>
       <c r="U12" s="64"/>
       <c r="V12" s="65"/>
-      <c r="W12" s="68"/>
+      <c r="W12" s="67"/>
       <c r="X12" s="63"/>
       <c r="Y12" s="64"/>
       <c r="Z12" s="64"/>
@@ -1255,57 +1274,57 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59" t="s">
+      <c r="C13" s="58"/>
+      <c r="D13" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59" t="s">
+      <c r="E13" s="58"/>
+      <c r="F13" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="59"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="67" t="s">
+      <c r="G13" s="58"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59" t="s">
+      <c r="J13" s="58"/>
+      <c r="K13" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59" t="s">
+      <c r="L13" s="58"/>
+      <c r="M13" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="N13" s="66"/>
+      <c r="N13" s="59"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="58" t="s">
+      <c r="Q13" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="59"/>
-      <c r="S13" s="59" t="s">
+      <c r="R13" s="58"/>
+      <c r="S13" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="59"/>
-      <c r="U13" s="59" t="s">
+      <c r="T13" s="58"/>
+      <c r="U13" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="V13" s="59"/>
-      <c r="W13" s="68"/>
-      <c r="X13" s="67" t="s">
+      <c r="V13" s="58"/>
+      <c r="W13" s="67"/>
+      <c r="X13" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="Y13" s="59"/>
-      <c r="Z13" s="59" t="s">
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="59" t="s">
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="66"/>
+      <c r="AC13" s="59"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
@@ -1329,7 +1348,7 @@
       <c r="G14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="57"/>
+      <c r="H14" s="68"/>
       <c r="I14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1369,7 +1388,7 @@
       <c r="V14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W14" s="57"/>
+      <c r="W14" s="68"/>
       <c r="X14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1642,7 +1661,7 @@
       <c r="E20" s="61"/>
       <c r="F20" s="61"/>
       <c r="G20" s="62"/>
-      <c r="H20" s="56" t="s">
+      <c r="H20" s="66" t="s">
         <v>15</v>
       </c>
       <c r="I20" s="60"/>
@@ -1662,7 +1681,7 @@
       <c r="T20" s="61"/>
       <c r="U20" s="61"/>
       <c r="V20" s="62"/>
-      <c r="W20" s="56" t="s">
+      <c r="W20" s="66" t="s">
         <v>15</v>
       </c>
       <c r="X20" s="60"/>
@@ -1682,7 +1701,7 @@
       <c r="AI20" s="61"/>
       <c r="AJ20" s="61"/>
       <c r="AK20" s="62"/>
-      <c r="AL20" s="56" t="s">
+      <c r="AL20" s="66" t="s">
         <v>15</v>
       </c>
       <c r="AM20" s="60"/>
@@ -1704,7 +1723,7 @@
       <c r="E21" s="64"/>
       <c r="F21" s="64"/>
       <c r="G21" s="65"/>
-      <c r="H21" s="68"/>
+      <c r="H21" s="67"/>
       <c r="I21" s="63"/>
       <c r="J21" s="64"/>
       <c r="K21" s="64"/>
@@ -1722,7 +1741,7 @@
       <c r="T21" s="64"/>
       <c r="U21" s="64"/>
       <c r="V21" s="65"/>
-      <c r="W21" s="68"/>
+      <c r="W21" s="67"/>
       <c r="X21" s="63"/>
       <c r="Y21" s="64"/>
       <c r="Z21" s="64"/>
@@ -1740,7 +1759,7 @@
       <c r="AI21" s="64"/>
       <c r="AJ21" s="64"/>
       <c r="AK21" s="65"/>
-      <c r="AL21" s="68"/>
+      <c r="AL21" s="67"/>
       <c r="AM21" s="63"/>
       <c r="AN21" s="64"/>
       <c r="AO21" s="64"/>
@@ -1750,83 +1769,83 @@
     </row>
     <row r="22" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59" t="s">
+      <c r="C22" s="58"/>
+      <c r="D22" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59" t="s">
+      <c r="E22" s="58"/>
+      <c r="F22" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="59"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="67" t="s">
+      <c r="G22" s="58"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59" t="s">
+      <c r="J22" s="58"/>
+      <c r="K22" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59" t="s">
+      <c r="L22" s="58"/>
+      <c r="M22" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="66"/>
+      <c r="N22" s="59"/>
       <c r="P22" s="11"/>
-      <c r="Q22" s="58" t="s">
+      <c r="Q22" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="R22" s="59"/>
-      <c r="S22" s="59" t="s">
+      <c r="R22" s="58"/>
+      <c r="S22" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="T22" s="59"/>
-      <c r="U22" s="59" t="s">
+      <c r="T22" s="58"/>
+      <c r="U22" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="V22" s="59"/>
-      <c r="W22" s="68"/>
-      <c r="X22" s="67" t="s">
+      <c r="V22" s="58"/>
+      <c r="W22" s="67"/>
+      <c r="X22" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="Y22" s="59"/>
-      <c r="Z22" s="59" t="s">
+      <c r="Y22" s="58"/>
+      <c r="Z22" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="AA22" s="59"/>
-      <c r="AB22" s="59" t="s">
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AC22" s="66"/>
+      <c r="AC22" s="59"/>
       <c r="AE22" s="11"/>
-      <c r="AF22" s="58" t="s">
+      <c r="AF22" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AG22" s="59"/>
-      <c r="AH22" s="59" t="s">
+      <c r="AG22" s="58"/>
+      <c r="AH22" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="AI22" s="59"/>
-      <c r="AJ22" s="59" t="s">
+      <c r="AI22" s="58"/>
+      <c r="AJ22" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AK22" s="59"/>
-      <c r="AL22" s="68"/>
-      <c r="AM22" s="67" t="s">
+      <c r="AK22" s="58"/>
+      <c r="AL22" s="67"/>
+      <c r="AM22" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="AN22" s="59"/>
-      <c r="AO22" s="59" t="s">
+      <c r="AN22" s="58"/>
+      <c r="AO22" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="AP22" s="59"/>
-      <c r="AQ22" s="59" t="s">
+      <c r="AP22" s="58"/>
+      <c r="AQ22" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AR22" s="66"/>
+      <c r="AR22" s="59"/>
     </row>
     <row r="23" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
@@ -1850,7 +1869,7 @@
       <c r="G23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="57"/>
+      <c r="H23" s="68"/>
       <c r="I23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1890,7 +1909,7 @@
       <c r="V23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="W23" s="57"/>
+      <c r="W23" s="68"/>
       <c r="X23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1930,7 +1949,7 @@
       <c r="AK23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AL23" s="57"/>
+      <c r="AL23" s="68"/>
       <c r="AM23" s="3" t="s">
         <v>7</v>
       </c>
@@ -2417,18 +2436,18 @@
       <c r="G29" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="67" t="s">
+      <c r="I29" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59" t="s">
+      <c r="J29" s="58"/>
+      <c r="K29" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59" t="s">
+      <c r="L29" s="58"/>
+      <c r="M29" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="66"/>
+      <c r="N29" s="59"/>
       <c r="P29" s="14">
         <v>200</v>
       </c>
@@ -2598,36 +2617,12 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="AG20:AK21"/>
-    <mergeCell ref="AL20:AL23"/>
-    <mergeCell ref="R20:V21"/>
-    <mergeCell ref="W20:W23"/>
-    <mergeCell ref="X20:AC21"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="X22:Y22"/>
-    <mergeCell ref="Z22:AA22"/>
-    <mergeCell ref="AB22:AC22"/>
-    <mergeCell ref="AM20:AR21"/>
-    <mergeCell ref="AF22:AG22"/>
-    <mergeCell ref="AH22:AI22"/>
-    <mergeCell ref="AJ22:AK22"/>
-    <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="AO22:AP22"/>
-    <mergeCell ref="AQ22:AR22"/>
-    <mergeCell ref="C20:G21"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:N21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="R11:V12"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
@@ -2644,12 +2639,36 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="R11:V12"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="C20:G21"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:N21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="AM20:AR21"/>
+    <mergeCell ref="AF22:AG22"/>
+    <mergeCell ref="AH22:AI22"/>
+    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AO22:AP22"/>
+    <mergeCell ref="AQ22:AR22"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="AG20:AK21"/>
+    <mergeCell ref="AL20:AL23"/>
+    <mergeCell ref="R20:V21"/>
+    <mergeCell ref="W20:W23"/>
+    <mergeCell ref="X20:AC21"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="X22:Y22"/>
+    <mergeCell ref="Z22:AA22"/>
+    <mergeCell ref="AB22:AC22"/>
   </mergeCells>
   <conditionalFormatting sqref="I38">
     <cfRule type="colorScale" priority="81">
@@ -3368,10 +3387,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A37A8E-CDB1-4DEE-B664-FA66341E80CD}">
-  <dimension ref="A1:CS13"/>
+  <dimension ref="A1:CS16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZ1" zoomScale="139" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="CJ15" sqref="CJ15"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3385,22 +3404,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59" t="s">
+      <c r="C1" s="58"/>
+      <c r="D1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59" t="s">
+      <c r="E1" s="58"/>
+      <c r="F1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="66"/>
-      <c r="H1" s="69" t="s">
+      <c r="G1" s="59"/>
+      <c r="H1" s="71" t="s">
         <v>22</v>
       </c>
       <c r="I1" s="61" t="s">
@@ -3421,33 +3440,33 @@
       <c r="R1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="59" t="s">
+      <c r="S1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59" t="s">
+      <c r="T1" s="58"/>
+      <c r="U1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59" t="s">
+      <c r="V1" s="58"/>
+      <c r="W1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="69" t="s">
+      <c r="X1" s="59"/>
+      <c r="Y1" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="59" t="s">
+      <c r="Z1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59" t="s">
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59" t="s">
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AE1" s="66"/>
+      <c r="AE1" s="59"/>
       <c r="AF1" s="60" t="s">
         <v>23</v>
       </c>
@@ -3461,33 +3480,33 @@
       <c r="AL1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="AM1" s="59" t="s">
+      <c r="AM1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="AN1" s="59"/>
-      <c r="AO1" s="59" t="s">
+      <c r="AN1" s="58"/>
+      <c r="AO1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="AP1" s="59"/>
-      <c r="AQ1" s="59" t="s">
+      <c r="AP1" s="58"/>
+      <c r="AQ1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="69" t="s">
+      <c r="AR1" s="59"/>
+      <c r="AS1" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="AT1" s="59" t="s">
+      <c r="AT1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="AU1" s="59"/>
-      <c r="AV1" s="59" t="s">
+      <c r="AU1" s="58"/>
+      <c r="AV1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="59"/>
-      <c r="AX1" s="59" t="s">
+      <c r="AW1" s="58"/>
+      <c r="AX1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AY1" s="66"/>
+      <c r="AY1" s="59"/>
       <c r="AZ1" s="60" t="s">
         <v>23</v>
       </c>
@@ -3501,33 +3520,33 @@
       <c r="BF1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="BG1" s="59" t="s">
+      <c r="BG1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="BH1" s="59"/>
-      <c r="BI1" s="59" t="s">
+      <c r="BH1" s="58"/>
+      <c r="BI1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="BJ1" s="59"/>
-      <c r="BK1" s="59" t="s">
+      <c r="BJ1" s="58"/>
+      <c r="BK1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="BL1" s="66"/>
-      <c r="BM1" s="69" t="s">
+      <c r="BL1" s="59"/>
+      <c r="BM1" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="BN1" s="59" t="s">
+      <c r="BN1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="BO1" s="59"/>
-      <c r="BP1" s="59" t="s">
+      <c r="BO1" s="58"/>
+      <c r="BP1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="BQ1" s="59"/>
-      <c r="BR1" s="59" t="s">
+      <c r="BQ1" s="58"/>
+      <c r="BR1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="BS1" s="66"/>
+      <c r="BS1" s="59"/>
       <c r="BT1" s="60" t="s">
         <v>23</v>
       </c>
@@ -3541,33 +3560,33 @@
       <c r="BZ1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="CA1" s="59" t="s">
+      <c r="CA1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="CB1" s="59"/>
-      <c r="CC1" s="59" t="s">
+      <c r="CB1" s="58"/>
+      <c r="CC1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="CD1" s="59"/>
-      <c r="CE1" s="59" t="s">
+      <c r="CD1" s="58"/>
+      <c r="CE1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="CF1" s="66"/>
-      <c r="CG1" s="69" t="s">
+      <c r="CF1" s="59"/>
+      <c r="CG1" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="CH1" s="59" t="s">
+      <c r="CH1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="CI1" s="59"/>
-      <c r="CJ1" s="59" t="s">
+      <c r="CI1" s="58"/>
+      <c r="CJ1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="CK1" s="59"/>
-      <c r="CL1" s="59" t="s">
+      <c r="CK1" s="58"/>
+      <c r="CL1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="CM1" s="66"/>
+      <c r="CM1" s="59"/>
       <c r="CN1" s="60" t="s">
         <v>23</v>
       </c>
@@ -3580,7 +3599,7 @@
       <c r="CS1" s="62"/>
     </row>
     <row r="2" spans="1:97" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
+      <c r="A2" s="68"/>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -3599,7 +3618,7 @@
       <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="70"/>
+      <c r="H2" s="73"/>
       <c r="I2" s="4" t="s">
         <v>24</v>
       </c>
@@ -3648,7 +3667,7 @@
       <c r="X2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="71"/>
+      <c r="Y2" s="72"/>
       <c r="Z2" s="4" t="s">
         <v>7</v>
       </c>
@@ -3706,7 +3725,7 @@
       <c r="AR2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AS2" s="71"/>
+      <c r="AS2" s="72"/>
       <c r="AT2" s="4" t="s">
         <v>7</v>
       </c>
@@ -3764,7 +3783,7 @@
       <c r="BL2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BM2" s="71"/>
+      <c r="BM2" s="72"/>
       <c r="BN2" s="4" t="s">
         <v>7</v>
       </c>
@@ -3822,7 +3841,7 @@
       <c r="CF2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="CG2" s="71"/>
+      <c r="CG2" s="72"/>
       <c r="CH2" s="4" t="s">
         <v>7</v>
       </c>
@@ -5397,13 +5416,83 @@
       <c r="I11" s="15"/>
     </row>
     <row r="13" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A13" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
       <c r="F13" s="28"/>
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="28">
+        <v>1.67626711011177E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.98468280591356705</v>
+      </c>
+      <c r="D15">
+        <v>38.641459608504</v>
+      </c>
+      <c r="H15" s="56">
+        <v>1.33002968116397E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:97" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <v>73</v>
+      </c>
+      <c r="C16" s="70">
+        <v>97.5</v>
+      </c>
+      <c r="D16" s="70"/>
+      <c r="E16">
+        <v>80.849999999999994</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="CH1:CI1"/>
-    <mergeCell ref="CJ1:CK1"/>
-    <mergeCell ref="CL1:CM1"/>
+  <mergeCells count="46">
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="CN1:CP1"/>
     <mergeCell ref="CQ1:CS1"/>
     <mergeCell ref="AI1:AK1"/>
@@ -5420,6 +5509,11 @@
     <mergeCell ref="BG1:BH1"/>
     <mergeCell ref="BI1:BJ1"/>
     <mergeCell ref="BK1:BL1"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="CH1:CI1"/>
+    <mergeCell ref="CJ1:CK1"/>
+    <mergeCell ref="CL1:CM1"/>
     <mergeCell ref="BM1:BM2"/>
     <mergeCell ref="AS1:AS2"/>
     <mergeCell ref="AT1:AU1"/>
@@ -5431,20 +5525,6 @@
     <mergeCell ref="AO1:AP1"/>
     <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="B7">
     <cfRule type="colorScale" priority="208">

</xml_diff>